<commit_message>
more resource updates / balance checking
</commit_message>
<xml_diff>
--- a/Resources/PartBalance.xlsx
+++ b/Resources/PartBalance.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BaseStats" sheetId="1" r:id="rId1"/>
     <sheet name="ScaledStats" sheetId="2" r:id="rId2"/>
     <sheet name="Graph" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -227,7 +227,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -844,6 +844,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -867,25 +886,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2252,6 +2252,338 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>InPower</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graph!$K$7:$K$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24762500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24525000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24287500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24050000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.238125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23575000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.233375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22862500000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22625000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22387500000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22150000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21912500000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.21675</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.21437500000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.21200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.20962500000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20725000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.204875</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.20250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.200125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.19775000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.19537500000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.193</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.19062499999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.18825000000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.18587500000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.18350000000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.18112500000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.17875000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.176375</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.17400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.17162500000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.16925000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.166875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.16450000000000004</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.16212500000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.15975</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.15737500000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.15500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.15262500000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.15024999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.14787500000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.14550000000000002</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.143125</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.14075000000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.13837500000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.13362500000000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.13125000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.12887500000000002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.1265</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.12412500000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.12175</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.11937500000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.11700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.114625</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.11225000000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.109875</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.10749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.105125</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.10275000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.10037500000000002</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.5624999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.325E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.0875000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>8.8500000000000023E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>8.6125000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.3749999999999991E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8.1375000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.9000000000000015E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.6624999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.425000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.1874999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.9499999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.7125000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.4750000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.2375000000000014E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.7624999999999982E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.5250000000000021E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.2875000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.0499999999999989E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.8125000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.5749999999999985E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.3375000000000025E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.1000000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.8624999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.6250000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.3874999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.1500000000000028E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.9125000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.6749999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.4375000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.200000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.9625000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.7250000000000015E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.4874999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.2500000000000011E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2260,11 +2592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="220476928"/>
-        <c:axId val="220478464"/>
+        <c:axId val="132838592"/>
+        <c:axId val="132831928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="220476928"/>
+        <c:axId val="132838592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,12 +2653,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220478464"/>
+        <c:crossAx val="132831928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="220478464"/>
+        <c:axId val="132831928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2715,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220476928"/>
+        <c:crossAx val="132838592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2995,13 +3327,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>276227</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>385765</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50357</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3068,7 +3400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3103,7 +3435,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3314,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
@@ -3349,39 +3681,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="53" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="48" t="s">
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="50"/>
+      <c r="X1" s="57"/>
       <c r="Y1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="51" t="s">
+      <c r="Z1" s="58" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3422,7 +3754,7 @@
       <c r="M2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="50" t="s">
         <v>67</v>
       </c>
       <c r="O2" s="42" t="s">
@@ -3458,7 +3790,7 @@
       <c r="Y2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="52"/>
+      <c r="Z2" s="59"/>
       <c r="AA2" t="s">
         <v>48</v>
       </c>
@@ -3502,7 +3834,7 @@
       <c r="M3" s="4">
         <v>0</v>
       </c>
-      <c r="N3" s="59"/>
+      <c r="N3" s="51"/>
       <c r="O3" s="5">
         <v>0.15</v>
       </c>
@@ -3581,7 +3913,7 @@
       <c r="M4" s="11">
         <v>0</v>
       </c>
-      <c r="N4" s="60"/>
+      <c r="N4" s="52"/>
       <c r="O4" s="12">
         <v>0.15</v>
       </c>
@@ -3660,7 +3992,7 @@
       <c r="M5" s="11">
         <v>0</v>
       </c>
-      <c r="N5" s="60"/>
+      <c r="N5" s="52"/>
       <c r="O5" s="12">
         <v>0.15</v>
       </c>
@@ -3734,14 +4066,14 @@
       <c r="K6" s="38">
         <v>600</v>
       </c>
-      <c r="L6" s="56">
+      <c r="L6" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M6" s="15">
         <f t="shared" ref="M6:M16" si="5">(N6*I6)/R6*D6</f>
         <v>46.875</v>
       </c>
-      <c r="N6" s="61">
+      <c r="N6" s="53">
         <v>5</v>
       </c>
       <c r="O6" s="43">
@@ -3818,14 +4150,14 @@
       <c r="K7" s="38">
         <v>2500</v>
       </c>
-      <c r="L7" s="56">
+      <c r="L7" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M7" s="11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="N7" s="60"/>
+      <c r="N7" s="52"/>
       <c r="O7" s="12">
         <v>0.15</v>
       </c>
@@ -3900,14 +4232,14 @@
       <c r="K8" s="38">
         <v>900</v>
       </c>
-      <c r="L8" s="56">
+      <c r="L8" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="N8" s="61">
+      <c r="N8" s="53">
         <v>5</v>
       </c>
       <c r="O8" s="43">
@@ -3984,14 +4316,14 @@
       <c r="K9" s="38">
         <v>900</v>
       </c>
-      <c r="L9" s="56">
+      <c r="L9" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="5"/>
         <v>17.5</v>
       </c>
-      <c r="N9" s="61">
+      <c r="N9" s="53">
         <v>5</v>
       </c>
       <c r="O9" s="43">
@@ -4068,14 +4400,14 @@
       <c r="K10" s="38">
         <v>750</v>
       </c>
-      <c r="L10" s="56">
+      <c r="L10" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="N10" s="61">
+      <c r="N10" s="53">
         <v>5</v>
       </c>
       <c r="O10" s="43">
@@ -4152,14 +4484,14 @@
       <c r="K11" s="38">
         <v>175</v>
       </c>
-      <c r="L11" s="56">
+      <c r="L11" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" si="5"/>
         <v>520</v>
       </c>
-      <c r="N11" s="61">
+      <c r="N11" s="53">
         <v>5</v>
       </c>
       <c r="O11" s="43">
@@ -4236,14 +4568,14 @@
       <c r="K12" s="38">
         <v>1750</v>
       </c>
-      <c r="L12" s="56">
+      <c r="L12" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="5"/>
         <v>2.34</v>
       </c>
-      <c r="N12" s="61">
+      <c r="N12" s="53">
         <v>6</v>
       </c>
       <c r="O12" s="43">
@@ -4320,14 +4652,14 @@
       <c r="K13" s="38">
         <v>1600</v>
       </c>
-      <c r="L13" s="56">
+      <c r="L13" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" si="5"/>
         <v>1.2600000000000002</v>
       </c>
-      <c r="N13" s="61">
+      <c r="N13" s="53">
         <v>3</v>
       </c>
       <c r="O13" s="43">
@@ -4404,14 +4736,14 @@
       <c r="K14" s="38">
         <v>1400</v>
       </c>
-      <c r="L14" s="56">
+      <c r="L14" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M14" s="15">
         <f t="shared" si="5"/>
         <v>0.72</v>
       </c>
-      <c r="N14" s="61">
+      <c r="N14" s="53">
         <v>3</v>
       </c>
       <c r="O14" s="43">
@@ -4488,14 +4820,14 @@
       <c r="K15" s="38">
         <v>500</v>
       </c>
-      <c r="L15" s="56">
+      <c r="L15" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M15" s="15">
         <f t="shared" si="5"/>
         <v>1.98</v>
       </c>
-      <c r="N15" s="61">
+      <c r="N15" s="53">
         <v>3</v>
       </c>
       <c r="O15" s="43">
@@ -4572,14 +4904,14 @@
       <c r="K16" s="38">
         <v>300</v>
       </c>
-      <c r="L16" s="56">
+      <c r="L16" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="5"/>
         <v>172.5</v>
       </c>
-      <c r="N16" s="61">
+      <c r="N16" s="53">
         <v>5</v>
       </c>
       <c r="O16" s="43">
@@ -4656,14 +4988,14 @@
       <c r="K17" s="38">
         <v>800</v>
       </c>
-      <c r="L17" s="56">
+      <c r="L17" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M17" s="15">
         <f>(N17*I17)/R17*D17</f>
         <v>16.64</v>
       </c>
-      <c r="N17" s="61">
+      <c r="N17" s="53">
         <v>8</v>
       </c>
       <c r="O17" s="43">
@@ -4740,14 +5072,14 @@
       <c r="K18" s="38">
         <v>1800</v>
       </c>
-      <c r="L18" s="56">
+      <c r="L18" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M18" s="15">
         <f t="shared" ref="M18:M19" si="8">(N18*I18)/R18*D18</f>
         <v>13.759999999999998</v>
       </c>
-      <c r="N18" s="61">
+      <c r="N18" s="53">
         <v>10</v>
       </c>
       <c r="O18" s="43">
@@ -4824,14 +5156,14 @@
       <c r="K19" s="21">
         <v>500</v>
       </c>
-      <c r="L19" s="57">
+      <c r="L19" s="49">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="M19" s="23">
         <f t="shared" si="8"/>
         <v>0.63</v>
       </c>
-      <c r="N19" s="62">
+      <c r="N19" s="54">
         <v>3</v>
       </c>
       <c r="O19" s="44">
@@ -4902,8 +5234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5080,6 +5412,10 @@
         <f>F7/I7</f>
         <v>0</v>
       </c>
+      <c r="K7">
+        <f>H7*0.25</f>
+        <v>0.25</v>
+      </c>
       <c r="L7">
         <f>A7</f>
         <v>0</v>
@@ -5125,8 +5461,12 @@
         <f t="shared" ref="J8:J71" si="8">F8/I8</f>
         <v>1.2760120612690322E-2</v>
       </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K71" si="9">H8*0.25</f>
+        <v>0.24762500000000001</v>
+      </c>
       <c r="L8">
-        <f t="shared" ref="L8:L71" si="9">A8</f>
+        <f t="shared" ref="L8:L71" si="10">A8</f>
         <v>1</v>
       </c>
     </row>
@@ -5170,8 +5510,12 @@
         <f t="shared" si="8"/>
         <v>2.5507102580406241E-2</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="9"/>
+        <v>0.24525000000000002</v>
+      </c>
       <c r="L9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
     </row>
@@ -5215,8 +5559,12 @@
         <f t="shared" si="8"/>
         <v>3.8240560466830963E-2</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="9"/>
+        <v>0.24287500000000001</v>
+      </c>
       <c r="L10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
     </row>
@@ -5260,8 +5608,12 @@
         <f t="shared" si="8"/>
         <v>5.09600936105125E-2</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="9"/>
+        <v>0.24050000000000002</v>
+      </c>
       <c r="L11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
@@ -5305,8 +5657,12 @@
         <f t="shared" si="8"/>
         <v>6.3665285365605007E-2</v>
       </c>
+      <c r="K12">
+        <f t="shared" si="9"/>
+        <v>0.238125</v>
+      </c>
       <c r="L12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
     </row>
@@ -5350,8 +5706,12 @@
         <f t="shared" si="8"/>
         <v>7.635570229671633E-2</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="9"/>
+        <v>0.23575000000000002</v>
+      </c>
       <c r="L13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
     </row>
@@ -5395,8 +5755,12 @@
         <f t="shared" si="8"/>
         <v>8.9030893324592658E-2</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="9"/>
+        <v>0.233375</v>
+      </c>
       <c r="L14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
     </row>
@@ -5440,8 +5804,12 @@
         <f t="shared" si="8"/>
         <v>0.10169038881910168</v>
       </c>
+      <c r="K15">
+        <f t="shared" si="9"/>
+        <v>0.23100000000000001</v>
+      </c>
       <c r="L15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
     </row>
@@ -5485,8 +5853,12 @@
         <f t="shared" si="8"/>
         <v>0.11433369963568256</v>
       </c>
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>0.22862500000000002</v>
+      </c>
       <c r="L16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
     </row>
@@ -5530,8 +5902,12 @@
         <f t="shared" si="8"/>
         <v>0.12696031609110764</v>
       </c>
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>0.22625000000000001</v>
+      </c>
       <c r="L17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
     </row>
@@ -5575,8 +5951,12 @@
         <f t="shared" si="8"/>
         <v>0.13956970687405035</v>
       </c>
+      <c r="K18">
+        <f t="shared" si="9"/>
+        <v>0.22387500000000002</v>
+      </c>
       <c r="L18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
     </row>
@@ -5620,8 +6000,12 @@
         <f t="shared" si="8"/>
         <v>0.15216131788556525</v>
       </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>0.22150000000000003</v>
+      </c>
       <c r="L19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -5665,8 +6049,12 @@
         <f t="shared" si="8"/>
         <v>0.16473457100416261</v>
       </c>
+      <c r="K20">
+        <f t="shared" si="9"/>
+        <v>0.21912500000000001</v>
+      </c>
       <c r="L20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
     </row>
@@ -5710,8 +6098,12 @@
         <f t="shared" si="8"/>
         <v>0.17728886276969463</v>
       </c>
+      <c r="K21">
+        <f t="shared" si="9"/>
+        <v>0.21675</v>
+      </c>
       <c r="L21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
     </row>
@@ -5755,8 +6147,12 @@
         <f t="shared" si="8"/>
         <v>0.18982356297975614</v>
       </c>
+      <c r="K22">
+        <f t="shared" si="9"/>
+        <v>0.21437500000000001</v>
+      </c>
       <c r="L22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
     </row>
@@ -5800,8 +6196,12 @@
         <f t="shared" si="8"/>
         <v>0.20233801319174005</v>
       </c>
+      <c r="K23">
+        <f t="shared" si="9"/>
+        <v>0.21200000000000002</v>
+      </c>
       <c r="L23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
     </row>
@@ -5845,8 +6245,12 @@
         <f t="shared" si="8"/>
         <v>0.21483152512306414</v>
       </c>
+      <c r="K24">
+        <f t="shared" si="9"/>
+        <v>0.20962500000000001</v>
+      </c>
       <c r="L24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
     </row>
@@ -5890,8 +6294,12 @@
         <f t="shared" si="8"/>
         <v>0.22730337894140162</v>
       </c>
+      <c r="K25">
+        <f t="shared" si="9"/>
+        <v>0.20725000000000002</v>
+      </c>
       <c r="L25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
     </row>
@@ -5935,8 +6343,12 @@
         <f t="shared" si="8"/>
         <v>0.2397528214359898</v>
       </c>
+      <c r="K26">
+        <f t="shared" si="9"/>
+        <v>0.204875</v>
+      </c>
       <c r="L26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>19</v>
       </c>
     </row>
@@ -5980,8 +6392,12 @@
         <f t="shared" si="8"/>
         <v>0.25217906406025214</v>
       </c>
+      <c r="K27">
+        <f t="shared" si="9"/>
+        <v>0.20250000000000001</v>
+      </c>
       <c r="L27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
     </row>
@@ -6025,8 +6441,12 @@
         <f t="shared" si="8"/>
         <v>0.26458128083504551</v>
       </c>
+      <c r="K28">
+        <f t="shared" si="9"/>
+        <v>0.200125</v>
+      </c>
       <c r="L28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
     </row>
@@ -6070,8 +6490,12 @@
         <f t="shared" si="8"/>
         <v>0.27695860610081235</v>
       </c>
+      <c r="K29">
+        <f t="shared" si="9"/>
+        <v>0.19775000000000001</v>
+      </c>
       <c r="L29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
     </row>
@@ -6115,8 +6539,12 @@
         <f t="shared" si="8"/>
         <v>0.2893101321057841</v>
       </c>
+      <c r="K30">
+        <f t="shared" si="9"/>
+        <v>0.19537500000000002</v>
+      </c>
       <c r="L30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>23</v>
       </c>
     </row>
@@ -6160,8 +6588,12 @@
         <f t="shared" si="8"/>
         <v>0.30163490641610996</v>
       </c>
+      <c r="K31">
+        <f t="shared" si="9"/>
+        <v>0.193</v>
+      </c>
       <c r="L31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
     </row>
@@ -6205,8 +6637,12 @@
         <f t="shared" si="8"/>
         <v>0.3139319291323836</v>
       </c>
+      <c r="K32">
+        <f t="shared" si="9"/>
+        <v>0.19062499999999999</v>
+      </c>
       <c r="L32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
     </row>
@@ -6250,8 +6686,12 @@
         <f t="shared" si="8"/>
         <v>0.32620014989546758</v>
       </c>
+      <c r="K33">
+        <f t="shared" si="9"/>
+        <v>0.18825000000000003</v>
+      </c>
       <c r="L33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
     </row>
@@ -6295,8 +6735,12 @@
         <f t="shared" si="8"/>
         <v>0.33843846466277172</v>
       </c>
+      <c r="K34">
+        <f t="shared" si="9"/>
+        <v>0.18587500000000001</v>
+      </c>
       <c r="L34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
@@ -6340,8 +6784,12 @@
         <f t="shared" si="8"/>
         <v>0.35064571223418717</v>
       </c>
+      <c r="K35">
+        <f t="shared" si="9"/>
+        <v>0.18350000000000002</v>
+      </c>
       <c r="L35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
     </row>
@@ -6385,8 +6833,12 @@
         <f t="shared" si="8"/>
         <v>0.36282067050469968</v>
       </c>
+      <c r="K36">
+        <f t="shared" si="9"/>
+        <v>0.18112500000000004</v>
+      </c>
       <c r="L36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>29</v>
       </c>
     </row>
@@ -6430,8 +6882,12 @@
         <f t="shared" si="8"/>
         <v>0.37496205241825953</v>
       </c>
+      <c r="K37">
+        <f t="shared" si="9"/>
+        <v>0.17875000000000002</v>
+      </c>
       <c r="L37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
     </row>
@@ -6475,8 +6931,12 @@
         <f t="shared" si="8"/>
         <v>0.38706850159474865</v>
       </c>
+      <c r="K38">
+        <f t="shared" si="9"/>
+        <v>0.176375</v>
+      </c>
       <c r="L38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
     </row>
@@ -6520,8 +6980,12 @@
         <f t="shared" si="8"/>
         <v>0.39913858759881293</v>
       </c>
+      <c r="K39">
+        <f t="shared" si="9"/>
+        <v>0.17400000000000002</v>
+      </c>
       <c r="L39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
     </row>
@@ -6565,8 +7029,12 @@
         <f t="shared" si="8"/>
         <v>0.4111708008158651</v>
       </c>
+      <c r="K40">
+        <f t="shared" si="9"/>
+        <v>0.17162500000000003</v>
+      </c>
       <c r="L40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>33</v>
       </c>
     </row>
@@ -6610,8 +7078,12 @@
         <f t="shared" si="8"/>
         <v>0.42316354689667351</v>
       </c>
+      <c r="K41">
+        <f t="shared" si="9"/>
+        <v>0.16925000000000001</v>
+      </c>
       <c r="L41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>34</v>
       </c>
     </row>
@@ -6655,8 +7127,12 @@
         <f t="shared" si="8"/>
         <v>0.43511514072755603</v>
       </c>
+      <c r="K42">
+        <f t="shared" si="9"/>
+        <v>0.166875</v>
+      </c>
       <c r="L42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>35</v>
       </c>
     </row>
@@ -6700,8 +7176,12 @@
         <f t="shared" si="8"/>
         <v>0.44702379987823421</v>
       </c>
+      <c r="K43">
+        <f t="shared" si="9"/>
+        <v>0.16450000000000004</v>
+      </c>
       <c r="L43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
     </row>
@@ -6745,8 +7225,12 @@
         <f t="shared" si="8"/>
         <v>0.4588876374737883</v>
       </c>
+      <c r="K44">
+        <f t="shared" si="9"/>
+        <v>0.16212500000000002</v>
+      </c>
       <c r="L44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>37</v>
       </c>
     </row>
@@ -6790,8 +7274,12 @@
         <f t="shared" si="8"/>
         <v>0.47070465443077353</v>
       </c>
+      <c r="K45">
+        <f t="shared" si="9"/>
+        <v>0.15975</v>
+      </c>
       <c r="L45">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
     </row>
@@ -6835,8 +7323,12 @@
         <f t="shared" si="8"/>
         <v>0.48247273099033494</v>
       </c>
+      <c r="K46">
+        <f t="shared" si="9"/>
+        <v>0.15737500000000001</v>
+      </c>
       <c r="L46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>39</v>
       </c>
     </row>
@@ -6880,8 +7372,12 @@
         <f t="shared" si="8"/>
         <v>0.4941896174729134</v>
       </c>
+      <c r="K47">
+        <f t="shared" si="9"/>
+        <v>0.15500000000000003</v>
+      </c>
       <c r="L47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
     </row>
@@ -6925,8 +7421,12 @@
         <f t="shared" si="8"/>
         <v>0.5058529241697558</v>
       </c>
+      <c r="K48">
+        <f t="shared" si="9"/>
+        <v>0.15262500000000001</v>
+      </c>
       <c r="L48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>41</v>
       </c>
     </row>
@@ -6970,8 +7470,12 @@
         <f t="shared" si="8"/>
         <v>0.5174601102757147</v>
       </c>
+      <c r="K49">
+        <f t="shared" si="9"/>
+        <v>0.15024999999999999</v>
+      </c>
       <c r="L49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>42</v>
       </c>
     </row>
@@ -7015,8 +7519,12 @@
         <f t="shared" si="8"/>
         <v>0.5290084717555571</v>
       </c>
+      <c r="K50">
+        <f t="shared" si="9"/>
+        <v>0.14787500000000001</v>
+      </c>
       <c r="L50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43</v>
       </c>
     </row>
@@ -7060,8 +7568,12 @@
         <f t="shared" si="8"/>
         <v>0.5404951280219219</v>
       </c>
+      <c r="K51">
+        <f t="shared" si="9"/>
+        <v>0.14550000000000002</v>
+      </c>
       <c r="L51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44</v>
       </c>
     </row>
@@ -7105,8 +7617,12 @@
         <f t="shared" si="8"/>
         <v>0.55191700728688919</v>
       </c>
+      <c r="K52">
+        <f t="shared" si="9"/>
+        <v>0.143125</v>
+      </c>
       <c r="L52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
     </row>
@@ -7150,8 +7666,12 @@
         <f t="shared" si="8"/>
         <v>0.56327083043049464</v>
       </c>
+      <c r="K53">
+        <f t="shared" si="9"/>
+        <v>0.14075000000000004</v>
+      </c>
       <c r="L53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46</v>
       </c>
     </row>
@@ -7195,8 +7715,12 @@
         <f t="shared" si="8"/>
         <v>0.57455309320800729</v>
       </c>
+      <c r="K54">
+        <f t="shared" si="9"/>
+        <v>0.13837500000000003</v>
+      </c>
       <c r="L54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>47</v>
       </c>
     </row>
@@ -7240,8 +7764,12 @@
         <f t="shared" si="8"/>
         <v>0.58576004659289449</v>
       </c>
+      <c r="K55">
+        <f t="shared" si="9"/>
+        <v>0.13600000000000001</v>
+      </c>
       <c r="L55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>48</v>
       </c>
     </row>
@@ -7285,8 +7813,12 @@
         <f t="shared" si="8"/>
         <v>0.59688767502352869</v>
       </c>
+      <c r="K56">
+        <f t="shared" si="9"/>
+        <v>0.13362500000000002</v>
+      </c>
       <c r="L56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49</v>
       </c>
     </row>
@@ -7330,8 +7862,12 @@
         <f t="shared" si="8"/>
         <v>0.60793167228810785</v>
       </c>
+      <c r="K57">
+        <f t="shared" si="9"/>
+        <v>0.13125000000000001</v>
+      </c>
       <c r="L57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
     </row>
@@ -7375,8 +7911,12 @@
         <f t="shared" si="8"/>
         <v>0.6188874147431157</v>
       </c>
+      <c r="K58">
+        <f t="shared" si="9"/>
+        <v>0.12887500000000002</v>
+      </c>
       <c r="L58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>51</v>
       </c>
     </row>
@@ -7420,8 +7960,12 @@
         <f t="shared" si="8"/>
         <v>0.62974993151489056</v>
       </c>
+      <c r="K59">
+        <f t="shared" si="9"/>
+        <v>0.1265</v>
+      </c>
       <c r="L59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>52</v>
       </c>
     </row>
@@ -7465,8 +8009,12 @@
         <f t="shared" si="8"/>
         <v>0.64051387128022574</v>
       </c>
+      <c r="K60">
+        <f t="shared" si="9"/>
+        <v>0.12412500000000001</v>
+      </c>
       <c r="L60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>53</v>
       </c>
     </row>
@@ -7510,8 +8058,12 @@
         <f t="shared" si="8"/>
         <v>0.65117346515886798</v>
       </c>
+      <c r="K61">
+        <f t="shared" si="9"/>
+        <v>0.12175</v>
+      </c>
       <c r="L61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>54</v>
       </c>
     </row>
@@ -7555,8 +8107,12 @@
         <f t="shared" si="8"/>
         <v>0.66172248517642751</v>
       </c>
+      <c r="K62">
+        <f t="shared" si="9"/>
+        <v>0.11937500000000001</v>
+      </c>
       <c r="L62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>55</v>
       </c>
     </row>
@@ -7600,8 +8156,12 @@
         <f t="shared" si="8"/>
         <v>0.67215419766828743</v>
       </c>
+      <c r="K63">
+        <f t="shared" si="9"/>
+        <v>0.11700000000000002</v>
+      </c>
       <c r="L63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>56</v>
       </c>
     </row>
@@ -7645,8 +8205,12 @@
         <f t="shared" si="8"/>
         <v>0.68246131089075668</v>
       </c>
+      <c r="K64">
+        <f t="shared" si="9"/>
+        <v>0.114625</v>
+      </c>
       <c r="L64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>57</v>
       </c>
     </row>
@@ -7690,8 +8254,12 @@
         <f t="shared" si="8"/>
         <v>0.69263591598152441</v>
       </c>
+      <c r="K65">
+        <f t="shared" si="9"/>
+        <v>0.11225000000000002</v>
+      </c>
       <c r="L65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>58</v>
       </c>
     </row>
@@ -7735,8 +8303,12 @@
         <f t="shared" si="8"/>
         <v>0.70266942026310797</v>
       </c>
+      <c r="K66">
+        <f t="shared" si="9"/>
+        <v>0.109875</v>
+      </c>
       <c r="L66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>59</v>
       </c>
     </row>
@@ -7780,8 +8352,12 @@
         <f t="shared" si="8"/>
         <v>0.71255247170513114</v>
       </c>
+      <c r="K67">
+        <f t="shared" si="9"/>
+        <v>0.10749999999999998</v>
+      </c>
       <c r="L67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>60</v>
       </c>
     </row>
@@ -7825,8 +8401,12 @@
         <f t="shared" si="8"/>
         <v>0.72227487314724348</v>
       </c>
+      <c r="K68">
+        <f t="shared" si="9"/>
+        <v>0.105125</v>
+      </c>
       <c r="L68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>61</v>
       </c>
     </row>
@@ -7870,8 +8450,12 @@
         <f t="shared" si="8"/>
         <v>0.7318254846259471</v>
       </c>
+      <c r="K69">
+        <f t="shared" si="9"/>
+        <v>0.10275000000000001</v>
+      </c>
       <c r="L69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
     </row>
@@ -7915,8 +8499,12 @@
         <f t="shared" si="8"/>
         <v>0.74119211183499778</v>
       </c>
+      <c r="K70">
+        <f t="shared" si="9"/>
+        <v>0.10037500000000002</v>
+      </c>
       <c r="L70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
     </row>
@@ -7960,8 +8548,12 @@
         <f t="shared" si="8"/>
         <v>0.75036137836703609</v>
       </c>
+      <c r="K71">
+        <f t="shared" si="9"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
       <c r="L71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
     </row>
@@ -7970,43 +8562,47 @@
         <v>65</v>
       </c>
       <c r="B72">
-        <f t="shared" ref="B72:B107" si="10">A72*0.01*$B$5</f>
+        <f t="shared" ref="B72:B107" si="11">A72*0.01*$B$5</f>
         <v>585</v>
       </c>
       <c r="C72">
-        <f t="shared" ref="C72:C107" si="11">B72/$B$5</f>
+        <f t="shared" ref="C72:C107" si="12">B72/$B$5</f>
         <v>0.65</v>
       </c>
       <c r="D72" s="47">
-        <f t="shared" ref="D72:D107" si="12">(100-A72)*$B$3*0.01</f>
+        <f t="shared" ref="D72:D107" si="13">(100-A72)*$B$3*0.01</f>
         <v>5.25</v>
       </c>
       <c r="E72" s="47">
-        <f t="shared" ref="E72:E107" si="13">D72/$B$3</f>
+        <f t="shared" ref="E72:E107" si="14">D72/$B$3</f>
         <v>0.35</v>
       </c>
       <c r="F72">
-        <f t="shared" ref="F72:F107" si="14">D72*B72/5252*0.745</f>
+        <f t="shared" ref="F72:F107" si="15">D72*B72/5252*0.745</f>
         <v>0.43565903465346534</v>
       </c>
       <c r="G72">
-        <f t="shared" ref="G72:G108" si="15">F72/$F$108</f>
+        <f t="shared" ref="G72:G108" si="16">F72/$F$108</f>
         <v>0.91</v>
       </c>
       <c r="H72">
-        <f t="shared" ref="H72:H107" si="16" xml:space="preserve"> $B$4 + 1 - (A72 * (1-$B$4)*0.01 + $B$4)</f>
+        <f t="shared" ref="H72:H107" si="17" xml:space="preserve"> $B$4 + 1 - (A72 * (1-$B$4)*0.01 + $B$4)</f>
         <v>0.38249999999999995</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72:I107" si="17">H72*$B$2</f>
+        <f t="shared" ref="I72:I107" si="18">H72*$B$2</f>
         <v>0.57374999999999998</v>
       </c>
       <c r="J72">
-        <f t="shared" ref="J72:J107" si="18">F72/I72</f>
+        <f t="shared" ref="J72:J107" si="19">F72/I72</f>
         <v>0.75931857891671517</v>
       </c>
+      <c r="K72">
+        <f t="shared" ref="K72:K108" si="20">H72*0.25</f>
+        <v>9.5624999999999988E-2</v>
+      </c>
       <c r="L72">
-        <f t="shared" ref="L72:L107" si="19">A72</f>
+        <f t="shared" ref="L72:L107" si="21">A72</f>
         <v>65</v>
       </c>
     </row>
@@ -8015,43 +8611,47 @@
         <v>66</v>
       </c>
       <c r="B73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>594</v>
       </c>
       <c r="C73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66</v>
       </c>
       <c r="D73" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.1000000000000005</v>
       </c>
       <c r="E73" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.34</v>
       </c>
       <c r="F73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.42972258187357198</v>
       </c>
       <c r="G73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.89760000000000018</v>
       </c>
       <c r="H73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.373</v>
       </c>
       <c r="I73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.5595</v>
       </c>
       <c r="J73">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.76804751005106697</v>
       </c>
+      <c r="K73">
+        <f t="shared" si="20"/>
+        <v>9.325E-2</v>
+      </c>
       <c r="L73">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>66</v>
       </c>
     </row>
@@ -8060,43 +8660,47 @@
         <v>67</v>
       </c>
       <c r="B74">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>603</v>
       </c>
       <c r="C74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.67</v>
       </c>
       <c r="D74" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.95</v>
       </c>
       <c r="E74" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33</v>
       </c>
       <c r="F74">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.42340313214013708</v>
       </c>
       <c r="G74">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.88440000000000007</v>
       </c>
       <c r="H74">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.36350000000000005</v>
       </c>
       <c r="I74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.54525000000000001</v>
       </c>
       <c r="J74">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.77653027444316747</v>
       </c>
+      <c r="K74">
+        <f t="shared" si="20"/>
+        <v>9.0875000000000011E-2</v>
+      </c>
       <c r="L74">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>67</v>
       </c>
     </row>
@@ -8105,43 +8709,47 @@
         <v>68</v>
       </c>
       <c r="B75">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>612</v>
       </c>
       <c r="C75">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.68</v>
       </c>
       <c r="D75" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.8</v>
       </c>
       <c r="E75" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.32</v>
       </c>
       <c r="F75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.41670068545316069</v>
       </c>
       <c r="G75">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.87040000000000006</v>
       </c>
       <c r="H75">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.35400000000000009</v>
       </c>
       <c r="I75">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.53100000000000014</v>
       </c>
       <c r="J75">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.78474705358410657</v>
       </c>
+      <c r="K75">
+        <f t="shared" si="20"/>
+        <v>8.8500000000000023E-2</v>
+      </c>
       <c r="L75">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>68</v>
       </c>
     </row>
@@ -8150,43 +8758,47 @@
         <v>69</v>
       </c>
       <c r="B76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>621</v>
       </c>
       <c r="C76">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.69</v>
       </c>
       <c r="D76" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.6500000000000004</v>
       </c>
       <c r="E76" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.31</v>
       </c>
       <c r="F76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.40961524181264281</v>
       </c>
       <c r="G76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.85560000000000014</v>
       </c>
       <c r="H76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.34450000000000003</v>
       </c>
       <c r="I76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.51675000000000004</v>
       </c>
       <c r="J76">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.79267584288852011</v>
       </c>
+      <c r="K76">
+        <f t="shared" si="20"/>
+        <v>8.6125000000000007E-2</v>
+      </c>
       <c r="L76">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>69</v>
       </c>
     </row>
@@ -8195,43 +8807,47 @@
         <v>70</v>
       </c>
       <c r="B77">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>630.00000000000011</v>
       </c>
       <c r="C77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.70000000000000018</v>
       </c>
       <c r="D77" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="E77" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.3</v>
       </c>
       <c r="F77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.40214680121858348</v>
       </c>
       <c r="G77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.8400000000000003</v>
       </c>
       <c r="H77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.33499999999999996</v>
       </c>
       <c r="I77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.50249999999999995</v>
       </c>
       <c r="J77">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.80029214172852448</v>
       </c>
+      <c r="K77">
+        <f t="shared" si="20"/>
+        <v>8.3749999999999991E-2</v>
+      </c>
       <c r="L77">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>70</v>
       </c>
     </row>
@@ -8240,43 +8856,47 @@
         <v>71</v>
       </c>
       <c r="B78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>639</v>
       </c>
       <c r="C78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.71</v>
       </c>
       <c r="D78" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.3500000000000005</v>
       </c>
       <c r="E78" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="F78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.39429536367098256</v>
       </c>
       <c r="G78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.82360000000000022</v>
       </c>
       <c r="H78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.32550000000000001</v>
       </c>
       <c r="I78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.48825000000000002</v>
       </c>
       <c r="J78">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.80756858918788033</v>
       </c>
+      <c r="K78">
+        <f t="shared" si="20"/>
+        <v>8.1375000000000003E-2</v>
+      </c>
       <c r="L78">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>71</v>
       </c>
     </row>
@@ -8285,43 +8905,47 @@
         <v>72</v>
       </c>
       <c r="B79">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>648</v>
       </c>
       <c r="C79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.72</v>
       </c>
       <c r="D79" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.2</v>
       </c>
       <c r="E79" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="F79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.38606092916984008</v>
       </c>
       <c r="G79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.80640000000000012</v>
       </c>
       <c r="H79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.31600000000000006</v>
       </c>
       <c r="I79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.47400000000000009</v>
       </c>
       <c r="J79">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8144745341135865</v>
       </c>
+      <c r="K79">
+        <f t="shared" si="20"/>
+        <v>7.9000000000000015E-2</v>
+      </c>
       <c r="L79">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>72</v>
       </c>
     </row>
@@ -8330,43 +8954,47 @@
         <v>73</v>
       </c>
       <c r="B80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>657</v>
       </c>
       <c r="C80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.73</v>
       </c>
       <c r="D80" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.05</v>
       </c>
       <c r="E80" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.26999999999999996</v>
       </c>
       <c r="F80">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.37744349771515617</v>
       </c>
       <c r="G80">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.78840000000000021</v>
       </c>
       <c r="H80">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.30649999999999999</v>
       </c>
       <c r="I80">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.45974999999999999</v>
       </c>
       <c r="J80">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.82097552520969264</v>
       </c>
+      <c r="K80">
+        <f t="shared" si="20"/>
+        <v>7.6624999999999999E-2</v>
+      </c>
       <c r="L80">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>73</v>
       </c>
     </row>
@@ -8375,43 +9003,47 @@
         <v>74</v>
       </c>
       <c r="B81">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>666</v>
       </c>
       <c r="C81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.74</v>
       </c>
       <c r="D81" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.9</v>
       </c>
       <c r="E81" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.26</v>
       </c>
       <c r="F81">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.36844306930693072</v>
       </c>
       <c r="G81">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.76960000000000017</v>
       </c>
       <c r="H81">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.29700000000000004</v>
       </c>
       <c r="I81">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.44550000000000006</v>
       </c>
       <c r="J81">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.82703270327032696</v>
       </c>
+      <c r="K81">
+        <f t="shared" si="20"/>
+        <v>7.425000000000001E-2</v>
+      </c>
       <c r="L81">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>74</v>
       </c>
     </row>
@@ -8420,43 +9052,47 @@
         <v>75</v>
       </c>
       <c r="B82">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>675</v>
       </c>
       <c r="C82">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
       <c r="D82" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.75</v>
       </c>
       <c r="E82" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.25</v>
       </c>
       <c r="F82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.35905964394516371</v>
       </c>
       <c r="G82">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.75</v>
       </c>
       <c r="H82">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.28749999999999998</v>
       </c>
       <c r="I82">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.43124999999999997</v>
       </c>
       <c r="J82">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.83260207291632171</v>
       </c>
+      <c r="K82">
+        <f t="shared" si="20"/>
+        <v>7.1874999999999994E-2</v>
+      </c>
       <c r="L82">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>75</v>
       </c>
     </row>
@@ -8465,43 +9101,47 @@
         <v>76</v>
       </c>
       <c r="B83">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>684</v>
       </c>
       <c r="C83">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.76</v>
       </c>
       <c r="D83" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.6</v>
       </c>
       <c r="E83" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.24000000000000002</v>
       </c>
       <c r="F83">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.34929322162985532</v>
       </c>
       <c r="G83">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.72960000000000014</v>
       </c>
       <c r="H83">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.27799999999999991</v>
       </c>
       <c r="I83">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.41699999999999987</v>
       </c>
       <c r="J83">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.83763362501164373</v>
       </c>
+      <c r="K83">
+        <f t="shared" si="20"/>
+        <v>6.9499999999999978E-2</v>
+      </c>
       <c r="L83">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>76</v>
       </c>
     </row>
@@ -8510,43 +9150,47 @@
         <v>77</v>
       </c>
       <c r="B84">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>693</v>
       </c>
       <c r="C84">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.77</v>
       </c>
       <c r="D84" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.45</v>
       </c>
       <c r="E84" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.23</v>
       </c>
       <c r="F84">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.33914380236100528</v>
       </c>
       <c r="G84">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.70839999999999992</v>
       </c>
       <c r="H84">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.26850000000000007</v>
       </c>
       <c r="I84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.40275000000000011</v>
       </c>
       <c r="J84">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.84207027277716995</v>
       </c>
+      <c r="K84">
+        <f t="shared" si="20"/>
+        <v>6.7125000000000018E-2</v>
+      </c>
       <c r="L84">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>77</v>
       </c>
     </row>
@@ -8555,43 +9199,47 @@
         <v>78</v>
       </c>
       <c r="B85">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>702</v>
       </c>
       <c r="C85">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.78</v>
       </c>
       <c r="D85" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.3000000000000003</v>
       </c>
       <c r="E85" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.22000000000000003</v>
       </c>
       <c r="F85">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.3286113861386139</v>
       </c>
       <c r="G85">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.68640000000000012</v>
       </c>
       <c r="H85">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.25900000000000001</v>
       </c>
       <c r="I85">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.38850000000000001</v>
       </c>
       <c r="J85">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.84584655376734597</v>
       </c>
+      <c r="K85">
+        <f t="shared" si="20"/>
+        <v>6.4750000000000002E-2</v>
+      </c>
       <c r="L85">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>78</v>
       </c>
     </row>
@@ -8600,43 +9248,47 @@
         <v>79</v>
       </c>
       <c r="B86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>711</v>
       </c>
       <c r="C86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.79</v>
       </c>
       <c r="D86" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.15</v>
       </c>
       <c r="E86" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.21</v>
       </c>
       <c r="F86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.31769597296268087</v>
       </c>
       <c r="G86">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.66360000000000008</v>
       </c>
       <c r="H86">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.24950000000000006</v>
       </c>
       <c r="I86">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.37425000000000008</v>
       </c>
       <c r="J86">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.84888703530442433</v>
       </c>
+      <c r="K86">
+        <f t="shared" si="20"/>
+        <v>6.2375000000000014E-2</v>
+      </c>
       <c r="L86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>79</v>
       </c>
     </row>
@@ -8645,43 +9297,47 @@
         <v>80</v>
       </c>
       <c r="B87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>720</v>
       </c>
       <c r="C87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.8</v>
       </c>
       <c r="D87" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="E87" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.2</v>
       </c>
       <c r="F87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.3063975628332064</v>
       </c>
       <c r="G87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.64000000000000012</v>
       </c>
       <c r="H87">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.24</v>
       </c>
       <c r="I87">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.36</v>
       </c>
       <c r="J87">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.85110434120335121</v>
       </c>
+      <c r="K87">
+        <f t="shared" si="20"/>
+        <v>0.06</v>
+      </c>
       <c r="L87">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>80</v>
       </c>
     </row>
@@ -8690,43 +9346,47 @@
         <v>81</v>
       </c>
       <c r="B88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>729</v>
       </c>
       <c r="C88">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.81</v>
       </c>
       <c r="D88" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.85</v>
       </c>
       <c r="E88" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.19</v>
       </c>
       <c r="F88">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.29471615575019044</v>
       </c>
       <c r="G88">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.61560000000000015</v>
       </c>
       <c r="H88">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.23049999999999993</v>
       </c>
       <c r="I88">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.34574999999999989</v>
       </c>
       <c r="J88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.85239669052838907</v>
       </c>
+      <c r="K88">
+        <f t="shared" si="20"/>
+        <v>5.7624999999999982E-2</v>
+      </c>
       <c r="L88">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>81</v>
       </c>
     </row>
@@ -8735,43 +9395,47 @@
         <v>82</v>
       </c>
       <c r="B89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>738</v>
       </c>
       <c r="C89">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.82</v>
       </c>
       <c r="D89" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.7</v>
       </c>
       <c r="E89" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.18000000000000002</v>
       </c>
       <c r="F89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.28265175171363294</v>
       </c>
       <c r="G89">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.59040000000000015</v>
       </c>
       <c r="H89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.22100000000000009</v>
       </c>
       <c r="I89">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.33150000000000013</v>
       </c>
       <c r="J89">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.85264480154942035</v>
       </c>
+      <c r="K89">
+        <f t="shared" si="20"/>
+        <v>5.5250000000000021E-2</v>
+      </c>
       <c r="L89">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>82</v>
       </c>
     </row>
@@ -8780,43 +9444,47 @@
         <v>83</v>
       </c>
       <c r="B90">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>747.00000000000011</v>
       </c>
       <c r="C90">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.83000000000000007</v>
       </c>
       <c r="D90" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.5500000000000003</v>
       </c>
       <c r="E90" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.17</v>
       </c>
       <c r="F90">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.27020435072353394</v>
       </c>
       <c r="G90">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.56440000000000012</v>
       </c>
       <c r="H90">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.21150000000000002</v>
       </c>
       <c r="I90">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.31725000000000003</v>
       </c>
       <c r="J90">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.85170796130349535</v>
       </c>
+      <c r="K90">
+        <f t="shared" si="20"/>
+        <v>5.2875000000000005E-2</v>
+      </c>
       <c r="L90">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>83</v>
       </c>
     </row>
@@ -8825,43 +9493,47 @@
         <v>84</v>
       </c>
       <c r="B91">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>756</v>
       </c>
       <c r="C91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.84</v>
       </c>
       <c r="D91" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.4</v>
       </c>
       <c r="E91" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.16</v>
       </c>
       <c r="F91">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.25737395277989339</v>
       </c>
       <c r="G91">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.53760000000000008</v>
       </c>
       <c r="H91">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.20199999999999996</v>
       </c>
       <c r="I91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.30299999999999994</v>
       </c>
       <c r="J91">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.84941898607225563</v>
       </c>
+      <c r="K91">
+        <f t="shared" si="20"/>
+        <v>5.0499999999999989E-2</v>
+      </c>
       <c r="L91">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>84</v>
       </c>
     </row>
@@ -8870,43 +9542,47 @@
         <v>85</v>
       </c>
       <c r="B92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>765</v>
       </c>
       <c r="C92">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.85</v>
       </c>
       <c r="D92" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.25</v>
       </c>
       <c r="E92" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.15</v>
       </c>
       <c r="F92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.24416055788271135</v>
       </c>
       <c r="G92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.51</v>
       </c>
       <c r="H92">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1925</v>
       </c>
       <c r="I92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.28875000000000001</v>
       </c>
       <c r="J92">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.84557768963709556</v>
       </c>
+      <c r="K92">
+        <f t="shared" si="20"/>
+        <v>4.8125000000000001E-2</v>
+      </c>
       <c r="L92">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>85</v>
       </c>
     </row>
@@ -8915,43 +9591,47 @@
         <v>86</v>
       </c>
       <c r="B93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>774</v>
       </c>
       <c r="C93">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.86</v>
       </c>
       <c r="D93" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.1</v>
       </c>
       <c r="E93" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="F93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.23056416603198784</v>
       </c>
       <c r="G93">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.48160000000000014</v>
       </c>
       <c r="H93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.18299999999999994</v>
       </c>
       <c r="I93">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.27449999999999991</v>
       </c>
       <c r="J93">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.83994231705642231</v>
       </c>
+      <c r="K93">
+        <f t="shared" si="20"/>
+        <v>4.5749999999999985E-2</v>
+      </c>
       <c r="L93">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>86</v>
       </c>
     </row>
@@ -8960,43 +9640,47 @@
         <v>87</v>
       </c>
       <c r="B94">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>783</v>
       </c>
       <c r="C94">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.87</v>
       </c>
       <c r="D94" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.95</v>
       </c>
       <c r="E94" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.13</v>
       </c>
       <c r="F94">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.21658477722772276</v>
       </c>
       <c r="G94">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.45240000000000002</v>
       </c>
       <c r="H94">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1735000000000001</v>
       </c>
       <c r="I94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.26025000000000015</v>
       </c>
       <c r="J94">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.83221816417952987</v>
       </c>
+      <c r="K94">
+        <f t="shared" si="20"/>
+        <v>4.3375000000000025E-2</v>
+      </c>
       <c r="L94">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>87</v>
       </c>
     </row>
@@ -9005,43 +9689,47 @@
         <v>88</v>
       </c>
       <c r="B95">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>792</v>
       </c>
       <c r="C95">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.88</v>
       </c>
       <c r="D95" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.8</v>
       </c>
       <c r="E95" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.12000000000000001</v>
       </c>
       <c r="F95">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.20222239146991625</v>
       </c>
       <c r="G95">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.42240000000000011</v>
       </c>
       <c r="H95">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.16400000000000003</v>
       </c>
       <c r="I95">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.24600000000000005</v>
       </c>
       <c r="J95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.82204224174762686</v>
       </c>
+      <c r="K95">
+        <f t="shared" si="20"/>
+        <v>4.1000000000000009E-2</v>
+      </c>
       <c r="L95">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>88</v>
       </c>
     </row>
@@ -9050,43 +9738,47 @@
         <v>89</v>
       </c>
       <c r="B96">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>801</v>
       </c>
       <c r="C96">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.89</v>
       </c>
       <c r="D96" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.6500000000000001</v>
       </c>
       <c r="E96" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.11000000000000001</v>
       </c>
       <c r="F96">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.18747700875856821</v>
       </c>
       <c r="G96">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.39160000000000011</v>
       </c>
       <c r="H96">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.15449999999999997</v>
       </c>
       <c r="I96">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.23174999999999996</v>
       </c>
       <c r="J96">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.80896228159036998</v>
       </c>
+      <c r="K96">
+        <f t="shared" si="20"/>
+        <v>3.8624999999999993E-2</v>
+      </c>
       <c r="L96">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>89</v>
       </c>
     </row>
@@ -9095,43 +9787,47 @@
         <v>90</v>
       </c>
       <c r="B97">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>810</v>
       </c>
       <c r="C97">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.9</v>
       </c>
       <c r="D97" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
       <c r="E97" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.1</v>
       </c>
       <c r="F97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.1723486290936786</v>
       </c>
       <c r="G97">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.36000000000000004</v>
       </c>
       <c r="H97">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.14500000000000002</v>
       </c>
       <c r="I97">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21750000000000003</v>
       </c>
       <c r="J97">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.79240749008587852</v>
       </c>
+      <c r="K97">
+        <f t="shared" si="20"/>
+        <v>3.6250000000000004E-2</v>
+      </c>
       <c r="L97">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>90</v>
       </c>
     </row>
@@ -9140,43 +9836,47 @@
         <v>91</v>
       </c>
       <c r="B98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>819</v>
       </c>
       <c r="C98">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.91</v>
       </c>
       <c r="D98" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.35</v>
       </c>
       <c r="E98" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.0000000000000011E-2</v>
       </c>
       <c r="F98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.15683725247524755</v>
       </c>
       <c r="G98">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.32760000000000006</v>
       </c>
       <c r="H98">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.13549999999999995</v>
       </c>
       <c r="I98">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.20324999999999993</v>
       </c>
       <c r="J98">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.77164699864820463</v>
       </c>
+      <c r="K98">
+        <f t="shared" si="20"/>
+        <v>3.3874999999999988E-2</v>
+      </c>
       <c r="L98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>91</v>
       </c>
     </row>
@@ -9185,43 +9885,47 @@
         <v>92</v>
       </c>
       <c r="B99">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>828</v>
       </c>
       <c r="C99">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.92</v>
       </c>
       <c r="D99" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.2</v>
       </c>
       <c r="E99" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.08</v>
       </c>
       <c r="F99">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14094287890327492</v>
       </c>
       <c r="G99">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.2944</v>
       </c>
       <c r="H99">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.12600000000000011</v>
       </c>
       <c r="I99">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.18900000000000017</v>
       </c>
       <c r="J99">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.74572951800674492</v>
       </c>
+      <c r="K99">
+        <f t="shared" si="20"/>
+        <v>3.1500000000000028E-2</v>
+      </c>
       <c r="L99">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>92</v>
       </c>
     </row>
@@ -9230,43 +9934,47 @@
         <v>93</v>
       </c>
       <c r="B100">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>837</v>
       </c>
       <c r="C100">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.93</v>
       </c>
       <c r="D100" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.05</v>
       </c>
       <c r="E100" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F100">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.12466550837776084</v>
       </c>
       <c r="G100">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.26040000000000002</v>
       </c>
       <c r="H100">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.11650000000000005</v>
       </c>
       <c r="I100">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.17475000000000007</v>
       </c>
       <c r="J100">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.71339346711164975</v>
       </c>
+      <c r="K100">
+        <f t="shared" si="20"/>
+        <v>2.9125000000000012E-2</v>
+      </c>
       <c r="L100">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>93</v>
       </c>
     </row>
@@ -9275,43 +9983,47 @@
         <v>94</v>
       </c>
       <c r="B101">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>846</v>
       </c>
       <c r="C101">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.94</v>
       </c>
       <c r="D101" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.9</v>
       </c>
       <c r="E101" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="F101">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.10800514089870525</v>
       </c>
       <c r="G101">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.22560000000000002</v>
       </c>
       <c r="H101">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.10699999999999998</v>
       </c>
       <c r="I101">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.16049999999999998</v>
       </c>
       <c r="J101">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.67292922678321032</v>
       </c>
+      <c r="K101">
+        <f t="shared" si="20"/>
+        <v>2.6749999999999996E-2</v>
+      </c>
       <c r="L101">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>94</v>
       </c>
     </row>
@@ -9320,43 +10032,47 @@
         <v>95</v>
       </c>
       <c r="B102">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>855.00000000000011</v>
       </c>
       <c r="C102">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.95000000000000018</v>
       </c>
       <c r="D102" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.75</v>
       </c>
       <c r="E102" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.05</v>
       </c>
       <c r="F102">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.096177646610816E-2</v>
       </c>
       <c r="G102">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.19000000000000003</v>
       </c>
       <c r="H102">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.7500000000000031E-2</v>
       </c>
       <c r="I102">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.14625000000000005</v>
       </c>
       <c r="J102">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.6219608647255257</v>
       </c>
+      <c r="K102">
+        <f t="shared" si="20"/>
+        <v>2.4375000000000008E-2</v>
+      </c>
       <c r="L102">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>95</v>
       </c>
     </row>
@@ -9365,43 +10081,47 @@
         <v>96</v>
       </c>
       <c r="B103">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>864</v>
       </c>
       <c r="C103">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.96</v>
       </c>
       <c r="D103" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
       <c r="E103" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.04</v>
       </c>
       <c r="F103">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>7.3535415079969538E-2</v>
       </c>
       <c r="G103">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.15360000000000001</v>
       </c>
       <c r="H103">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.8000000000000078E-2</v>
       </c>
       <c r="I103">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.13200000000000012</v>
       </c>
       <c r="J103">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.55708647787855659</v>
       </c>
+      <c r="K103">
+        <f t="shared" si="20"/>
+        <v>2.200000000000002E-2</v>
+      </c>
       <c r="L103">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>96</v>
       </c>
     </row>
@@ -9410,43 +10130,47 @@
         <v>97</v>
       </c>
       <c r="B104">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>873</v>
       </c>
       <c r="C104">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.97</v>
       </c>
       <c r="D104" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.45</v>
       </c>
       <c r="E104" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.0000000000000002E-2</v>
       </c>
       <c r="F104">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.5726056740289423E-2</v>
       </c>
       <c r="G104">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.11640000000000003</v>
       </c>
       <c r="H104">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.8500000000000014E-2</v>
       </c>
       <c r="I104">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.11775000000000002</v>
       </c>
       <c r="J104">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.47325738208313728</v>
       </c>
+      <c r="K104">
+        <f t="shared" si="20"/>
+        <v>1.9625000000000004E-2</v>
+      </c>
       <c r="L104">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>97</v>
       </c>
     </row>
@@ -9455,43 +10179,47 @@
         <v>98</v>
       </c>
       <c r="B105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>882</v>
       </c>
       <c r="C105">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.98</v>
       </c>
       <c r="D105" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.3</v>
       </c>
       <c r="E105" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.02</v>
       </c>
       <c r="F105">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3.7533701447067781E-2</v>
       </c>
       <c r="G105">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.8399999999999997E-2</v>
       </c>
       <c r="H105">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.9000000000000061E-2</v>
       </c>
       <c r="I105">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.10350000000000009</v>
       </c>
       <c r="J105">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.36264445842577536</v>
       </c>
+      <c r="K105">
+        <f t="shared" si="20"/>
+        <v>1.7250000000000015E-2</v>
+      </c>
       <c r="L105">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>98</v>
       </c>
     </row>
@@ -9500,43 +10228,47 @@
         <v>99</v>
       </c>
       <c r="B106">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>891</v>
       </c>
       <c r="C106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.99</v>
       </c>
       <c r="D106" s="47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.15</v>
       </c>
       <c r="E106" s="47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.01</v>
       </c>
       <c r="F106">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.8958349200304647E-2</v>
       </c>
       <c r="G106">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.960000000000001E-2</v>
       </c>
       <c r="H106">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="I106">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.9249999999999996E-2</v>
       </c>
       <c r="J106">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.21241847843478598</v>
       </c>
+      <c r="K106">
+        <f t="shared" si="20"/>
+        <v>1.4874999999999999E-2</v>
+      </c>
       <c r="L106">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>99</v>
       </c>
     </row>
@@ -9545,43 +10277,47 @@
         <v>100</v>
       </c>
       <c r="B107">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>900</v>
       </c>
       <c r="C107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="D107" s="47">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E107" s="47">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F107">
+      <c r="E107" s="47">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G107">
+      <c r="F107">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
+      <c r="G107">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
       <c r="H107">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="I107">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.5000000000000067E-2</v>
       </c>
       <c r="J107">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
+      <c r="K107">
+        <f t="shared" si="20"/>
+        <v>1.2500000000000011E-2</v>
+      </c>
       <c r="L107">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>100</v>
       </c>
     </row>
@@ -9591,8 +10327,12 @@
         <v>0.47874619192688495</v>
       </c>
       <c r="G108">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="20"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work on motor formulas.  Not even wolfram can properly solve the power equations....
</commit_message>
<xml_diff>
--- a/Resources/PartBalance.xlsx
+++ b/Resources/PartBalance.xlsx
@@ -1,23 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BaseStats" sheetId="1" r:id="rId1"/>
     <sheet name="ScaledStats" sheetId="2" r:id="rId2"/>
     <sheet name="Graph" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet2!$C$21:$C$22</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Sheet2!$F$21:$F$31</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet2!$C$21</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">Sheet2!$D$21:$D$31</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
   <si>
     <t>Repulsor</t>
   </si>
@@ -285,14 +318,45 @@
   <si>
     <t>what are the relationships between these values?</t>
   </si>
+  <si>
+    <t>&lt;---wtf is up with this?</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>yhat</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>mgc from solver</t>
+  </si>
+  <si>
+    <t>{{0.001,3.7585},{0.05,2.6715},{0.1,2.309},{0.15,2.0784},{0.2,1.9098},{0.25,1.7776},{0.3,1.6697},{0.35,1.579},{0.4,1.501},{0.45,1.4328},{0.5,1.3725}}</t>
+  </si>
+  <si>
+    <t>mgc from wolfram</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -857,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -994,6 +1058,21 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,18 +1097,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2736,11 +2803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="130212544"/>
-        <c:axId val="130209800"/>
+        <c:axId val="152999808"/>
+        <c:axId val="153001344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130212544"/>
+        <c:axId val="152999808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2797,12 +2864,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130209800"/>
+        <c:crossAx val="153001344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130209800"/>
+        <c:axId val="153001344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2859,7 +2926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130212544"/>
+        <c:crossAx val="152999808"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4547,301 +4614,301 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6530179148062315E-3</c:v>
+                  <c:v>2.0582353974546733E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.728823456253269E-2</c:v>
+                  <c:v>4.1080194711126207E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5905155971739344E-2</c:v>
+                  <c:v>6.1491444015362169E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4503269723919948E-2</c:v>
+                  <c:v>8.1813954992237869E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3082044084268474E-2</c:v>
+                  <c:v>0.10204550918356921</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.1640927082827852E-2</c:v>
+                  <c:v>0.12218381356114935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0179345542684122E-2</c:v>
+                  <c:v>0.14222649736700138</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.8696704051612129E-2</c:v>
+                  <c:v>0.16217110879159394</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.7192383873295148E-2</c:v>
+                  <c:v>0.1820151114802393</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.566574179393581E-2</c:v>
+                  <c:v>0.20175588085721691</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4116108899740383E-2</c:v>
+                  <c:v>0.22139070025643051</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.10254278928039431</c:v>
+                  <c:v>0.24091675684661182</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11094505865324863</c:v>
+                  <c:v>0.26033113733823338</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.11932216290250172</c:v>
+                  <c:v>0.27963082345836099</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.12767331652718567</c:v>
+                  <c:v>0.2988126871786812</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13599770099124517</c:v>
+                  <c:v>0.31787348568085072</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.14429446296842649</c:v>
+                  <c:v>0.33680985604214309</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.152562712474069</c:v>
+                  <c:v>0.35561830962309454</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.16080152087520327</c:v>
+                  <c:v>0.37429522613746891</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1690099187696078</c:v>
+                  <c:v>0.39283684738336427</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.17718689372364294</c:v>
+                  <c:v>0.41123927061265109</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.18533138785777004</c:v>
+                  <c:v>0.42949844151416616</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.19344229526765433</c:v>
+                  <c:v>0.4476101467841514</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.2015184592676395</c:v>
+                  <c:v>0.46557000625533373</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.20955866944215484</c:v>
+                  <c:v>0.48337346455374897</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.21756165848925815</c:v>
+                  <c:v>0.50101578224991949</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.22552609883901545</c:v>
+                  <c:v>0.51849202646826642</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.23345059902775236</c:v>
+                  <c:v>0.53579706091566071</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.24133369980736674</c:v>
+                  <c:v>0.55292553528676069</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.24917386996683616</c:v>
+                  <c:v>0.56987187400020933</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.25696950184077377</c:v>
+                  <c:v>0.58663026421586906</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.2647189064773407</c:v>
+                  <c:v>0.60319464307897219</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.27242030843498788</c:v>
+                  <c:v>0.61955868413237059</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.28007184017433345</c:v>
+                  <c:v>0.63571578283288666</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.28767153600794104</c:v>
+                  <c:v>0.65165904110209139</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.2952173255667942</c:v>
+                  <c:v>0.66738125083555822</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.30270702673782207</c:v>
+                  <c:v>0.68287487628775101</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.31013833802182816</c:v>
+                  <c:v>0.69813203524207368</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.31750883025556198</c:v>
+                  <c:v>0.71314447886720567</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.32481593763533995</c:v>
+                  <c:v>0.72790357015152796</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.3320569479724827</c:v>
+                  <c:v>0.74240026079715471</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.33922899210276025</c:v>
+                  <c:v>0.75662506644365157</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.3463290323629008</c:v>
+                  <c:v>0.77056804007885449</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.35335385003685549</c:v>
+                  <c:v>0.78421874348012355</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.36030003166273</c:v>
+                  <c:v>0.79756621651368564</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.36716395407789959</c:v>
+                  <c:v>0.81059894410228672</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.37394176806453233</c:v>
+                  <c:v>0.82330482065188981</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.38062938044028566</c:v>
+                  <c:v>0.83567111170642927</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.38722243441894549</c:v>
+                  <c:v>0.84768441257531135</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.39371628804283632</c:v>
+                  <c:v>0.85933060365110925</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.40010599046245948</c:v>
+                  <c:v>0.87059480210437379</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.4063862558084253</c:v>
+                  <c:v>0.8814613096081515</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.41255143436565045</c:v>
+                  <c:v>0.891913555706214</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.41859548071916186</c:v>
+                  <c:v>0.9019340363955024</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.42451191849371173</c:v>
+                  <c:v>0.91150424744421243</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.43029380125455796</c:v>
+                  <c:v>0.92060461191144938</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.43593366907280945</c:v>
+                  <c:v>0.92921440127155985</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.44142350018392651</c:v>
+                  <c:v>0.93731164947497114</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.4467546570802487</c:v>
+                  <c:v>0.94487305919637898</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.45191782627525551</c:v>
+                  <c:v>0.9518738994289212</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.45690295085556465</c:v>
+                  <c:v>0.95828789347780752</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.46169915479267631</c:v>
+                  <c:v>0.96408709628667322</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.46629465781553647</c:v>
+                  <c:v>0.96924175989229144</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.47067667944139824</c:v>
+                  <c:v>0.9737201856453227</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.47483133051913146</c:v>
+                  <c:v>0.97748856165313691</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.4787434903472596</c:v>
+                  <c:v>0.98051078369140132</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.48239666707757284</c:v>
+                  <c:v>0.9827482575892772</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.4857728386903778</c:v>
+                  <c:v>0.98415968081305982</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.48885227131186781</c:v>
+                  <c:v>0.98470080064806564</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.49161331101564981</c:v>
+                  <c:v>0.98432414600036189</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.49403214448100846</c:v>
+                  <c:v>0.9829787293986858</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.49608252293397359</c:v>
+                  <c:v>0.98060971526073737</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.49773544262721481</c:v>
+                  <c:v>0.97715804988250177</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.49895877366099323</c:v>
+                  <c:v>0.97256004789690242</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.49971682713129228</c:v>
+                  <c:v>0.96674692910749793</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.49996984830958663</c:v>
+                  <c:v>0.95964429860793277</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.49967342067508097</c:v>
+                  <c:v>0.95117156191632157</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.49877776195279039</c:v>
+                  <c:v>0.94124126544593856</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.49722688861548242</c:v>
+                  <c:v>0.92975835095034176</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.49495761925385129</c:v>
+                  <c:v>0.91661931056118318</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.49189837935624914</c:v>
+                  <c:v>0.90171122660390257</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.4879677597453046</c:v>
+                  <c:v>0.88491067743421226</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.48307276732908011</c:v>
+                  <c:v>0.86608248696551104</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.47710668872338463</c:v>
+                  <c:v>0.84507829120031042</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.46994646296176845</c:v>
+                  <c:v>0.82173488974137321</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.46144942644595788</c:v>
+                  <c:v>0.79587234368918136</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.45144924788395635</c:v>
+                  <c:v>0.7672917732074247</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.43975080787553716</c:v>
+                  <c:v>0.73577279793694983</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.42612368903852299</c:v>
+                  <c:v>0.70107055081202985</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.41029381596042941</c:v>
+                  <c:v>0.66291217995942708</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.39193260099203459</c:v>
+                  <c:v>0.62099273328552229</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.3706426823249771</c:v>
+                  <c:v>0.57497029480656048</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.34593893726070557</c:v>
+                  <c:v>0.52446020904081769</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.31722283779451393</c:v>
+                  <c:v>0.46902818754118625</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.28374725586535449</c:v>
+                  <c:v>0.408182036734277</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.24456729421955006</c:v>
+                  <c:v>0.34136167427795788</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.19847021071261714</c:v>
+                  <c:v>0.26792700606693509</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.14387327407124664</c:v>
+                  <c:v>0.18714310923957489</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>7.8671016087825452E-2</c:v>
+                  <c:v>9.816199587860748E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>0</c:v>
@@ -4859,11 +4926,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="130213328"/>
-        <c:axId val="130206272"/>
+        <c:axId val="152744704"/>
+        <c:axId val="152746240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130213328"/>
+        <c:axId val="152744704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4920,12 +4987,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130206272"/>
+        <c:crossAx val="152746240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130206272"/>
+        <c:axId val="152746240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4982,7 +5049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="130213328"/>
+        <c:crossAx val="152744704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5292,11 +5359,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405946304"/>
-        <c:axId val="405944736"/>
+        <c:axId val="152688896"/>
+        <c:axId val="152690688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405946304"/>
+        <c:axId val="152688896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5353,12 +5420,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405944736"/>
+        <c:crossAx val="152690688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405944736"/>
+        <c:axId val="152690688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5415,7 +5482,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405946304"/>
+        <c:crossAx val="152688896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5456,6 +5523,382 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$5:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$5:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7585000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6715</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3090000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0783999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9097999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7776000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6697</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.579</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4328000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3725000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="152786432"/>
+        <c:axId val="152787968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152786432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152787968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152787968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152786432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$21:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$21:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>3.7585000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3090000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0783999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9097999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7776000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6697</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.579</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4328000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3725000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="152807680"/>
+        <c:axId val="198967296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152807680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="198967296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="198967296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4.5"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152807680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -7236,6 +7679,73 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7279,7 +7789,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7314,7 +7824,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7560,39 +8070,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="63" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="58" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="60"/>
+      <c r="X1" s="75"/>
       <c r="Y1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="61" t="s">
+      <c r="Z1" s="76" t="s">
         <v>38</v>
       </c>
     </row>
@@ -7669,7 +8179,7 @@
       <c r="Y2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="62"/>
+      <c r="Z2" s="77"/>
       <c r="AA2" t="s">
         <v>48</v>
       </c>
@@ -14224,8 +14734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14266,7 +14776,7 @@
       </c>
       <c r="J1" s="55">
         <f>L108</f>
-        <v>0.49996984830958663</v>
+        <v>0.98470080064806564</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -14274,21 +14784,21 @@
         <v>68</v>
       </c>
       <c r="B2" s="56">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
       </c>
       <c r="F2">
         <f>1 / B2*F1</f>
-        <v>80504.93145468393</v>
+        <v>40252.465727341965</v>
       </c>
       <c r="I2" t="s">
         <v>69</v>
       </c>
       <c r="J2">
         <f>K108</f>
-        <v>185885.88672886521</v>
+        <v>78069.421237720715</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -14300,7 +14810,7 @@
       </c>
       <c r="G3">
         <f>J2/F2</f>
-        <v>2.3090000000000002</v>
+        <v>1.939494136</v>
       </c>
       <c r="K3" t="s">
         <v>81</v>
@@ -14311,9 +14821,9 @@
         <v>60</v>
       </c>
       <c r="B4" s="57">
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="67"/>
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="59"/>
       <c r="E4" t="s">
         <v>82</v>
       </c>
@@ -14321,14 +14831,15 @@
         <f>H89</f>
         <v>23765.055765422698</v>
       </c>
-      <c r="I4" s="66" t="s">
+      <c r="I4" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="J4" s="66" t="s">
+      <c r="J4" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="68">
-        <v>2.3090000000000002</v>
+      <c r="K4" s="60">
+        <f>5.92824117*B4^2 + -5.904378534*B4 + 2.883240196</f>
+        <v>1.939494136</v>
       </c>
       <c r="L4" t="s">
         <v>83</v>
@@ -14422,7 +14933,7 @@
       </c>
       <c r="K7">
         <f>J7 * $F$2 * $K$4</f>
-        <v>185885.88672886521</v>
+        <v>78069.421237720715</v>
       </c>
       <c r="L7">
         <f>IFERROR(H7/K7,1)</f>
@@ -14467,15 +14978,15 @@
       </c>
       <c r="J8">
         <f t="shared" ref="J8:J71" si="8">(100-A8) * 0.01 * (1 - $B$4) + $B$4</f>
-        <v>0.99099999999999999</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="K8">
         <f t="shared" ref="K8:K71" si="9">J8 * $F$2 * $K$4</f>
-        <v>184212.91374830541</v>
+        <v>77444.865867818953</v>
       </c>
       <c r="L8">
         <f t="shared" ref="L8:L71" si="10">IFERROR(H8/K8,1)</f>
-        <v>8.6530179148062315E-3</v>
+        <v>2.0582353974546733E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -14516,15 +15027,15 @@
       </c>
       <c r="J9">
         <f t="shared" si="8"/>
-        <v>0.98199999999999998</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="K9">
         <f t="shared" si="9"/>
-        <v>182539.94076774563</v>
+        <v>76820.310497917177</v>
       </c>
       <c r="L9">
         <f t="shared" si="10"/>
-        <v>1.728823456253269E-2</v>
+        <v>4.1080194711126207E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -14565,15 +15076,15 @@
       </c>
       <c r="J10">
         <f t="shared" si="8"/>
-        <v>0.97299999999999998</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="K10">
         <f t="shared" si="9"/>
-        <v>180866.96778718583</v>
+        <v>76195.755128015415</v>
       </c>
       <c r="L10">
         <f t="shared" si="10"/>
-        <v>2.5905155971739344E-2</v>
+        <v>6.1491444015362169E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -14614,15 +15125,15 @@
       </c>
       <c r="J11">
         <f t="shared" si="8"/>
-        <v>0.96399999999999997</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="K11">
         <f t="shared" si="9"/>
-        <v>179193.99480662603</v>
+        <v>75571.199758113653</v>
       </c>
       <c r="L11">
         <f t="shared" si="10"/>
-        <v>3.4503269723919948E-2</v>
+        <v>8.1813954992237869E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -14663,15 +15174,15 @@
       </c>
       <c r="J12">
         <f t="shared" si="8"/>
-        <v>0.95500000000000007</v>
+        <v>0.96000000000000019</v>
       </c>
       <c r="K12">
         <f t="shared" si="9"/>
-        <v>177521.02182606628</v>
+        <v>74946.644388211906</v>
       </c>
       <c r="L12">
         <f t="shared" si="10"/>
-        <v>4.3082044084268474E-2</v>
+        <v>0.10204550918356921</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -14712,15 +15223,15 @@
       </c>
       <c r="J13">
         <f t="shared" si="8"/>
-        <v>0.94600000000000006</v>
+        <v>0.95200000000000018</v>
       </c>
       <c r="K13">
         <f t="shared" si="9"/>
-        <v>175848.04884550648</v>
+        <v>74322.089018310129</v>
       </c>
       <c r="L13">
         <f t="shared" si="10"/>
-        <v>5.1640927082827852E-2</v>
+        <v>0.12218381356114935</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -14761,15 +15272,15 @@
       </c>
       <c r="J14">
         <f t="shared" si="8"/>
-        <v>0.93700000000000006</v>
+        <v>0.94400000000000017</v>
       </c>
       <c r="K14">
         <f t="shared" si="9"/>
-        <v>174175.0758649467</v>
+        <v>73697.533648408367</v>
       </c>
       <c r="L14">
         <f t="shared" si="10"/>
-        <v>6.0179345542684122E-2</v>
+        <v>0.14222649736700138</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -14810,15 +15321,15 @@
       </c>
       <c r="J15">
         <f t="shared" si="8"/>
-        <v>0.92800000000000005</v>
+        <v>0.93600000000000017</v>
       </c>
       <c r="K15">
         <f t="shared" si="9"/>
-        <v>172502.10288438693</v>
+        <v>73072.978278506605</v>
       </c>
       <c r="L15">
         <f t="shared" si="10"/>
-        <v>6.8696704051612129E-2</v>
+        <v>0.16217110879159394</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -14859,15 +15370,15 @@
       </c>
       <c r="J16">
         <f t="shared" si="8"/>
-        <v>0.91900000000000004</v>
+        <v>0.92800000000000016</v>
       </c>
       <c r="K16">
         <f t="shared" si="9"/>
-        <v>170829.12990382715</v>
+        <v>72448.422908604829</v>
       </c>
       <c r="L16">
         <f t="shared" si="10"/>
-        <v>7.7192383873295148E-2</v>
+        <v>0.1820151114802393</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -14908,15 +15419,15 @@
       </c>
       <c r="J17">
         <f t="shared" si="8"/>
-        <v>0.91</v>
+        <v>0.92000000000000015</v>
       </c>
       <c r="K17">
         <f t="shared" si="9"/>
-        <v>169156.15692326735</v>
+        <v>71823.867538703082</v>
       </c>
       <c r="L17">
         <f t="shared" si="10"/>
-        <v>8.566574179393581E-2</v>
+        <v>0.20175588085721691</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -14957,15 +15468,15 @@
       </c>
       <c r="J18">
         <f t="shared" si="8"/>
-        <v>0.90100000000000002</v>
+        <v>0.91200000000000014</v>
       </c>
       <c r="K18">
         <f t="shared" si="9"/>
-        <v>167483.18394270758</v>
+        <v>71199.312168801305</v>
       </c>
       <c r="L18">
         <f t="shared" si="10"/>
-        <v>9.4116108899740383E-2</v>
+        <v>0.22139070025643051</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -15006,15 +15517,15 @@
       </c>
       <c r="J19">
         <f t="shared" si="8"/>
-        <v>0.89200000000000002</v>
+        <v>0.90400000000000014</v>
       </c>
       <c r="K19">
         <f t="shared" si="9"/>
-        <v>165810.21096214777</v>
+        <v>70574.756798899543</v>
       </c>
       <c r="L19">
         <f t="shared" si="10"/>
-        <v>0.10254278928039431</v>
+        <v>0.24091675684661182</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -15055,15 +15566,15 @@
       </c>
       <c r="J20">
         <f t="shared" si="8"/>
-        <v>0.88300000000000001</v>
+        <v>0.89600000000000013</v>
       </c>
       <c r="K20">
         <f t="shared" si="9"/>
-        <v>164137.23798158797</v>
+        <v>69950.201428997767</v>
       </c>
       <c r="L20">
         <f t="shared" si="10"/>
-        <v>0.11094505865324863</v>
+        <v>0.26033113733823338</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -15104,15 +15615,15 @@
       </c>
       <c r="J21">
         <f t="shared" si="8"/>
-        <v>0.874</v>
+        <v>0.88800000000000012</v>
       </c>
       <c r="K21">
         <f t="shared" si="9"/>
-        <v>162464.26500102819</v>
+        <v>69325.646059096005</v>
       </c>
       <c r="L21">
         <f t="shared" si="10"/>
-        <v>0.11932216290250172</v>
+        <v>0.27963082345836099</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -15153,15 +15664,15 @@
       </c>
       <c r="J22">
         <f t="shared" si="8"/>
-        <v>0.86499999999999999</v>
+        <v>0.88000000000000012</v>
       </c>
       <c r="K22">
         <f t="shared" si="9"/>
-        <v>160791.29202046839</v>
+        <v>68701.090689194229</v>
       </c>
       <c r="L22">
         <f t="shared" si="10"/>
-        <v>0.12767331652718567</v>
+        <v>0.2988126871786812</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -15202,15 +15713,15 @@
       </c>
       <c r="J23">
         <f t="shared" si="8"/>
-        <v>0.85599999999999998</v>
+        <v>0.87200000000000011</v>
       </c>
       <c r="K23">
         <f t="shared" si="9"/>
-        <v>159118.31903990859</v>
+        <v>68076.535319292467</v>
       </c>
       <c r="L23">
         <f t="shared" si="10"/>
-        <v>0.13599770099124517</v>
+        <v>0.31787348568085072</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -15251,15 +15762,15 @@
       </c>
       <c r="J24">
         <f t="shared" si="8"/>
-        <v>0.84700000000000009</v>
+        <v>0.8640000000000001</v>
       </c>
       <c r="K24">
         <f t="shared" si="9"/>
-        <v>157445.34605934884</v>
+        <v>67451.979949390705</v>
       </c>
       <c r="L24">
         <f t="shared" si="10"/>
-        <v>0.14429446296842649</v>
+        <v>0.33680985604214309</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -15300,15 +15811,15 @@
       </c>
       <c r="J25">
         <f t="shared" si="8"/>
-        <v>0.83800000000000008</v>
+        <v>0.85600000000000009</v>
       </c>
       <c r="K25">
         <f t="shared" si="9"/>
-        <v>155772.37307878904</v>
+        <v>66827.424579488943</v>
       </c>
       <c r="L25">
         <f t="shared" si="10"/>
-        <v>0.152562712474069</v>
+        <v>0.35561830962309454</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -15349,15 +15860,15 @@
       </c>
       <c r="J26">
         <f t="shared" si="8"/>
-        <v>0.82900000000000007</v>
+        <v>0.84800000000000009</v>
       </c>
       <c r="K26">
         <f t="shared" si="9"/>
-        <v>154099.40009822926</v>
+        <v>66202.869209587181</v>
       </c>
       <c r="L26">
         <f t="shared" si="10"/>
-        <v>0.16080152087520327</v>
+        <v>0.37429522613746891</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -15398,15 +15909,15 @@
       </c>
       <c r="J27">
         <f t="shared" si="8"/>
-        <v>0.82000000000000006</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="K27">
         <f t="shared" si="9"/>
-        <v>152426.42711766946</v>
+        <v>65578.313839685405</v>
       </c>
       <c r="L27">
         <f t="shared" si="10"/>
-        <v>0.1690099187696078</v>
+        <v>0.39283684738336427</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -15447,15 +15958,15 @@
       </c>
       <c r="J28">
         <f t="shared" si="8"/>
-        <v>0.81100000000000005</v>
+        <v>0.83200000000000007</v>
       </c>
       <c r="K28">
         <f t="shared" si="9"/>
-        <v>150753.45413710969</v>
+        <v>64953.758469783643</v>
       </c>
       <c r="L28">
         <f t="shared" si="10"/>
-        <v>0.17718689372364294</v>
+        <v>0.41123927061265109</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -15496,15 +16007,15 @@
       </c>
       <c r="J29">
         <f t="shared" si="8"/>
-        <v>0.80200000000000005</v>
+        <v>0.82400000000000007</v>
       </c>
       <c r="K29">
         <f t="shared" si="9"/>
-        <v>149080.48115654991</v>
+        <v>64329.203099881874</v>
       </c>
       <c r="L29">
         <f t="shared" si="10"/>
-        <v>0.18533138785777004</v>
+        <v>0.42949844151416616</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -15545,15 +16056,15 @@
       </c>
       <c r="J30">
         <f t="shared" si="8"/>
-        <v>0.79300000000000004</v>
+        <v>0.81600000000000006</v>
       </c>
       <c r="K30">
         <f t="shared" si="9"/>
-        <v>147407.50817599014</v>
+        <v>63704.647729980112</v>
       </c>
       <c r="L30">
         <f t="shared" si="10"/>
-        <v>0.19344229526765433</v>
+        <v>0.4476101467841514</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -15594,15 +16105,15 @@
       </c>
       <c r="J31">
         <f t="shared" si="8"/>
-        <v>0.78400000000000003</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="K31">
         <f t="shared" si="9"/>
-        <v>145734.53519543033</v>
+        <v>63080.092360078343</v>
       </c>
       <c r="L31">
         <f t="shared" si="10"/>
-        <v>0.2015184592676395</v>
+        <v>0.46557000625533373</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -15643,15 +16154,15 @@
       </c>
       <c r="J32">
         <f t="shared" si="8"/>
-        <v>0.77500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="K32">
         <f t="shared" si="9"/>
-        <v>144061.56221487053</v>
+        <v>62455.536990176581</v>
       </c>
       <c r="L32">
         <f t="shared" si="10"/>
-        <v>0.20955866944215484</v>
+        <v>0.48337346455374897</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -15692,15 +16203,15 @@
       </c>
       <c r="J33">
         <f t="shared" si="8"/>
-        <v>0.76600000000000001</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="K33">
         <f t="shared" si="9"/>
-        <v>142388.58923431076</v>
+        <v>61830.981620274812</v>
       </c>
       <c r="L33">
         <f t="shared" si="10"/>
-        <v>0.21756165848925815</v>
+        <v>0.50101578224991949</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -15741,15 +16252,15 @@
       </c>
       <c r="J34">
         <f t="shared" si="8"/>
-        <v>0.75700000000000001</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="K34">
         <f t="shared" si="9"/>
-        <v>140715.61625375098</v>
+        <v>61206.426250373042</v>
       </c>
       <c r="L34">
         <f t="shared" si="10"/>
-        <v>0.22552609883901545</v>
+        <v>0.51849202646826642</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -15790,15 +16301,15 @@
       </c>
       <c r="J35">
         <f t="shared" si="8"/>
-        <v>0.748</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="K35">
         <f t="shared" si="9"/>
-        <v>139042.64327319118</v>
+        <v>60581.870880471281</v>
       </c>
       <c r="L35">
         <f t="shared" si="10"/>
-        <v>0.23345059902775236</v>
+        <v>0.53579706091566071</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -15839,15 +16350,15 @@
       </c>
       <c r="J36">
         <f t="shared" si="8"/>
-        <v>0.73899999999999999</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="K36">
         <f t="shared" si="9"/>
-        <v>137369.67029263137</v>
+        <v>59957.315510569511</v>
       </c>
       <c r="L36">
         <f t="shared" si="10"/>
-        <v>0.24133369980736674</v>
+        <v>0.55292553528676069</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -15888,15 +16399,15 @@
       </c>
       <c r="J37">
         <f t="shared" si="8"/>
-        <v>0.73000000000000009</v>
+        <v>0.76</v>
       </c>
       <c r="K37">
         <f t="shared" si="9"/>
-        <v>135696.6973120716</v>
+        <v>59332.760140667742</v>
       </c>
       <c r="L37">
         <f t="shared" si="10"/>
-        <v>0.24917386996683616</v>
+        <v>0.56987187400020933</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -15937,15 +16448,15 @@
       </c>
       <c r="J38">
         <f t="shared" si="8"/>
-        <v>0.72100000000000009</v>
+        <v>0.752</v>
       </c>
       <c r="K38">
         <f t="shared" si="9"/>
-        <v>134023.72433151182</v>
+        <v>58708.204770765973</v>
       </c>
       <c r="L38">
         <f t="shared" si="10"/>
-        <v>0.25696950184077377</v>
+        <v>0.58663026421586906</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15986,15 +16497,15 @@
       </c>
       <c r="J39">
         <f t="shared" si="8"/>
-        <v>0.71200000000000008</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="K39">
         <f t="shared" si="9"/>
-        <v>132350.75135095205</v>
+        <v>58083.649400864211</v>
       </c>
       <c r="L39">
         <f t="shared" si="10"/>
-        <v>0.2647189064773407</v>
+        <v>0.60319464307897219</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -16035,29 +16546,29 @@
       </c>
       <c r="J40">
         <f t="shared" si="8"/>
-        <v>0.70300000000000007</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="K40">
         <f t="shared" si="9"/>
-        <v>130677.77837039225</v>
+        <v>57459.094030962442</v>
       </c>
       <c r="L40">
         <f t="shared" si="10"/>
-        <v>0.27242030843498788</v>
-      </c>
-      <c r="O40" s="69" t="s">
+        <v>0.61955868413237059</v>
+      </c>
+      <c r="O40" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="P40" s="70"/>
-      <c r="Q40" s="70" t="s">
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="R40" s="70"/>
-      <c r="S40" s="70" t="s">
+      <c r="R40" s="62"/>
+      <c r="S40" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="T40" s="70"/>
-      <c r="U40" s="71" t="s">
+      <c r="T40" s="62"/>
+      <c r="U40" s="63" t="s">
         <v>86</v>
       </c>
     </row>
@@ -16099,33 +16610,33 @@
       </c>
       <c r="J41">
         <f t="shared" si="8"/>
-        <v>0.69400000000000006</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="K41">
         <f t="shared" si="9"/>
-        <v>129004.80538983246</v>
+        <v>56834.538661060673</v>
       </c>
       <c r="L41">
         <f t="shared" si="10"/>
-        <v>0.28007184017433345</v>
-      </c>
-      <c r="O41" s="72">
+        <v>0.63571578283288666</v>
+      </c>
+      <c r="O41" s="64">
         <v>0</v>
       </c>
-      <c r="P41" s="73">
+      <c r="P41" s="65">
         <v>3.2</v>
       </c>
-      <c r="Q41" s="73">
+      <c r="Q41" s="65">
         <v>0</v>
       </c>
-      <c r="R41" s="73"/>
-      <c r="S41" s="73">
+      <c r="R41" s="65"/>
+      <c r="S41" s="65">
         <v>0</v>
       </c>
-      <c r="T41" s="73">
+      <c r="T41" s="65">
         <v>4</v>
       </c>
-      <c r="U41" s="74">
+      <c r="U41" s="66">
         <v>0</v>
       </c>
     </row>
@@ -16167,34 +16678,34 @@
       </c>
       <c r="J42">
         <f t="shared" si="8"/>
-        <v>0.68500000000000005</v>
+        <v>0.72</v>
       </c>
       <c r="K42">
         <f t="shared" si="9"/>
-        <v>127331.83240927268</v>
+        <v>56209.983291158918</v>
       </c>
       <c r="L42">
         <f t="shared" si="10"/>
-        <v>0.28767153600794104</v>
-      </c>
-      <c r="O42" s="72">
+        <v>0.65165904110209139</v>
+      </c>
+      <c r="O42" s="64">
         <v>0.05</v>
       </c>
-      <c r="P42" s="73">
+      <c r="P42" s="65">
         <v>2.6715</v>
       </c>
-      <c r="Q42" s="73">
+      <c r="Q42" s="65">
         <f>P41-P42</f>
         <v>0.52850000000000019</v>
       </c>
-      <c r="R42" s="73"/>
-      <c r="S42" s="73">
+      <c r="R42" s="65"/>
+      <c r="S42" s="65">
         <v>0.05</v>
       </c>
-      <c r="T42" s="73">
+      <c r="T42" s="65">
         <v>2.6715</v>
       </c>
-      <c r="U42" s="74">
+      <c r="U42" s="66">
         <f>T41-T42</f>
         <v>1.3285</v>
       </c>
@@ -16237,35 +16748,35 @@
       </c>
       <c r="J43">
         <f t="shared" si="8"/>
-        <v>0.67600000000000005</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="K43">
         <f t="shared" si="9"/>
-        <v>125658.85942871289</v>
+        <v>55585.427921257149</v>
       </c>
       <c r="L43">
         <f t="shared" si="10"/>
-        <v>0.2952173255667942</v>
-      </c>
-      <c r="O43" s="72">
+        <v>0.66738125083555822</v>
+      </c>
+      <c r="O43" s="64">
         <v>0.1</v>
       </c>
-      <c r="P43" s="73">
+      <c r="P43" s="65">
         <v>2.3090000000000002</v>
       </c>
-      <c r="Q43" s="73">
-        <f t="shared" ref="Q43:Q52" si="11">P42-P43</f>
+      <c r="Q43" s="65">
+        <f t="shared" ref="Q43:Q51" si="11">P42-P43</f>
         <v>0.36249999999999982</v>
       </c>
-      <c r="R43" s="73"/>
-      <c r="S43" s="73">
+      <c r="R43" s="65"/>
+      <c r="S43" s="65">
         <v>0.1</v>
       </c>
-      <c r="T43" s="73">
+      <c r="T43" s="65">
         <v>2.3090000000000002</v>
       </c>
-      <c r="U43" s="74">
-        <f t="shared" ref="U43:U52" si="12">T42-T43</f>
+      <c r="U43" s="66">
+        <f t="shared" ref="U43:U51" si="12">T42-T43</f>
         <v>0.36249999999999982</v>
       </c>
     </row>
@@ -16307,34 +16818,34 @@
       </c>
       <c r="J44">
         <f t="shared" si="8"/>
-        <v>0.66700000000000004</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="K44">
         <f t="shared" si="9"/>
-        <v>123985.88644815311</v>
+        <v>54960.87255135538</v>
       </c>
       <c r="L44">
         <f t="shared" si="10"/>
-        <v>0.30270702673782207</v>
-      </c>
-      <c r="O44" s="72">
+        <v>0.68287487628775101</v>
+      </c>
+      <c r="O44" s="64">
         <v>0.15</v>
       </c>
-      <c r="P44" s="73">
+      <c r="P44" s="65">
         <v>2.0783999999999998</v>
       </c>
-      <c r="Q44" s="73">
+      <c r="Q44" s="65">
         <f t="shared" si="11"/>
         <v>0.23060000000000036</v>
       </c>
-      <c r="R44" s="73"/>
-      <c r="S44" s="73">
+      <c r="R44" s="65"/>
+      <c r="S44" s="65">
         <v>0.15</v>
       </c>
-      <c r="T44" s="73">
+      <c r="T44" s="65">
         <v>2.0783999999999998</v>
       </c>
-      <c r="U44" s="74">
+      <c r="U44" s="66">
         <f t="shared" si="12"/>
         <v>0.23060000000000036</v>
       </c>
@@ -16377,34 +16888,34 @@
       </c>
       <c r="J45">
         <f t="shared" si="8"/>
-        <v>0.65800000000000003</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="K45">
         <f t="shared" si="9"/>
-        <v>122312.9134675933</v>
+        <v>54336.317181453618</v>
       </c>
       <c r="L45">
         <f t="shared" si="10"/>
-        <v>0.31013833802182816</v>
-      </c>
-      <c r="O45" s="72">
+        <v>0.69813203524207368</v>
+      </c>
+      <c r="O45" s="64">
         <v>0.2</v>
       </c>
-      <c r="P45" s="73">
+      <c r="P45" s="65">
         <v>1.9097999999999999</v>
       </c>
-      <c r="Q45" s="73">
+      <c r="Q45" s="65">
         <f t="shared" si="11"/>
         <v>0.16859999999999986</v>
       </c>
-      <c r="R45" s="73"/>
-      <c r="S45" s="73">
+      <c r="R45" s="65"/>
+      <c r="S45" s="65">
         <v>0.2</v>
       </c>
-      <c r="T45" s="73">
+      <c r="T45" s="65">
         <v>1.9097999999999999</v>
       </c>
-      <c r="U45" s="74">
+      <c r="U45" s="66">
         <f t="shared" si="12"/>
         <v>0.16859999999999986</v>
       </c>
@@ -16447,34 +16958,34 @@
       </c>
       <c r="J46">
         <f t="shared" si="8"/>
-        <v>0.64900000000000002</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="K46">
         <f t="shared" si="9"/>
-        <v>120639.94048703351</v>
+        <v>53711.761811551849</v>
       </c>
       <c r="L46">
         <f t="shared" si="10"/>
-        <v>0.31750883025556198</v>
-      </c>
-      <c r="O46" s="72">
+        <v>0.71314447886720567</v>
+      </c>
+      <c r="O46" s="64">
         <v>0.25</v>
       </c>
-      <c r="P46" s="73">
+      <c r="P46" s="65">
         <v>1.7776000000000001</v>
       </c>
-      <c r="Q46" s="73">
+      <c r="Q46" s="65">
         <f t="shared" si="11"/>
         <v>0.13219999999999987</v>
       </c>
-      <c r="R46" s="73"/>
-      <c r="S46" s="73">
+      <c r="R46" s="65"/>
+      <c r="S46" s="65">
         <v>0.25</v>
       </c>
-      <c r="T46" s="73">
+      <c r="T46" s="65">
         <v>1.7776000000000001</v>
       </c>
-      <c r="U46" s="74">
+      <c r="U46" s="66">
         <f t="shared" si="12"/>
         <v>0.13219999999999987</v>
       </c>
@@ -16517,34 +17028,34 @@
       </c>
       <c r="J47">
         <f t="shared" si="8"/>
-        <v>0.64</v>
+        <v>0.67999999999999994</v>
       </c>
       <c r="K47">
         <f t="shared" si="9"/>
-        <v>118966.96750647374</v>
+        <v>53087.20644165008</v>
       </c>
       <c r="L47">
         <f t="shared" si="10"/>
-        <v>0.32481593763533995</v>
-      </c>
-      <c r="O47" s="72">
+        <v>0.72790357015152796</v>
+      </c>
+      <c r="O47" s="64">
         <v>0.3</v>
       </c>
-      <c r="P47" s="73">
+      <c r="P47" s="65">
         <v>1.6697</v>
       </c>
-      <c r="Q47" s="73">
+      <c r="Q47" s="65">
         <f>P46-P47</f>
         <v>0.10790000000000011</v>
       </c>
-      <c r="R47" s="73"/>
-      <c r="S47" s="73">
+      <c r="R47" s="65"/>
+      <c r="S47" s="65">
         <v>0.3</v>
       </c>
-      <c r="T47" s="73">
+      <c r="T47" s="65">
         <v>1.6697</v>
       </c>
-      <c r="U47" s="74">
+      <c r="U47" s="66">
         <f t="shared" si="12"/>
         <v>0.10790000000000011</v>
       </c>
@@ -16587,34 +17098,34 @@
       </c>
       <c r="J48">
         <f t="shared" si="8"/>
-        <v>0.63100000000000001</v>
+        <v>0.67199999999999993</v>
       </c>
       <c r="K48">
         <f t="shared" si="9"/>
-        <v>117293.99452591395</v>
+        <v>52462.651071748318</v>
       </c>
       <c r="L48">
         <f t="shared" si="10"/>
-        <v>0.3320569479724827</v>
-      </c>
-      <c r="O48" s="72">
+        <v>0.74240026079715471</v>
+      </c>
+      <c r="O48" s="64">
         <v>0.35</v>
       </c>
-      <c r="P48" s="73">
+      <c r="P48" s="65">
         <v>1.579</v>
       </c>
-      <c r="Q48" s="73">
+      <c r="Q48" s="65">
         <f>P47-P48</f>
         <v>9.0700000000000003E-2</v>
       </c>
-      <c r="R48" s="73"/>
-      <c r="S48" s="73">
+      <c r="R48" s="65"/>
+      <c r="S48" s="65">
         <v>0.35</v>
       </c>
-      <c r="T48" s="73">
+      <c r="T48" s="65">
         <v>1.579</v>
       </c>
-      <c r="U48" s="74">
+      <c r="U48" s="66">
         <f t="shared" si="12"/>
         <v>9.0700000000000003E-2</v>
       </c>
@@ -16657,34 +17168,34 @@
       </c>
       <c r="J49">
         <f t="shared" si="8"/>
-        <v>0.622</v>
+        <v>0.66399999999999992</v>
       </c>
       <c r="K49">
         <f t="shared" si="9"/>
-        <v>115621.02154535416</v>
+        <v>51838.095701846549</v>
       </c>
       <c r="L49">
         <f t="shared" si="10"/>
-        <v>0.33922899210276025</v>
-      </c>
-      <c r="O49" s="72">
+        <v>0.75662506644365157</v>
+      </c>
+      <c r="O49" s="64">
         <v>0.4</v>
       </c>
-      <c r="P49" s="73">
+      <c r="P49" s="65">
         <v>1.5009999999999999</v>
       </c>
-      <c r="Q49" s="73">
+      <c r="Q49" s="65">
         <f>P48-P49</f>
         <v>7.8000000000000069E-2</v>
       </c>
-      <c r="R49" s="73"/>
-      <c r="S49" s="73">
+      <c r="R49" s="65"/>
+      <c r="S49" s="65">
         <v>0.4</v>
       </c>
-      <c r="T49" s="73">
+      <c r="T49" s="65">
         <v>1.5009999999999999</v>
       </c>
-      <c r="U49" s="74">
+      <c r="U49" s="66">
         <f t="shared" si="12"/>
         <v>7.8000000000000069E-2</v>
       </c>
@@ -16727,34 +17238,34 @@
       </c>
       <c r="J50">
         <f t="shared" si="8"/>
-        <v>0.6130000000000001</v>
+        <v>0.65600000000000014</v>
       </c>
       <c r="K50">
         <f t="shared" si="9"/>
-        <v>113948.0485647944</v>
+        <v>51213.540331944801</v>
       </c>
       <c r="L50">
         <f t="shared" si="10"/>
-        <v>0.3463290323629008</v>
-      </c>
-      <c r="O50" s="72">
+        <v>0.77056804007885449</v>
+      </c>
+      <c r="O50" s="64">
         <v>0.45</v>
       </c>
-      <c r="P50" s="73">
+      <c r="P50" s="65">
         <v>1.4328000000000001</v>
       </c>
-      <c r="Q50" s="73">
+      <c r="Q50" s="65">
         <f t="shared" si="11"/>
         <v>6.8199999999999816E-2</v>
       </c>
-      <c r="R50" s="73"/>
-      <c r="S50" s="73">
+      <c r="R50" s="65"/>
+      <c r="S50" s="65">
         <v>0.45</v>
       </c>
-      <c r="T50" s="73">
+      <c r="T50" s="65">
         <v>1.4328000000000001</v>
       </c>
-      <c r="U50" s="74">
+      <c r="U50" s="66">
         <f t="shared" si="12"/>
         <v>6.8199999999999816E-2</v>
       </c>
@@ -16797,34 +17308,34 @@
       </c>
       <c r="J51">
         <f t="shared" si="8"/>
-        <v>0.60400000000000009</v>
+        <v>0.64800000000000013</v>
       </c>
       <c r="K51">
         <f t="shared" si="9"/>
-        <v>112275.07558423461</v>
+        <v>50588.984962043032</v>
       </c>
       <c r="L51">
         <f t="shared" si="10"/>
-        <v>0.35335385003685549</v>
-      </c>
-      <c r="O51" s="72">
+        <v>0.78421874348012355</v>
+      </c>
+      <c r="O51" s="64">
         <v>0.5</v>
       </c>
-      <c r="P51" s="73">
+      <c r="P51" s="65">
         <v>1.3725000000000001</v>
       </c>
-      <c r="Q51" s="73">
+      <c r="Q51" s="65">
         <f t="shared" si="11"/>
         <v>6.030000000000002E-2</v>
       </c>
-      <c r="R51" s="73"/>
-      <c r="S51" s="73">
+      <c r="R51" s="65"/>
+      <c r="S51" s="65">
         <v>0.5</v>
       </c>
-      <c r="T51" s="73">
+      <c r="T51" s="65">
         <v>1.3725000000000001</v>
       </c>
-      <c r="U51" s="74">
+      <c r="U51" s="66">
         <f t="shared" si="12"/>
         <v>6.030000000000002E-2</v>
       </c>
@@ -16867,23 +17378,23 @@
       </c>
       <c r="J52">
         <f t="shared" si="8"/>
-        <v>0.59500000000000008</v>
+        <v>0.64000000000000012</v>
       </c>
       <c r="K52">
         <f t="shared" si="9"/>
-        <v>110602.10260367481</v>
+        <v>49964.42959214127</v>
       </c>
       <c r="L52">
         <f t="shared" si="10"/>
-        <v>0.36030003166273</v>
-      </c>
-      <c r="O52" s="72"/>
-      <c r="P52" s="73"/>
-      <c r="Q52" s="73"/>
-      <c r="R52" s="73"/>
-      <c r="S52" s="73"/>
-      <c r="T52" s="73"/>
-      <c r="U52" s="74"/>
+        <v>0.79756621651368564</v>
+      </c>
+      <c r="O52" s="64"/>
+      <c r="P52" s="65"/>
+      <c r="Q52" s="65"/>
+      <c r="R52" s="65"/>
+      <c r="S52" s="65"/>
+      <c r="T52" s="65"/>
+      <c r="U52" s="66"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -16923,25 +17434,25 @@
       </c>
       <c r="J53">
         <f t="shared" si="8"/>
-        <v>0.58600000000000008</v>
+        <v>0.63200000000000012</v>
       </c>
       <c r="K53">
         <f t="shared" si="9"/>
-        <v>108929.12962311502</v>
+        <v>49339.874222239501</v>
       </c>
       <c r="L53">
         <f t="shared" si="10"/>
-        <v>0.36716395407789959</v>
-      </c>
-      <c r="O53" s="72"/>
-      <c r="P53" s="73" t="s">
+        <v>0.81059894410228672</v>
+      </c>
+      <c r="O53" s="64"/>
+      <c r="P53" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="Q53" s="73"/>
-      <c r="R53" s="73"/>
-      <c r="S53" s="73"/>
-      <c r="T53" s="73"/>
-      <c r="U53" s="74"/>
+      <c r="Q53" s="65"/>
+      <c r="R53" s="65"/>
+      <c r="S53" s="65"/>
+      <c r="T53" s="65"/>
+      <c r="U53" s="66"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -16981,25 +17492,25 @@
       </c>
       <c r="J54">
         <f t="shared" si="8"/>
-        <v>0.57700000000000007</v>
+        <v>0.62400000000000011</v>
       </c>
       <c r="K54">
         <f t="shared" si="9"/>
-        <v>107256.15664255524</v>
+        <v>48715.318852337732</v>
       </c>
       <c r="L54">
         <f t="shared" si="10"/>
-        <v>0.37394176806453233</v>
-      </c>
-      <c r="O54" s="72"/>
-      <c r="P54" s="73" t="s">
+        <v>0.82330482065188981</v>
+      </c>
+      <c r="O54" s="64"/>
+      <c r="P54" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="Q54" s="73"/>
-      <c r="R54" s="73"/>
-      <c r="S54" s="73"/>
-      <c r="T54" s="73"/>
-      <c r="U54" s="74"/>
+      <c r="Q54" s="65"/>
+      <c r="R54" s="65"/>
+      <c r="S54" s="65"/>
+      <c r="T54" s="65"/>
+      <c r="U54" s="66"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -17039,23 +17550,23 @@
       </c>
       <c r="J55">
         <f t="shared" si="8"/>
-        <v>0.56800000000000006</v>
+        <v>0.6160000000000001</v>
       </c>
       <c r="K55">
         <f t="shared" si="9"/>
-        <v>105583.18366199546</v>
+        <v>48090.76348243597</v>
       </c>
       <c r="L55">
         <f t="shared" si="10"/>
-        <v>0.38062938044028566</v>
-      </c>
-      <c r="O55" s="72"/>
-      <c r="P55" s="73"/>
-      <c r="Q55" s="73"/>
-      <c r="R55" s="73"/>
-      <c r="S55" s="73"/>
-      <c r="T55" s="73"/>
-      <c r="U55" s="74"/>
+        <v>0.83567111170642927</v>
+      </c>
+      <c r="O55" s="64"/>
+      <c r="P55" s="65"/>
+      <c r="Q55" s="65"/>
+      <c r="R55" s="65"/>
+      <c r="S55" s="65"/>
+      <c r="T55" s="65"/>
+      <c r="U55" s="66"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -17095,23 +17606,23 @@
       </c>
       <c r="J56">
         <f t="shared" si="8"/>
-        <v>0.55900000000000005</v>
+        <v>0.6080000000000001</v>
       </c>
       <c r="K56">
         <f t="shared" si="9"/>
-        <v>103910.21068143567</v>
+        <v>47466.208112534201</v>
       </c>
       <c r="L56">
         <f t="shared" si="10"/>
-        <v>0.38722243441894549</v>
-      </c>
-      <c r="O56" s="72"/>
-      <c r="P56" s="73"/>
-      <c r="Q56" s="73"/>
-      <c r="R56" s="73"/>
-      <c r="S56" s="73"/>
-      <c r="T56" s="73"/>
-      <c r="U56" s="74"/>
+        <v>0.84768441257531135</v>
+      </c>
+      <c r="O56" s="64"/>
+      <c r="P56" s="65"/>
+      <c r="Q56" s="65"/>
+      <c r="R56" s="65"/>
+      <c r="S56" s="65"/>
+      <c r="T56" s="65"/>
+      <c r="U56" s="66"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -17151,23 +17662,23 @@
       </c>
       <c r="J57">
         <f t="shared" si="8"/>
-        <v>0.55000000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="K57">
         <f t="shared" si="9"/>
-        <v>102237.23770087586</v>
+        <v>46841.652742632432</v>
       </c>
       <c r="L57">
         <f t="shared" si="10"/>
-        <v>0.39371628804283632</v>
-      </c>
-      <c r="O57" s="72"/>
-      <c r="P57" s="73"/>
-      <c r="Q57" s="73"/>
-      <c r="R57" s="73"/>
-      <c r="S57" s="73"/>
-      <c r="T57" s="73"/>
-      <c r="U57" s="74"/>
+        <v>0.85933060365110925</v>
+      </c>
+      <c r="O57" s="64"/>
+      <c r="P57" s="65"/>
+      <c r="Q57" s="65"/>
+      <c r="R57" s="65"/>
+      <c r="S57" s="65"/>
+      <c r="T57" s="65"/>
+      <c r="U57" s="66"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -17207,23 +17718,23 @@
       </c>
       <c r="J58">
         <f t="shared" si="8"/>
-        <v>0.54100000000000004</v>
+        <v>0.59200000000000008</v>
       </c>
       <c r="K58">
         <f t="shared" si="9"/>
-        <v>100564.26472031607</v>
+        <v>46217.09737273067</v>
       </c>
       <c r="L58">
         <f t="shared" si="10"/>
-        <v>0.40010599046245948</v>
-      </c>
-      <c r="O58" s="72"/>
-      <c r="P58" s="73"/>
-      <c r="Q58" s="73"/>
-      <c r="R58" s="73"/>
-      <c r="S58" s="73"/>
-      <c r="T58" s="73"/>
-      <c r="U58" s="74"/>
+        <v>0.87059480210437379</v>
+      </c>
+      <c r="O58" s="64"/>
+      <c r="P58" s="65"/>
+      <c r="Q58" s="65"/>
+      <c r="R58" s="65"/>
+      <c r="S58" s="65"/>
+      <c r="T58" s="65"/>
+      <c r="U58" s="66"/>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -17263,23 +17774,23 @@
       </c>
       <c r="J59">
         <f t="shared" si="8"/>
-        <v>0.53200000000000003</v>
+        <v>0.58400000000000007</v>
       </c>
       <c r="K59">
         <f t="shared" si="9"/>
-        <v>98891.2917397563</v>
+        <v>45592.542002828908</v>
       </c>
       <c r="L59">
         <f t="shared" si="10"/>
-        <v>0.4063862558084253</v>
-      </c>
-      <c r="O59" s="72"/>
-      <c r="P59" s="73"/>
-      <c r="Q59" s="73"/>
-      <c r="R59" s="73"/>
-      <c r="S59" s="73"/>
-      <c r="T59" s="73"/>
-      <c r="U59" s="74"/>
+        <v>0.8814613096081515</v>
+      </c>
+      <c r="O59" s="64"/>
+      <c r="P59" s="65"/>
+      <c r="Q59" s="65"/>
+      <c r="R59" s="65"/>
+      <c r="S59" s="65"/>
+      <c r="T59" s="65"/>
+      <c r="U59" s="66"/>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -17319,23 +17830,23 @@
       </c>
       <c r="J60">
         <f t="shared" si="8"/>
-        <v>0.52300000000000002</v>
+        <v>0.57600000000000007</v>
       </c>
       <c r="K60">
         <f t="shared" si="9"/>
-        <v>97218.318759196511</v>
+        <v>44967.986632927139</v>
       </c>
       <c r="L60">
         <f t="shared" si="10"/>
-        <v>0.41255143436565045</v>
-      </c>
-      <c r="O60" s="72"/>
-      <c r="P60" s="73"/>
-      <c r="Q60" s="73"/>
-      <c r="R60" s="73"/>
-      <c r="S60" s="73"/>
-      <c r="T60" s="73"/>
-      <c r="U60" s="74"/>
+        <v>0.891913555706214</v>
+      </c>
+      <c r="O60" s="64"/>
+      <c r="P60" s="65"/>
+      <c r="Q60" s="65"/>
+      <c r="R60" s="65"/>
+      <c r="S60" s="65"/>
+      <c r="T60" s="65"/>
+      <c r="U60" s="66"/>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -17375,23 +17886,23 @@
       </c>
       <c r="J61">
         <f t="shared" si="8"/>
-        <v>0.51400000000000001</v>
+        <v>0.56800000000000006</v>
       </c>
       <c r="K61">
         <f t="shared" si="9"/>
-        <v>95545.345778636722</v>
+        <v>44343.43126302537</v>
       </c>
       <c r="L61">
         <f t="shared" si="10"/>
-        <v>0.41859548071916186</v>
-      </c>
-      <c r="O61" s="72"/>
-      <c r="P61" s="73"/>
-      <c r="Q61" s="73"/>
-      <c r="R61" s="73"/>
-      <c r="S61" s="73"/>
-      <c r="T61" s="73"/>
-      <c r="U61" s="74"/>
+        <v>0.9019340363955024</v>
+      </c>
+      <c r="O61" s="64"/>
+      <c r="P61" s="65"/>
+      <c r="Q61" s="65"/>
+      <c r="R61" s="65"/>
+      <c r="S61" s="65"/>
+      <c r="T61" s="65"/>
+      <c r="U61" s="66"/>
     </row>
     <row r="62" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -17431,23 +17942,23 @@
       </c>
       <c r="J62">
         <f t="shared" si="8"/>
-        <v>0.505</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K62">
         <f t="shared" si="9"/>
-        <v>93872.372798076933</v>
+        <v>43718.875893123608</v>
       </c>
       <c r="L62">
         <f t="shared" si="10"/>
-        <v>0.42451191849371173</v>
-      </c>
-      <c r="O62" s="75"/>
-      <c r="P62" s="76"/>
-      <c r="Q62" s="76"/>
-      <c r="R62" s="76"/>
-      <c r="S62" s="76"/>
-      <c r="T62" s="76"/>
-      <c r="U62" s="77"/>
+        <v>0.91150424744421243</v>
+      </c>
+      <c r="O62" s="67"/>
+      <c r="P62" s="68"/>
+      <c r="Q62" s="68"/>
+      <c r="R62" s="68"/>
+      <c r="S62" s="68"/>
+      <c r="T62" s="68"/>
+      <c r="U62" s="69"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -17487,15 +17998,15 @@
       </c>
       <c r="J63">
         <f t="shared" si="8"/>
-        <v>0.496</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="K63">
         <f t="shared" si="9"/>
-        <v>92199.399817517144</v>
+        <v>43094.320523221839</v>
       </c>
       <c r="L63">
         <f t="shared" si="10"/>
-        <v>0.43029380125455796</v>
+        <v>0.92060461191144938</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -17536,15 +18047,15 @@
       </c>
       <c r="J64">
         <f t="shared" si="8"/>
-        <v>0.48699999999999999</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="K64">
         <f t="shared" si="9"/>
-        <v>90526.426836957355</v>
+        <v>42469.76515332007</v>
       </c>
       <c r="L64">
         <f t="shared" si="10"/>
-        <v>0.43593366907280945</v>
+        <v>0.92921440127155985</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -17585,15 +18096,15 @@
       </c>
       <c r="J65">
         <f t="shared" si="8"/>
-        <v>0.47799999999999998</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="K65">
         <f t="shared" si="9"/>
-        <v>88853.453856397566</v>
+        <v>41845.209783418308</v>
       </c>
       <c r="L65">
         <f t="shared" si="10"/>
-        <v>0.44142350018392651</v>
+        <v>0.93731164947497114</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -17634,15 +18145,15 @@
       </c>
       <c r="J66">
         <f t="shared" si="8"/>
-        <v>0.46900000000000008</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="K66">
         <f t="shared" si="9"/>
-        <v>87180.480875837791</v>
+        <v>41220.654413516539</v>
       </c>
       <c r="L66">
         <f t="shared" si="10"/>
-        <v>0.4467546570802487</v>
+        <v>0.94487305919637898</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -17683,15 +18194,15 @@
       </c>
       <c r="J67">
         <f t="shared" si="8"/>
-        <v>0.46000000000000008</v>
+        <v>0.52</v>
       </c>
       <c r="K67">
         <f t="shared" si="9"/>
-        <v>85507.507895278017</v>
+        <v>40596.099043614769</v>
       </c>
       <c r="L67">
         <f t="shared" si="10"/>
-        <v>0.45191782627525551</v>
+        <v>0.9518738994289212</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -17732,15 +18243,15 @@
       </c>
       <c r="J68">
         <f t="shared" si="8"/>
-        <v>0.45100000000000007</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="K68">
         <f t="shared" si="9"/>
-        <v>83834.534914718228</v>
+        <v>39971.543673713008</v>
       </c>
       <c r="L68">
         <f t="shared" si="10"/>
-        <v>0.45690295085556465</v>
+        <v>0.95828789347780752</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -17781,15 +18292,15 @@
       </c>
       <c r="J69">
         <f t="shared" si="8"/>
-        <v>0.44200000000000006</v>
+        <v>0.504</v>
       </c>
       <c r="K69">
         <f t="shared" si="9"/>
-        <v>82161.561934158424</v>
+        <v>39346.988303811238</v>
       </c>
       <c r="L69">
         <f t="shared" si="10"/>
-        <v>0.46169915479267631</v>
+        <v>0.96408709628667322</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -17830,15 +18341,15 @@
       </c>
       <c r="J70">
         <f t="shared" si="8"/>
-        <v>0.43300000000000005</v>
+        <v>0.496</v>
       </c>
       <c r="K70">
         <f t="shared" si="9"/>
-        <v>80488.588953598635</v>
+        <v>38722.432933909477</v>
       </c>
       <c r="L70">
         <f t="shared" si="10"/>
-        <v>0.46629465781553647</v>
+        <v>0.96924175989229144</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -17879,15 +18390,15 @@
       </c>
       <c r="J71">
         <f t="shared" si="8"/>
-        <v>0.42400000000000004</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="K71">
         <f t="shared" si="9"/>
-        <v>78815.615973038861</v>
+        <v>38097.877564007707</v>
       </c>
       <c r="L71">
         <f t="shared" si="10"/>
-        <v>0.47067667944139824</v>
+        <v>0.9737201856453227</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -17928,15 +18439,15 @@
       </c>
       <c r="J72">
         <f t="shared" ref="J72:J107" si="21">(100-A72) * 0.01 * (1 - $B$4) + $B$4</f>
-        <v>0.41500000000000004</v>
+        <v>0.48000000000000004</v>
       </c>
       <c r="K72">
         <f t="shared" ref="K72:K107" si="22">J72 * $F$2 * $K$4</f>
-        <v>77142.642992479072</v>
+        <v>37473.322194105946</v>
       </c>
       <c r="L72">
         <f t="shared" ref="L72:L107" si="23">IFERROR(H72/K72,1)</f>
-        <v>0.47483133051913146</v>
+        <v>0.97748856165313691</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -17977,15 +18488,15 @@
       </c>
       <c r="J73">
         <f t="shared" si="21"/>
-        <v>0.40600000000000003</v>
+        <v>0.47200000000000003</v>
       </c>
       <c r="K73">
         <f t="shared" si="22"/>
-        <v>75469.670011919283</v>
+        <v>36848.766824204176</v>
       </c>
       <c r="L73">
         <f t="shared" si="23"/>
-        <v>0.4787434903472596</v>
+        <v>0.98051078369140132</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -18026,15 +18537,15 @@
       </c>
       <c r="J74">
         <f t="shared" si="21"/>
-        <v>0.39700000000000002</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K74">
         <f t="shared" si="22"/>
-        <v>73796.697031359494</v>
+        <v>36224.211454302414</v>
       </c>
       <c r="L74">
         <f t="shared" si="23"/>
-        <v>0.48239666707757284</v>
+        <v>0.9827482575892772</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -18075,15 +18586,15 @@
       </c>
       <c r="J75">
         <f t="shared" si="21"/>
-        <v>0.38800000000000001</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="K75">
         <f t="shared" si="22"/>
-        <v>72123.724050799705</v>
+        <v>35599.656084400653</v>
       </c>
       <c r="L75">
         <f t="shared" si="23"/>
-        <v>0.4857728386903778</v>
+        <v>0.98415968081305982</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -18124,15 +18635,15 @@
       </c>
       <c r="J76">
         <f t="shared" si="21"/>
-        <v>0.379</v>
+        <v>0.44800000000000001</v>
       </c>
       <c r="K76">
         <f t="shared" si="22"/>
-        <v>70450.751070239916</v>
+        <v>34975.100714498883</v>
       </c>
       <c r="L76">
         <f t="shared" si="23"/>
-        <v>0.48885227131186781</v>
+        <v>0.98470080064806564</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -18173,15 +18684,15 @@
       </c>
       <c r="J77">
         <f t="shared" si="21"/>
-        <v>0.37</v>
+        <v>0.44</v>
       </c>
       <c r="K77">
         <f t="shared" si="22"/>
-        <v>68777.778089680127</v>
+        <v>34350.545344597114</v>
       </c>
       <c r="L77">
         <f t="shared" si="23"/>
-        <v>0.49161331101564981</v>
+        <v>0.98432414600036189</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -18222,15 +18733,15 @@
       </c>
       <c r="J78">
         <f t="shared" si="21"/>
-        <v>0.36099999999999999</v>
+        <v>0.432</v>
       </c>
       <c r="K78">
         <f t="shared" si="22"/>
-        <v>67104.805109120338</v>
+        <v>33725.989974695352</v>
       </c>
       <c r="L78">
         <f t="shared" si="23"/>
-        <v>0.49403214448100846</v>
+        <v>0.9829787293986858</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -18271,15 +18782,15 @@
       </c>
       <c r="J79">
         <f t="shared" si="21"/>
-        <v>0.35200000000000009</v>
+        <v>0.42400000000000004</v>
       </c>
       <c r="K79">
         <f t="shared" si="22"/>
-        <v>65431.832128560571</v>
+        <v>33101.434604793591</v>
       </c>
       <c r="L79">
         <f t="shared" si="23"/>
-        <v>0.49608252293397359</v>
+        <v>0.98060971526073737</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -18320,15 +18831,15 @@
       </c>
       <c r="J80">
         <f t="shared" si="21"/>
-        <v>0.34300000000000003</v>
+        <v>0.41600000000000004</v>
       </c>
       <c r="K80">
         <f t="shared" si="22"/>
-        <v>63758.859148000767</v>
+        <v>32476.879234891821</v>
       </c>
       <c r="L80">
         <f t="shared" si="23"/>
-        <v>0.49773544262721481</v>
+        <v>0.97715804988250177</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -18369,15 +18880,15 @@
       </c>
       <c r="J81">
         <f t="shared" si="21"/>
-        <v>0.33400000000000002</v>
+        <v>0.40800000000000003</v>
       </c>
       <c r="K81">
         <f t="shared" si="22"/>
-        <v>62085.886167440985</v>
+        <v>31852.323864990056</v>
       </c>
       <c r="L81">
         <f t="shared" si="23"/>
-        <v>0.49895877366099323</v>
+        <v>0.97256004789690242</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -18418,15 +18929,15 @@
       </c>
       <c r="J82">
         <f t="shared" si="21"/>
-        <v>0.32500000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="K82">
         <f t="shared" si="22"/>
-        <v>60412.913186881189</v>
+        <v>31227.76849508829</v>
       </c>
       <c r="L82">
         <f t="shared" si="23"/>
-        <v>0.49971682713129228</v>
+        <v>0.96674692910749793</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -18467,15 +18978,15 @@
       </c>
       <c r="J83">
         <f t="shared" si="21"/>
-        <v>0.316</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="K83">
         <f t="shared" si="22"/>
-        <v>58739.940206321407</v>
+        <v>30603.213125186521</v>
       </c>
       <c r="L83">
         <f t="shared" si="23"/>
-        <v>0.49996984830958663</v>
+        <v>0.95964429860793277</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -18516,15 +19027,15 @@
       </c>
       <c r="J84">
         <f t="shared" si="21"/>
-        <v>0.30700000000000005</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="K84">
         <f t="shared" si="22"/>
-        <v>57066.967225761626</v>
+        <v>29978.657755284756</v>
       </c>
       <c r="L84">
         <f t="shared" si="23"/>
-        <v>0.49967342067508097</v>
+        <v>0.95117156191632157</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -18565,15 +19076,15 @@
       </c>
       <c r="J85">
         <f t="shared" si="21"/>
-        <v>0.29800000000000004</v>
+        <v>0.376</v>
       </c>
       <c r="K85">
         <f t="shared" si="22"/>
-        <v>55393.994245201844</v>
+        <v>29354.102385382987</v>
       </c>
       <c r="L85">
         <f t="shared" si="23"/>
-        <v>0.49877776195279039</v>
+        <v>0.94124126544593856</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -18614,15 +19125,15 @@
       </c>
       <c r="J86">
         <f t="shared" si="21"/>
-        <v>0.28900000000000003</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="K86">
         <f t="shared" si="22"/>
-        <v>53721.021264642048</v>
+        <v>28729.547015481221</v>
       </c>
       <c r="L86">
         <f t="shared" si="23"/>
-        <v>0.49722688861548242</v>
+        <v>0.92975835095034176</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -18663,15 +19174,15 @@
       </c>
       <c r="J87">
         <f t="shared" si="21"/>
-        <v>0.28000000000000003</v>
+        <v>0.36000000000000004</v>
       </c>
       <c r="K87">
         <f t="shared" si="22"/>
-        <v>52048.048284082266</v>
+        <v>28104.991645579463</v>
       </c>
       <c r="L87">
         <f t="shared" si="23"/>
-        <v>0.49495761925385129</v>
+        <v>0.91661931056118318</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -18712,15 +19223,15 @@
       </c>
       <c r="J88">
         <f t="shared" si="21"/>
-        <v>0.27100000000000002</v>
+        <v>0.35200000000000004</v>
       </c>
       <c r="K88">
         <f t="shared" si="22"/>
-        <v>50375.07530352247</v>
+        <v>27480.436275677694</v>
       </c>
       <c r="L88">
         <f t="shared" si="23"/>
-        <v>0.49189837935624914</v>
+        <v>0.90171122660390257</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -18761,15 +19272,15 @@
       </c>
       <c r="J89">
         <f t="shared" si="21"/>
-        <v>0.26200000000000001</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="K89">
         <f t="shared" si="22"/>
-        <v>48702.102322962688</v>
+        <v>26855.880905775924</v>
       </c>
       <c r="L89">
         <f t="shared" si="23"/>
-        <v>0.4879677597453046</v>
+        <v>0.88491067743421226</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -18810,15 +19321,15 @@
       </c>
       <c r="J90">
         <f t="shared" si="21"/>
-        <v>0.253</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="K90">
         <f t="shared" si="22"/>
-        <v>47029.129342402899</v>
+        <v>26231.325535874163</v>
       </c>
       <c r="L90">
         <f t="shared" si="23"/>
-        <v>0.48307276732908011</v>
+        <v>0.86608248696551104</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -18859,15 +19370,15 @@
       </c>
       <c r="J91">
         <f t="shared" si="21"/>
-        <v>0.24400000000000002</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="K91">
         <f t="shared" si="22"/>
-        <v>45356.15636184311</v>
+        <v>25606.770165972397</v>
       </c>
       <c r="L91">
         <f t="shared" si="23"/>
-        <v>0.47710668872338463</v>
+        <v>0.84507829120031042</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -18908,15 +19419,15 @@
       </c>
       <c r="J92">
         <f t="shared" si="21"/>
-        <v>0.23500000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="K92">
         <f t="shared" si="22"/>
-        <v>43683.183381283328</v>
+        <v>24982.214796070632</v>
       </c>
       <c r="L92">
         <f t="shared" si="23"/>
-        <v>0.46994646296176845</v>
+        <v>0.82173488974137321</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -18957,15 +19468,15 @@
       </c>
       <c r="J93">
         <f t="shared" si="21"/>
-        <v>0.22600000000000003</v>
+        <v>0.31200000000000006</v>
       </c>
       <c r="K93">
         <f t="shared" si="22"/>
-        <v>42010.210400723547</v>
+        <v>24357.659426168866</v>
       </c>
       <c r="L93">
         <f t="shared" si="23"/>
-        <v>0.46144942644595788</v>
+        <v>0.79587234368918136</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -19006,15 +19517,15 @@
       </c>
       <c r="J94">
         <f t="shared" si="21"/>
-        <v>0.21700000000000003</v>
+        <v>0.30400000000000005</v>
       </c>
       <c r="K94">
         <f t="shared" si="22"/>
-        <v>40337.23742016375</v>
+        <v>23733.104056267101</v>
       </c>
       <c r="L94">
         <f t="shared" si="23"/>
-        <v>0.45144924788395635</v>
+        <v>0.7672917732074247</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -19055,15 +19566,15 @@
       </c>
       <c r="J95">
         <f t="shared" si="21"/>
-        <v>0.20800000000000002</v>
+        <v>0.29600000000000004</v>
       </c>
       <c r="K95">
         <f t="shared" si="22"/>
-        <v>38664.264439603969</v>
+        <v>23108.548686365335</v>
       </c>
       <c r="L95">
         <f t="shared" si="23"/>
-        <v>0.43975080787553716</v>
+        <v>0.73577279793694983</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -19104,15 +19615,15 @@
       </c>
       <c r="J96">
         <f t="shared" si="21"/>
-        <v>0.19900000000000001</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="K96">
         <f t="shared" si="22"/>
-        <v>36991.29145904418</v>
+        <v>22483.993316463569</v>
       </c>
       <c r="L96">
         <f t="shared" si="23"/>
-        <v>0.42612368903852299</v>
+        <v>0.70107055081202985</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -19153,15 +19664,15 @@
       </c>
       <c r="J97">
         <f t="shared" si="21"/>
-        <v>0.19</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K97">
         <f t="shared" si="22"/>
-        <v>35318.318478484391</v>
+        <v>21859.437946561804</v>
       </c>
       <c r="L97">
         <f t="shared" si="23"/>
-        <v>0.41029381596042941</v>
+        <v>0.66291217995942708</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -19202,15 +19713,15 @@
       </c>
       <c r="J98">
         <f t="shared" si="21"/>
-        <v>0.18099999999999999</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="K98">
         <f t="shared" si="22"/>
-        <v>33645.345497924602</v>
+        <v>21234.882576660035</v>
       </c>
       <c r="L98">
         <f t="shared" si="23"/>
-        <v>0.39193260099203459</v>
+        <v>0.62099273328552229</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -19251,15 +19762,15 @@
       </c>
       <c r="J99">
         <f t="shared" si="21"/>
-        <v>0.17200000000000001</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="K99">
         <f t="shared" si="22"/>
-        <v>31972.372517364816</v>
+        <v>20610.327206758269</v>
       </c>
       <c r="L99">
         <f t="shared" si="23"/>
-        <v>0.3706426823249771</v>
+        <v>0.57497029480656048</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -19300,15 +19811,15 @@
       </c>
       <c r="J100">
         <f t="shared" si="21"/>
-        <v>0.16300000000000003</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="K100">
         <f t="shared" si="22"/>
-        <v>30299.399536805035</v>
+        <v>19985.771836856504</v>
       </c>
       <c r="L100">
         <f t="shared" si="23"/>
-        <v>0.34593893726070557</v>
+        <v>0.52446020904081769</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -19349,15 +19860,15 @@
       </c>
       <c r="J101">
         <f t="shared" si="21"/>
-        <v>0.154</v>
+        <v>0.248</v>
       </c>
       <c r="K101">
         <f t="shared" si="22"/>
-        <v>28626.426556245242</v>
+        <v>19361.216466954738</v>
       </c>
       <c r="L101">
         <f t="shared" si="23"/>
-        <v>0.31722283779451393</v>
+        <v>0.46902818754118625</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -19398,15 +19909,15 @@
       </c>
       <c r="J102">
         <f t="shared" si="21"/>
-        <v>0.14500000000000002</v>
+        <v>0.24000000000000002</v>
       </c>
       <c r="K102">
         <f t="shared" si="22"/>
-        <v>26953.453575685457</v>
+        <v>18736.661097052973</v>
       </c>
       <c r="L102">
         <f t="shared" si="23"/>
-        <v>0.28374725586535449</v>
+        <v>0.408182036734277</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -19447,15 +19958,15 @@
       </c>
       <c r="J103">
         <f t="shared" si="21"/>
-        <v>0.13600000000000001</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="K103">
         <f t="shared" si="22"/>
-        <v>25280.480595125671</v>
+        <v>18112.105727151207</v>
       </c>
       <c r="L103">
         <f t="shared" si="23"/>
-        <v>0.24456729421955006</v>
+        <v>0.34136167427795788</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -19496,15 +20007,15 @@
       </c>
       <c r="J104">
         <f t="shared" si="21"/>
-        <v>0.127</v>
+        <v>0.224</v>
       </c>
       <c r="K104">
         <f t="shared" si="22"/>
-        <v>23607.507614565882</v>
+        <v>17487.550357249442</v>
       </c>
       <c r="L104">
         <f t="shared" si="23"/>
-        <v>0.19847021071261714</v>
+        <v>0.26792700606693509</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
@@ -19545,15 +20056,15 @@
       </c>
       <c r="J105">
         <f t="shared" si="21"/>
-        <v>0.11800000000000001</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="K105">
         <f t="shared" si="22"/>
-        <v>21934.534634006093</v>
+        <v>16862.994987347676</v>
       </c>
       <c r="L105">
         <f t="shared" si="23"/>
-        <v>0.14387327407124664</v>
+        <v>0.18714310923957489</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -19594,15 +20105,15 @@
       </c>
       <c r="J106">
         <f t="shared" si="21"/>
-        <v>0.10900000000000001</v>
+        <v>0.20800000000000002</v>
       </c>
       <c r="K106">
         <f t="shared" si="22"/>
-        <v>20261.561653446312</v>
+        <v>16238.439617445911</v>
       </c>
       <c r="L106">
         <f t="shared" si="23"/>
-        <v>7.8671016087825452E-2</v>
+        <v>9.816199587860748E-2</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -19643,11 +20154,11 @@
       </c>
       <c r="J107">
         <f t="shared" si="21"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K107">
         <f t="shared" si="22"/>
-        <v>18588.588672886523</v>
+        <v>15613.884247544145</v>
       </c>
       <c r="L107">
         <f t="shared" si="23"/>
@@ -19665,12 +20176,621 @@
       </c>
       <c r="K108">
         <f>LARGE(K7:K107,1)</f>
-        <v>185885.88672886521</v>
+        <v>78069.421237720715</v>
       </c>
       <c r="L108">
         <f>LARGE(L7:L107,1)</f>
-        <v>0.49996984830958663</v>
-      </c>
+        <v>0.98470080064806564</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="58">
+        <v>0</v>
+      </c>
+      <c r="B5" s="58">
+        <v>3.2</v>
+      </c>
+      <c r="C5" s="58">
+        <f>B5-B6</f>
+        <v>-0.5585</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58">
+        <v>0</v>
+      </c>
+      <c r="F5" s="58">
+        <v>4</v>
+      </c>
+      <c r="G5" s="58">
+        <f>F5-F6</f>
+        <v>0.24149999999999983</v>
+      </c>
+      <c r="H5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1E-3</v>
+      </c>
+      <c r="B6">
+        <v>3.7585000000000002</v>
+      </c>
+      <c r="C6" s="70">
+        <f t="shared" ref="C6:C16" si="0">B6-B7</f>
+        <v>1.0870000000000002</v>
+      </c>
+      <c r="E6">
+        <v>1E-3</v>
+      </c>
+      <c r="F6">
+        <v>3.7585000000000002</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G16" si="1">F6-F7</f>
+        <v>1.0870000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.05</v>
+      </c>
+      <c r="B7">
+        <v>2.6715</v>
+      </c>
+      <c r="C7" s="70">
+        <f t="shared" si="0"/>
+        <v>0.36249999999999982</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="F7">
+        <v>2.6715</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.36249999999999982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.1</v>
+      </c>
+      <c r="B8">
+        <v>2.3090000000000002</v>
+      </c>
+      <c r="C8" s="70">
+        <f t="shared" si="0"/>
+        <v>0.23060000000000036</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>2.3090000000000002</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.23060000000000036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.15</v>
+      </c>
+      <c r="B9">
+        <v>2.0783999999999998</v>
+      </c>
+      <c r="C9" s="70">
+        <f t="shared" si="0"/>
+        <v>0.16859999999999986</v>
+      </c>
+      <c r="E9">
+        <v>0.15</v>
+      </c>
+      <c r="F9">
+        <v>2.0783999999999998</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.16859999999999986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.2</v>
+      </c>
+      <c r="B10">
+        <v>1.9097999999999999</v>
+      </c>
+      <c r="C10" s="70">
+        <f t="shared" si="0"/>
+        <v>0.13219999999999987</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="F10">
+        <v>1.9097999999999999</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.13219999999999987</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.25</v>
+      </c>
+      <c r="B11">
+        <v>1.7776000000000001</v>
+      </c>
+      <c r="C11" s="70">
+        <f t="shared" si="0"/>
+        <v>0.10790000000000011</v>
+      </c>
+      <c r="E11">
+        <v>0.25</v>
+      </c>
+      <c r="F11">
+        <v>1.7776000000000001</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.10790000000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.3</v>
+      </c>
+      <c r="B12">
+        <v>1.6697</v>
+      </c>
+      <c r="C12" s="70">
+        <f t="shared" si="0"/>
+        <v>9.0700000000000003E-2</v>
+      </c>
+      <c r="E12">
+        <v>0.3</v>
+      </c>
+      <c r="F12">
+        <v>1.6697</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>9.0700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.35</v>
+      </c>
+      <c r="B13">
+        <v>1.579</v>
+      </c>
+      <c r="C13" s="70">
+        <f t="shared" si="0"/>
+        <v>7.8000000000000069E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.35</v>
+      </c>
+      <c r="F13">
+        <v>1.579</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>7.8000000000000069E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.4</v>
+      </c>
+      <c r="B14">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="C14" s="70">
+        <f t="shared" si="0"/>
+        <v>6.8199999999999816E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.4</v>
+      </c>
+      <c r="F14">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>6.8199999999999816E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.45</v>
+      </c>
+      <c r="B15">
+        <v>1.4328000000000001</v>
+      </c>
+      <c r="C15" s="70">
+        <f t="shared" si="0"/>
+        <v>6.030000000000002E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.45</v>
+      </c>
+      <c r="F15">
+        <v>1.4328000000000001</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>6.030000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.5</v>
+      </c>
+      <c r="B16">
+        <v>1.3725000000000001</v>
+      </c>
+      <c r="C16" s="70">
+        <f t="shared" si="0"/>
+        <v>1.3725000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+      <c r="F16">
+        <v>1.3725000000000001</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1.3725000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21">
+        <v>5.9282411169999998</v>
+      </c>
+      <c r="D21">
+        <v>3.7585000000000002</v>
+      </c>
+      <c r="E21">
+        <v>1E-3</v>
+      </c>
+      <c r="F21" s="59">
+        <v>3.7585000000000002</v>
+      </c>
+      <c r="G21" s="59"/>
+      <c r="H21" t="str">
+        <f>"{"&amp;E21&amp;","&amp;F21&amp;"}"</f>
+        <v>{0.001,3.7585}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22">
+        <v>-5.9043785340000001</v>
+      </c>
+      <c r="D22">
+        <v>2.6715</v>
+      </c>
+      <c r="E22">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="59">
+        <v>2.6715</v>
+      </c>
+      <c r="G22" s="59"/>
+      <c r="H22" t="str">
+        <f t="shared" ref="H22:H31" si="2">"{"&amp;E22&amp;","&amp;F22&amp;"}"</f>
+        <v>{0.05,2.6715}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23">
+        <v>2.883240196</v>
+      </c>
+      <c r="D23">
+        <v>2.3090000000000002</v>
+      </c>
+      <c r="E23">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="59">
+        <v>2.3090000000000002</v>
+      </c>
+      <c r="G23" s="59"/>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.1,2.309}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>2.0783999999999998</v>
+      </c>
+      <c r="E24">
+        <v>0.15</v>
+      </c>
+      <c r="F24" s="59">
+        <v>2.0783999999999998</v>
+      </c>
+      <c r="G24" s="59"/>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.15,2.0784}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25">
+        <v>1.9097999999999999</v>
+      </c>
+      <c r="E25">
+        <v>0.2</v>
+      </c>
+      <c r="F25" s="59">
+        <v>1.9097999999999999</v>
+      </c>
+      <c r="G25" s="59"/>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.2,1.9098}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26">
+        <v>5.9281800000000002</v>
+      </c>
+      <c r="D26">
+        <v>1.7776000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0.25</v>
+      </c>
+      <c r="F26" s="59">
+        <v>1.7776000000000001</v>
+      </c>
+      <c r="G26" s="59"/>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.25,1.7776}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27">
+        <v>-5.9043400000000004</v>
+      </c>
+      <c r="D27">
+        <v>1.6697</v>
+      </c>
+      <c r="E27">
+        <v>0.3</v>
+      </c>
+      <c r="F27" s="59">
+        <v>1.6697</v>
+      </c>
+      <c r="G27" s="59"/>
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.3,1.6697}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28">
+        <v>2.8832399999999998</v>
+      </c>
+      <c r="D28">
+        <v>1.579</v>
+      </c>
+      <c r="E28">
+        <v>0.35</v>
+      </c>
+      <c r="F28" s="59">
+        <v>1.579</v>
+      </c>
+      <c r="G28" s="59"/>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.35,1.579}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="E29">
+        <v>0.4</v>
+      </c>
+      <c r="F29" s="59">
+        <v>1.5009999999999999</v>
+      </c>
+      <c r="G29" s="59"/>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.4,1.501}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>1.4328000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.45</v>
+      </c>
+      <c r="F30" s="59">
+        <v>1.4328000000000001</v>
+      </c>
+      <c r="G30" s="59"/>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.45,1.4328}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>1.3725000000000001</v>
+      </c>
+      <c r="E31">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="59">
+        <v>1.3725000000000001</v>
+      </c>
+      <c r="G31" s="59"/>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>{0.5,1.3725}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F32" s="71"/>
+      <c r="G32" s="72"/>
+      <c r="H32" t="str">
+        <f>H21&amp;","&amp;H22&amp;","&amp;H23&amp;","&amp;H24&amp;","&amp;H25&amp;","&amp;H26&amp;","&amp;H27&amp;","&amp;H28&amp;","&amp;H29&amp;","&amp;H30&amp;","&amp;H31</f>
+        <v>{0.001,3.7585},{0.05,2.6715},{0.1,2.309},{0.15,2.0784},{0.2,1.9098},{0.25,1.7776},{0.3,1.6697},{0.35,1.579},{0.4,1.501},{0.45,1.4328},{0.5,1.3725}</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>0.6</v>
+      </c>
+      <c r="F33" s="71"/>
+      <c r="G33" s="72"/>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>0.65</v>
+      </c>
+      <c r="F34" s="71"/>
+      <c r="G34" s="72"/>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>0.7</v>
+      </c>
+      <c r="F35" s="71"/>
+      <c r="G35" s="72"/>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>0.75</v>
+      </c>
+      <c r="F36" s="71"/>
+      <c r="G36" s="72"/>
+      <c r="H36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>0.8</v>
+      </c>
+      <c r="F37" s="71"/>
+      <c r="G37" s="72"/>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>0.85</v>
+      </c>
+      <c r="F38" s="71"/>
+      <c r="G38" s="72"/>
+    </row>
+    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>0.9</v>
+      </c>
+      <c r="F39" s="71"/>
+      <c r="G39" s="72"/>
+    </row>
+    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>0.95</v>
+      </c>
+      <c r="F40" s="71"/>
+      <c r="G40" s="72"/>
+    </row>
+    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="71"/>
+      <c r="G41" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more work on motor graph
</commit_message>
<xml_diff>
--- a/Resources/PartBalance.xlsx
+++ b/Resources/PartBalance.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BaseStats" sheetId="1" r:id="rId1"/>
@@ -45,12 +45,12 @@
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
   <si>
     <t>Repulsor</t>
   </si>
@@ -343,10 +343,13 @@
     <t>mgc from solver</t>
   </si>
   <si>
-    <t>{{0.001,3.7585},{0.05,2.6715},{0.1,2.309},{0.15,2.0784},{0.2,1.9098},{0.25,1.7776},{0.3,1.6697},{0.35,1.579},{0.4,1.501},{0.45,1.4328},{0.5,1.3725}}</t>
+    <t>mgc from wolfram</t>
   </si>
   <si>
-    <t>mgc from wolfram</t>
+    <t>pf 0 ratings -- why the F are they different?  When all other points use the same values?</t>
+  </si>
+  <si>
+    <t>eff</t>
   </si>
 </sst>
 </file>
@@ -2803,11 +2806,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152999808"/>
-        <c:axId val="153001344"/>
+        <c:axId val="242917816"/>
+        <c:axId val="242918208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152999808"/>
+        <c:axId val="242917816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2864,12 +2867,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153001344"/>
+        <c:crossAx val="242918208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153001344"/>
+        <c:axId val="242918208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2926,7 +2929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152999808"/>
+        <c:crossAx val="242917816"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4614,304 +4617,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0582353974546733E-2</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1080194711126207E-2</c:v>
+                  <c:v>2.0000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.1491444015362169E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1813954992237869E-2</c:v>
+                  <c:v>4.0000000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10204550918356921</c:v>
+                  <c:v>4.9999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12218381356114935</c:v>
+                  <c:v>6.0000000000000012E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14222649736700138</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16217110879159394</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1820151114802393</c:v>
+                  <c:v>9.0000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20175588085721691</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22139070025643051</c:v>
+                  <c:v>0.11000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24091675684661182</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26033113733823338</c:v>
+                  <c:v>0.13000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27963082345836099</c:v>
+                  <c:v>0.14000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2988126871786812</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.31787348568085072</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.33680985604214309</c:v>
+                  <c:v>0.16999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.35561830962309454</c:v>
+                  <c:v>0.18000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.37429522613746891</c:v>
+                  <c:v>0.18999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.39283684738336427</c:v>
+                  <c:v>0.19999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.41123927061265109</c:v>
+                  <c:v>0.21000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.42949844151416616</c:v>
+                  <c:v>0.22000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.4476101467841514</c:v>
+                  <c:v>0.23000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.46557000625533373</c:v>
+                  <c:v>0.24000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.48337346455374897</c:v>
+                  <c:v>0.25000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.50101578224991949</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.51849202646826642</c:v>
+                  <c:v>0.27000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.53579706091566071</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.55292553528676069</c:v>
+                  <c:v>0.29000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.56987187400020933</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.58663026421586906</c:v>
+                  <c:v>0.30999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.60319464307897219</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.61955868413237059</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.63571578283288666</c:v>
+                  <c:v>0.33999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.65165904110209139</c:v>
+                  <c:v>0.35000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.66738125083555822</c:v>
+                  <c:v>0.36000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.68287487628775101</c:v>
+                  <c:v>0.37000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.69813203524207368</c:v>
+                  <c:v>0.38000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.71314447886720567</c:v>
+                  <c:v>0.39000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.72790357015152796</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.74240026079715471</c:v>
+                  <c:v>0.40999999999999992</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.75662506644365157</c:v>
+                  <c:v>0.4200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.77056804007885449</c:v>
+                  <c:v>0.4300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.78421874348012355</c:v>
+                  <c:v>0.44000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.79756621651368564</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.81059894410228672</c:v>
+                  <c:v>0.45999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.82330482065188981</c:v>
+                  <c:v>0.47000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.83567111170642927</c:v>
+                  <c:v>0.48000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.84768441257531135</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.85933060365110925</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.87059480210437379</c:v>
+                  <c:v>0.51000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.8814613096081515</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.891913555706214</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.9019340363955024</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.91150424744421243</c:v>
+                  <c:v>0.55000000000000016</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.92060461191144938</c:v>
+                  <c:v>0.56000000000000016</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.92921440127155985</c:v>
+                  <c:v>0.57000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.93731164947497114</c:v>
+                  <c:v>0.58000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.94487305919637898</c:v>
+                  <c:v>0.59000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.9518738994289212</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.95828789347780752</c:v>
+                  <c:v>0.6100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.96408709628667322</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.96924175989229144</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.9737201856453227</c:v>
+                  <c:v>0.64000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.97748856165313691</c:v>
+                  <c:v>0.64999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.98051078369140132</c:v>
+                  <c:v>0.65999999999999992</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.9827482575892772</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.98415968081305982</c:v>
+                  <c:v>0.67999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.98470080064806564</c:v>
+                  <c:v>0.69000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.98432414600036189</c:v>
+                  <c:v>0.70000000000000029</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.9829787293986858</c:v>
+                  <c:v>0.7100000000000003</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.98060971526073737</c:v>
+                  <c:v>0.71999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.97715804988250177</c:v>
+                  <c:v>0.72999999999999987</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.97256004789690242</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.96674692910749793</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.95964429860793277</c:v>
+                  <c:v>0.76000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.95117156191632157</c:v>
+                  <c:v>0.76999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.94124126544593856</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.92975835095034176</c:v>
+                  <c:v>0.79000000000000015</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.91661931056118318</c:v>
+                  <c:v>0.79999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.90171122660390257</c:v>
+                  <c:v>0.80999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.88491067743421226</c:v>
+                  <c:v>0.82000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.86608248696551104</c:v>
+                  <c:v>0.83000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.84507829120031042</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.82173488974137321</c:v>
+                  <c:v>0.85000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.79587234368918136</c:v>
+                  <c:v>0.8600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.7672917732074247</c:v>
+                  <c:v>0.87000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.73577279793694983</c:v>
+                  <c:v>0.88000000000000012</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.70107055081202985</c:v>
+                  <c:v>0.8899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.66291217995942708</c:v>
+                  <c:v>0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.62099273328552229</c:v>
+                  <c:v>0.91000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.57497029480656048</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.52446020904081769</c:v>
+                  <c:v>0.92999999999999994</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.46902818754118625</c:v>
+                  <c:v>0.94000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.408182036734277</c:v>
+                  <c:v>0.95000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.34136167427795788</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.26792700606693509</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.18714310923957489</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>9.816199587860748E-2</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4926,11 +4929,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152744704"/>
-        <c:axId val="152746240"/>
+        <c:axId val="242915464"/>
+        <c:axId val="242915856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152744704"/>
+        <c:axId val="242915464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4987,12 +4990,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152746240"/>
+        <c:crossAx val="242915856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="152746240"/>
+        <c:axId val="242915856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5049,7 +5052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152744704"/>
+        <c:crossAx val="242915464"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5359,11 +5362,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152688896"/>
-        <c:axId val="152690688"/>
+        <c:axId val="242917032"/>
+        <c:axId val="143827048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152688896"/>
+        <c:axId val="242917032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5420,12 +5423,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152690688"/>
+        <c:crossAx val="143827048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="152690688"/>
+        <c:axId val="143827048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5482,7 +5485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152688896"/>
+        <c:crossAx val="242917032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5646,6 +5649,95 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$21:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$21:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.8773417457071169</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6028418720925002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3520847537699998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1309688410324998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.93949413388</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7776606323124999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.64546833633</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5429172459325</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4700073611200002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4267386818925001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4131112082499999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -5654,11 +5746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152786432"/>
-        <c:axId val="152787968"/>
+        <c:axId val="187776936"/>
+        <c:axId val="187771448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152786432"/>
+        <c:axId val="187776936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5668,12 +5760,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152787968"/>
+        <c:crossAx val="187771448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="152787968"/>
+        <c:axId val="187771448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5684,7 +5776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152786432"/>
+        <c:crossAx val="187776936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5768,36 +5860,6 @@
                 <c:pt idx="10">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.95</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5808,37 +5870,37 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3.7585000000000002</c:v>
+                  <c:v>2.8773417457071169</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6715</c:v>
+                  <c:v>2.6028418720925002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3090000000000002</c:v>
+                  <c:v>2.3520847537699998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0783999999999998</c:v>
+                  <c:v>2.1309688410324998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9097999999999999</c:v>
+                  <c:v>1.93949413388</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7776000000000001</c:v>
+                  <c:v>1.7776606323124999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6697</c:v>
+                  <c:v>1.64546833633</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.579</c:v>
+                  <c:v>1.5429172459325</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5009999999999999</c:v>
+                  <c:v>1.4700073611200002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4328000000000001</c:v>
+                  <c:v>1.4267386818925001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3725000000000001</c:v>
+                  <c:v>1.4131112082499999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5853,11 +5915,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152807680"/>
-        <c:axId val="198967296"/>
+        <c:axId val="187771056"/>
+        <c:axId val="187773800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152807680"/>
+        <c:axId val="187771056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5867,12 +5929,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198967296"/>
+        <c:crossAx val="187773800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198967296"/>
+        <c:axId val="187773800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
@@ -5885,7 +5947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152807680"/>
+        <c:crossAx val="187771056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7719,8 +7781,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>123826</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -7789,7 +7851,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7824,7 +7886,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -14734,8 +14796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14776,7 +14838,7 @@
       </c>
       <c r="J1" s="55">
         <f>L108</f>
-        <v>0.98470080064806564</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -14798,7 +14860,7 @@
       </c>
       <c r="J2">
         <f>K108</f>
-        <v>78069.421237720715</v>
+        <v>161009.86290936786</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -14810,7 +14872,7 @@
       </c>
       <c r="G3">
         <f>J2/F2</f>
-        <v>1.939494136</v>
+        <v>4</v>
       </c>
       <c r="K3" t="s">
         <v>81</v>
@@ -14821,7 +14883,7 @@
         <v>60</v>
       </c>
       <c r="B4" s="57">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="59"/>
       <c r="E4" t="s">
@@ -14838,8 +14900,7 @@
         <v>79</v>
       </c>
       <c r="K4" s="60">
-        <f>5.92824117*B4^2 + -5.904378534*B4 + 2.883240196</f>
-        <v>1.939494136</v>
+        <v>4</v>
       </c>
       <c r="L4" t="s">
         <v>83</v>
@@ -14933,7 +14994,7 @@
       </c>
       <c r="K7">
         <f>J7 * $F$2 * $K$4</f>
-        <v>78069.421237720715</v>
+        <v>161009.86290936786</v>
       </c>
       <c r="L7">
         <f>IFERROR(H7/K7,1)</f>
@@ -14978,15 +15039,15 @@
       </c>
       <c r="J8">
         <f t="shared" ref="J8:J71" si="8">(100-A8) * 0.01 * (1 - $B$4) + $B$4</f>
-        <v>0.99199999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="K8">
         <f t="shared" ref="K8:K71" si="9">J8 * $F$2 * $K$4</f>
-        <v>77444.865867818953</v>
+        <v>159399.76428027419</v>
       </c>
       <c r="L8">
         <f t="shared" ref="L8:L71" si="10">IFERROR(H8/K8,1)</f>
-        <v>2.0582353974546733E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -15027,15 +15088,15 @@
       </c>
       <c r="J9">
         <f t="shared" si="8"/>
-        <v>0.98399999999999999</v>
+        <v>0.98</v>
       </c>
       <c r="K9">
         <f t="shared" si="9"/>
-        <v>76820.310497917177</v>
+        <v>157789.66565118049</v>
       </c>
       <c r="L9">
         <f t="shared" si="10"/>
-        <v>4.1080194711126207E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -15076,15 +15137,15 @@
       </c>
       <c r="J10">
         <f t="shared" si="8"/>
-        <v>0.97599999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="K10">
         <f t="shared" si="9"/>
-        <v>76195.755128015415</v>
+        <v>156179.56702208682</v>
       </c>
       <c r="L10">
         <f t="shared" si="10"/>
-        <v>6.1491444015362169E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -15125,15 +15186,15 @@
       </c>
       <c r="J11">
         <f t="shared" si="8"/>
-        <v>0.96799999999999997</v>
+        <v>0.96</v>
       </c>
       <c r="K11">
         <f t="shared" si="9"/>
-        <v>75571.199758113653</v>
+        <v>154569.46839299315</v>
       </c>
       <c r="L11">
         <f t="shared" si="10"/>
-        <v>8.1813954992237869E-2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -15174,15 +15235,15 @@
       </c>
       <c r="J12">
         <f t="shared" si="8"/>
-        <v>0.96000000000000019</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="K12">
         <f t="shared" si="9"/>
-        <v>74946.644388211906</v>
+        <v>152959.36976389948</v>
       </c>
       <c r="L12">
         <f t="shared" si="10"/>
-        <v>0.10204550918356921</v>
+        <v>4.9999999999999996E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -15223,15 +15284,15 @@
       </c>
       <c r="J13">
         <f t="shared" si="8"/>
-        <v>0.95200000000000018</v>
+        <v>0.94000000000000006</v>
       </c>
       <c r="K13">
         <f t="shared" si="9"/>
-        <v>74322.089018310129</v>
+        <v>151349.27113480581</v>
       </c>
       <c r="L13">
         <f t="shared" si="10"/>
-        <v>0.12218381356114935</v>
+        <v>6.0000000000000012E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -15272,15 +15333,15 @@
       </c>
       <c r="J14">
         <f t="shared" si="8"/>
-        <v>0.94400000000000017</v>
+        <v>0.93</v>
       </c>
       <c r="K14">
         <f t="shared" si="9"/>
-        <v>73697.533648408367</v>
+        <v>149739.17250571211</v>
       </c>
       <c r="L14">
         <f t="shared" si="10"/>
-        <v>0.14222649736700138</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -15321,15 +15382,15 @@
       </c>
       <c r="J15">
         <f t="shared" si="8"/>
-        <v>0.93600000000000017</v>
+        <v>0.92</v>
       </c>
       <c r="K15">
         <f t="shared" si="9"/>
-        <v>73072.978278506605</v>
+        <v>148129.07387661844</v>
       </c>
       <c r="L15">
         <f t="shared" si="10"/>
-        <v>0.16217110879159394</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -15370,15 +15431,15 @@
       </c>
       <c r="J16">
         <f t="shared" si="8"/>
-        <v>0.92800000000000016</v>
+        <v>0.91</v>
       </c>
       <c r="K16">
         <f t="shared" si="9"/>
-        <v>72448.422908604829</v>
+        <v>146518.97524752477</v>
       </c>
       <c r="L16">
         <f t="shared" si="10"/>
-        <v>0.1820151114802393</v>
+        <v>9.0000000000000011E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -15419,15 +15480,15 @@
       </c>
       <c r="J17">
         <f t="shared" si="8"/>
-        <v>0.92000000000000015</v>
+        <v>0.9</v>
       </c>
       <c r="K17">
         <f t="shared" si="9"/>
-        <v>71823.867538703082</v>
+        <v>144908.87661843107</v>
       </c>
       <c r="L17">
         <f t="shared" si="10"/>
-        <v>0.20175588085721691</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -15468,15 +15529,15 @@
       </c>
       <c r="J18">
         <f t="shared" si="8"/>
-        <v>0.91200000000000014</v>
+        <v>0.89</v>
       </c>
       <c r="K18">
         <f t="shared" si="9"/>
-        <v>71199.312168801305</v>
+        <v>143298.7779893374</v>
       </c>
       <c r="L18">
         <f t="shared" si="10"/>
-        <v>0.22139070025643051</v>
+        <v>0.11000000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -15517,15 +15578,15 @@
       </c>
       <c r="J19">
         <f t="shared" si="8"/>
-        <v>0.90400000000000014</v>
+        <v>0.88</v>
       </c>
       <c r="K19">
         <f t="shared" si="9"/>
-        <v>70574.756798899543</v>
+        <v>141688.67936024372</v>
       </c>
       <c r="L19">
         <f t="shared" si="10"/>
-        <v>0.24091675684661182</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -15566,15 +15627,15 @@
       </c>
       <c r="J20">
         <f t="shared" si="8"/>
-        <v>0.89600000000000013</v>
+        <v>0.87</v>
       </c>
       <c r="K20">
         <f t="shared" si="9"/>
-        <v>69950.201428997767</v>
+        <v>140078.58073115002</v>
       </c>
       <c r="L20">
         <f t="shared" si="10"/>
-        <v>0.26033113733823338</v>
+        <v>0.13000000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -15615,15 +15676,15 @@
       </c>
       <c r="J21">
         <f t="shared" si="8"/>
-        <v>0.88800000000000012</v>
+        <v>0.86</v>
       </c>
       <c r="K21">
         <f t="shared" si="9"/>
-        <v>69325.646059096005</v>
+        <v>138468.48210205635</v>
       </c>
       <c r="L21">
         <f t="shared" si="10"/>
-        <v>0.27963082345836099</v>
+        <v>0.14000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -15664,15 +15725,15 @@
       </c>
       <c r="J22">
         <f t="shared" si="8"/>
-        <v>0.88000000000000012</v>
+        <v>0.85</v>
       </c>
       <c r="K22">
         <f t="shared" si="9"/>
-        <v>68701.090689194229</v>
+        <v>136858.38347296268</v>
       </c>
       <c r="L22">
         <f t="shared" si="10"/>
-        <v>0.2988126871786812</v>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -15713,15 +15774,15 @@
       </c>
       <c r="J23">
         <f t="shared" si="8"/>
-        <v>0.87200000000000011</v>
+        <v>0.84</v>
       </c>
       <c r="K23">
         <f t="shared" si="9"/>
-        <v>68076.535319292467</v>
+        <v>135248.28484386901</v>
       </c>
       <c r="L23">
         <f t="shared" si="10"/>
-        <v>0.31787348568085072</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -15762,15 +15823,15 @@
       </c>
       <c r="J24">
         <f t="shared" si="8"/>
-        <v>0.8640000000000001</v>
+        <v>0.83000000000000007</v>
       </c>
       <c r="K24">
         <f t="shared" si="9"/>
-        <v>67451.979949390705</v>
+        <v>133638.18621477534</v>
       </c>
       <c r="L24">
         <f t="shared" si="10"/>
-        <v>0.33680985604214309</v>
+        <v>0.16999999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -15811,15 +15872,15 @@
       </c>
       <c r="J25">
         <f t="shared" si="8"/>
-        <v>0.85600000000000009</v>
+        <v>0.82000000000000006</v>
       </c>
       <c r="K25">
         <f t="shared" si="9"/>
-        <v>66827.424579488943</v>
+        <v>132028.08758568164</v>
       </c>
       <c r="L25">
         <f t="shared" si="10"/>
-        <v>0.35561830962309454</v>
+        <v>0.18000000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -15860,15 +15921,15 @@
       </c>
       <c r="J26">
         <f t="shared" si="8"/>
-        <v>0.84800000000000009</v>
+        <v>0.81</v>
       </c>
       <c r="K26">
         <f t="shared" si="9"/>
-        <v>66202.869209587181</v>
+        <v>130417.98895658797</v>
       </c>
       <c r="L26">
         <f t="shared" si="10"/>
-        <v>0.37429522613746891</v>
+        <v>0.18999999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -15909,15 +15970,15 @@
       </c>
       <c r="J27">
         <f t="shared" si="8"/>
-        <v>0.84000000000000008</v>
+        <v>0.8</v>
       </c>
       <c r="K27">
         <f t="shared" si="9"/>
-        <v>65578.313839685405</v>
+        <v>128807.8903274943</v>
       </c>
       <c r="L27">
         <f t="shared" si="10"/>
-        <v>0.39283684738336427</v>
+        <v>0.19999999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -15958,15 +16019,15 @@
       </c>
       <c r="J28">
         <f t="shared" si="8"/>
-        <v>0.83200000000000007</v>
+        <v>0.79</v>
       </c>
       <c r="K28">
         <f t="shared" si="9"/>
-        <v>64953.758469783643</v>
+        <v>127197.79169840062</v>
       </c>
       <c r="L28">
         <f t="shared" si="10"/>
-        <v>0.41123927061265109</v>
+        <v>0.21000000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -16007,15 +16068,15 @@
       </c>
       <c r="J29">
         <f t="shared" si="8"/>
-        <v>0.82400000000000007</v>
+        <v>0.78</v>
       </c>
       <c r="K29">
         <f t="shared" si="9"/>
-        <v>64329.203099881874</v>
+        <v>125587.69306930693</v>
       </c>
       <c r="L29">
         <f t="shared" si="10"/>
-        <v>0.42949844151416616</v>
+        <v>0.22000000000000006</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -16056,15 +16117,15 @@
       </c>
       <c r="J30">
         <f t="shared" si="8"/>
-        <v>0.81600000000000006</v>
+        <v>0.77</v>
       </c>
       <c r="K30">
         <f t="shared" si="9"/>
-        <v>63704.647729980112</v>
+        <v>123977.59444021326</v>
       </c>
       <c r="L30">
         <f t="shared" si="10"/>
-        <v>0.4476101467841514</v>
+        <v>0.23000000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -16105,15 +16166,15 @@
       </c>
       <c r="J31">
         <f t="shared" si="8"/>
-        <v>0.80800000000000005</v>
+        <v>0.76</v>
       </c>
       <c r="K31">
         <f t="shared" si="9"/>
-        <v>63080.092360078343</v>
+        <v>122367.49581111957</v>
       </c>
       <c r="L31">
         <f t="shared" si="10"/>
-        <v>0.46557000625533373</v>
+        <v>0.24000000000000005</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -16154,15 +16215,15 @@
       </c>
       <c r="J32">
         <f t="shared" si="8"/>
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="K32">
         <f t="shared" si="9"/>
-        <v>62455.536990176581</v>
+        <v>120757.39718202589</v>
       </c>
       <c r="L32">
         <f t="shared" si="10"/>
-        <v>0.48337346455374897</v>
+        <v>0.25000000000000006</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -16203,15 +16264,15 @@
       </c>
       <c r="J33">
         <f t="shared" si="8"/>
-        <v>0.79200000000000004</v>
+        <v>0.74</v>
       </c>
       <c r="K33">
         <f t="shared" si="9"/>
-        <v>61830.981620274812</v>
+        <v>119147.29855293222</v>
       </c>
       <c r="L33">
         <f t="shared" si="10"/>
-        <v>0.50101578224991949</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -16252,15 +16313,15 @@
       </c>
       <c r="J34">
         <f t="shared" si="8"/>
-        <v>0.78400000000000003</v>
+        <v>0.73</v>
       </c>
       <c r="K34">
         <f t="shared" si="9"/>
-        <v>61206.426250373042</v>
+        <v>117537.19992383853</v>
       </c>
       <c r="L34">
         <f t="shared" si="10"/>
-        <v>0.51849202646826642</v>
+        <v>0.27000000000000007</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -16301,15 +16362,15 @@
       </c>
       <c r="J35">
         <f t="shared" si="8"/>
-        <v>0.77600000000000002</v>
+        <v>0.72</v>
       </c>
       <c r="K35">
         <f t="shared" si="9"/>
-        <v>60581.870880471281</v>
+        <v>115927.10129474486</v>
       </c>
       <c r="L35">
         <f t="shared" si="10"/>
-        <v>0.53579706091566071</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -16350,15 +16411,15 @@
       </c>
       <c r="J36">
         <f t="shared" si="8"/>
-        <v>0.76800000000000002</v>
+        <v>0.71</v>
       </c>
       <c r="K36">
         <f t="shared" si="9"/>
-        <v>59957.315510569511</v>
+        <v>114317.00266565118</v>
       </c>
       <c r="L36">
         <f t="shared" si="10"/>
-        <v>0.55292553528676069</v>
+        <v>0.29000000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -16399,15 +16460,15 @@
       </c>
       <c r="J37">
         <f t="shared" si="8"/>
-        <v>0.76</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="K37">
         <f t="shared" si="9"/>
-        <v>59332.760140667742</v>
+        <v>112706.90403655752</v>
       </c>
       <c r="L37">
         <f t="shared" si="10"/>
-        <v>0.56987187400020933</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -16448,15 +16509,15 @@
       </c>
       <c r="J38">
         <f t="shared" si="8"/>
-        <v>0.752</v>
+        <v>0.69000000000000006</v>
       </c>
       <c r="K38">
         <f t="shared" si="9"/>
-        <v>58708.204770765973</v>
+        <v>111096.80540746383</v>
       </c>
       <c r="L38">
         <f t="shared" si="10"/>
-        <v>0.58663026421586906</v>
+        <v>0.30999999999999994</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16497,15 +16558,15 @@
       </c>
       <c r="J39">
         <f t="shared" si="8"/>
-        <v>0.74399999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="K39">
         <f t="shared" si="9"/>
-        <v>58083.649400864211</v>
+        <v>109486.70677837015</v>
       </c>
       <c r="L39">
         <f t="shared" si="10"/>
-        <v>0.60319464307897219</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -16546,15 +16607,15 @@
       </c>
       <c r="J40">
         <f t="shared" si="8"/>
-        <v>0.73599999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="K40">
         <f t="shared" si="9"/>
-        <v>57459.094030962442</v>
+        <v>107876.60814927648</v>
       </c>
       <c r="L40">
         <f t="shared" si="10"/>
-        <v>0.61955868413237059</v>
+        <v>0.33</v>
       </c>
       <c r="O40" s="61" t="s">
         <v>84</v>
@@ -16610,15 +16671,15 @@
       </c>
       <c r="J41">
         <f t="shared" si="8"/>
-        <v>0.72799999999999998</v>
+        <v>0.66</v>
       </c>
       <c r="K41">
         <f t="shared" si="9"/>
-        <v>56834.538661060673</v>
+        <v>106266.50952018279</v>
       </c>
       <c r="L41">
         <f t="shared" si="10"/>
-        <v>0.63571578283288666</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="O41" s="64">
         <v>0</v>
@@ -16678,15 +16739,15 @@
       </c>
       <c r="J42">
         <f t="shared" si="8"/>
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="K42">
         <f t="shared" si="9"/>
-        <v>56209.983291158918</v>
+        <v>104656.41089108911</v>
       </c>
       <c r="L42">
         <f t="shared" si="10"/>
-        <v>0.65165904110209139</v>
+        <v>0.35000000000000009</v>
       </c>
       <c r="O42" s="64">
         <v>0.05</v>
@@ -16748,15 +16809,15 @@
       </c>
       <c r="J43">
         <f t="shared" si="8"/>
-        <v>0.71199999999999997</v>
+        <v>0.64</v>
       </c>
       <c r="K43">
         <f t="shared" si="9"/>
-        <v>55585.427921257149</v>
+        <v>103046.31226199544</v>
       </c>
       <c r="L43">
         <f t="shared" si="10"/>
-        <v>0.66738125083555822</v>
+        <v>0.36000000000000004</v>
       </c>
       <c r="O43" s="64">
         <v>0.1</v>
@@ -16818,15 +16879,15 @@
       </c>
       <c r="J44">
         <f t="shared" si="8"/>
-        <v>0.70399999999999996</v>
+        <v>0.63</v>
       </c>
       <c r="K44">
         <f t="shared" si="9"/>
-        <v>54960.87255135538</v>
+        <v>101436.21363290175</v>
       </c>
       <c r="L44">
         <f t="shared" si="10"/>
-        <v>0.68287487628775101</v>
+        <v>0.37000000000000005</v>
       </c>
       <c r="O44" s="64">
         <v>0.15</v>
@@ -16888,15 +16949,15 @@
       </c>
       <c r="J45">
         <f t="shared" si="8"/>
-        <v>0.69599999999999995</v>
+        <v>0.62</v>
       </c>
       <c r="K45">
         <f t="shared" si="9"/>
-        <v>54336.317181453618</v>
+        <v>99826.115003808067</v>
       </c>
       <c r="L45">
         <f t="shared" si="10"/>
-        <v>0.69813203524207368</v>
+        <v>0.38000000000000006</v>
       </c>
       <c r="O45" s="64">
         <v>0.2</v>
@@ -16958,15 +17019,15 @@
       </c>
       <c r="J46">
         <f t="shared" si="8"/>
-        <v>0.68799999999999994</v>
+        <v>0.61</v>
       </c>
       <c r="K46">
         <f t="shared" si="9"/>
-        <v>53711.761811551849</v>
+        <v>98216.016374714396</v>
       </c>
       <c r="L46">
         <f t="shared" si="10"/>
-        <v>0.71314447886720567</v>
+        <v>0.39000000000000007</v>
       </c>
       <c r="O46" s="64">
         <v>0.25</v>
@@ -17028,15 +17089,15 @@
       </c>
       <c r="J47">
         <f t="shared" si="8"/>
-        <v>0.67999999999999994</v>
+        <v>0.6</v>
       </c>
       <c r="K47">
         <f t="shared" si="9"/>
-        <v>53087.20644165008</v>
+        <v>96605.917745620711</v>
       </c>
       <c r="L47">
         <f t="shared" si="10"/>
-        <v>0.72790357015152796</v>
+        <v>0.4</v>
       </c>
       <c r="O47" s="64">
         <v>0.3</v>
@@ -17098,15 +17159,15 @@
       </c>
       <c r="J48">
         <f t="shared" si="8"/>
-        <v>0.67199999999999993</v>
+        <v>0.59</v>
       </c>
       <c r="K48">
         <f t="shared" si="9"/>
-        <v>52462.651071748318</v>
+        <v>94995.81911652704</v>
       </c>
       <c r="L48">
         <f t="shared" si="10"/>
-        <v>0.74240026079715471</v>
+        <v>0.40999999999999992</v>
       </c>
       <c r="O48" s="64">
         <v>0.35</v>
@@ -17168,15 +17229,15 @@
       </c>
       <c r="J49">
         <f t="shared" si="8"/>
-        <v>0.66399999999999992</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K49">
         <f t="shared" si="9"/>
-        <v>51838.095701846549</v>
+        <v>93385.720487433355</v>
       </c>
       <c r="L49">
         <f t="shared" si="10"/>
-        <v>0.75662506644365157</v>
+        <v>0.4200000000000001</v>
       </c>
       <c r="O49" s="64">
         <v>0.4</v>
@@ -17238,15 +17299,15 @@
       </c>
       <c r="J50">
         <f t="shared" si="8"/>
-        <v>0.65600000000000014</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="K50">
         <f t="shared" si="9"/>
-        <v>51213.540331944801</v>
+        <v>91775.621858339684</v>
       </c>
       <c r="L50">
         <f t="shared" si="10"/>
-        <v>0.77056804007885449</v>
+        <v>0.4300000000000001</v>
       </c>
       <c r="O50" s="64">
         <v>0.45</v>
@@ -17308,15 +17369,15 @@
       </c>
       <c r="J51">
         <f t="shared" si="8"/>
-        <v>0.64800000000000013</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="K51">
         <f t="shared" si="9"/>
-        <v>50588.984962043032</v>
+        <v>90165.523229246013</v>
       </c>
       <c r="L51">
         <f t="shared" si="10"/>
-        <v>0.78421874348012355</v>
+        <v>0.44000000000000006</v>
       </c>
       <c r="O51" s="64">
         <v>0.5</v>
@@ -17378,15 +17439,15 @@
       </c>
       <c r="J52">
         <f t="shared" si="8"/>
-        <v>0.64000000000000012</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K52">
         <f t="shared" si="9"/>
-        <v>49964.42959214127</v>
+        <v>88555.424600152328</v>
       </c>
       <c r="L52">
         <f t="shared" si="10"/>
-        <v>0.79756621651368564</v>
+        <v>0.45</v>
       </c>
       <c r="O52" s="64"/>
       <c r="P52" s="65"/>
@@ -17434,15 +17495,15 @@
       </c>
       <c r="J53">
         <f t="shared" si="8"/>
-        <v>0.63200000000000012</v>
+        <v>0.54</v>
       </c>
       <c r="K53">
         <f t="shared" si="9"/>
-        <v>49339.874222239501</v>
+        <v>86945.325971058657</v>
       </c>
       <c r="L53">
         <f t="shared" si="10"/>
-        <v>0.81059894410228672</v>
+        <v>0.45999999999999991</v>
       </c>
       <c r="O53" s="64"/>
       <c r="P53" s="65" t="s">
@@ -17492,15 +17553,15 @@
       </c>
       <c r="J54">
         <f t="shared" si="8"/>
-        <v>0.62400000000000011</v>
+        <v>0.53</v>
       </c>
       <c r="K54">
         <f t="shared" si="9"/>
-        <v>48715.318852337732</v>
+        <v>85335.227341964972</v>
       </c>
       <c r="L54">
         <f t="shared" si="10"/>
-        <v>0.82330482065188981</v>
+        <v>0.47000000000000008</v>
       </c>
       <c r="O54" s="64"/>
       <c r="P54" s="65" t="s">
@@ -17550,15 +17611,15 @@
       </c>
       <c r="J55">
         <f t="shared" si="8"/>
-        <v>0.6160000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="K55">
         <f t="shared" si="9"/>
-        <v>48090.76348243597</v>
+        <v>83725.128712871287</v>
       </c>
       <c r="L55">
         <f t="shared" si="10"/>
-        <v>0.83567111170642927</v>
+        <v>0.48000000000000004</v>
       </c>
       <c r="O55" s="64"/>
       <c r="P55" s="65"/>
@@ -17606,15 +17667,15 @@
       </c>
       <c r="J56">
         <f t="shared" si="8"/>
-        <v>0.6080000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="K56">
         <f t="shared" si="9"/>
-        <v>47466.208112534201</v>
+        <v>82115.030083777616</v>
       </c>
       <c r="L56">
         <f t="shared" si="10"/>
-        <v>0.84768441257531135</v>
+        <v>0.49</v>
       </c>
       <c r="O56" s="64"/>
       <c r="P56" s="65"/>
@@ -17662,15 +17723,15 @@
       </c>
       <c r="J57">
         <f t="shared" si="8"/>
-        <v>0.60000000000000009</v>
+        <v>0.5</v>
       </c>
       <c r="K57">
         <f t="shared" si="9"/>
-        <v>46841.652742632432</v>
+        <v>80504.93145468393</v>
       </c>
       <c r="L57">
         <f t="shared" si="10"/>
-        <v>0.85933060365110925</v>
+        <v>0.5</v>
       </c>
       <c r="O57" s="64"/>
       <c r="P57" s="65"/>
@@ -17718,15 +17779,15 @@
       </c>
       <c r="J58">
         <f t="shared" si="8"/>
-        <v>0.59200000000000008</v>
+        <v>0.49</v>
       </c>
       <c r="K58">
         <f t="shared" si="9"/>
-        <v>46217.09737273067</v>
+        <v>78894.832825590245</v>
       </c>
       <c r="L58">
         <f t="shared" si="10"/>
-        <v>0.87059480210437379</v>
+        <v>0.51000000000000012</v>
       </c>
       <c r="O58" s="64"/>
       <c r="P58" s="65"/>
@@ -17774,15 +17835,15 @@
       </c>
       <c r="J59">
         <f t="shared" si="8"/>
-        <v>0.58400000000000007</v>
+        <v>0.48</v>
       </c>
       <c r="K59">
         <f t="shared" si="9"/>
-        <v>45592.542002828908</v>
+        <v>77284.734196496574</v>
       </c>
       <c r="L59">
         <f t="shared" si="10"/>
-        <v>0.8814613096081515</v>
+        <v>0.52</v>
       </c>
       <c r="O59" s="64"/>
       <c r="P59" s="65"/>
@@ -17830,15 +17891,15 @@
       </c>
       <c r="J60">
         <f t="shared" si="8"/>
-        <v>0.57600000000000007</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="K60">
         <f t="shared" si="9"/>
-        <v>44967.986632927139</v>
+        <v>75674.635567402904</v>
       </c>
       <c r="L60">
         <f t="shared" si="10"/>
-        <v>0.891913555706214</v>
+        <v>0.53</v>
       </c>
       <c r="O60" s="64"/>
       <c r="P60" s="65"/>
@@ -17886,15 +17947,15 @@
       </c>
       <c r="J61">
         <f t="shared" si="8"/>
-        <v>0.56800000000000006</v>
+        <v>0.46</v>
       </c>
       <c r="K61">
         <f t="shared" si="9"/>
-        <v>44343.43126302537</v>
+        <v>74064.536938309218</v>
       </c>
       <c r="L61">
         <f t="shared" si="10"/>
-        <v>0.9019340363955024</v>
+        <v>0.54</v>
       </c>
       <c r="O61" s="64"/>
       <c r="P61" s="65"/>
@@ -17942,15 +18003,15 @@
       </c>
       <c r="J62">
         <f t="shared" si="8"/>
-        <v>0.56000000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="K62">
         <f t="shared" si="9"/>
-        <v>43718.875893123608</v>
+        <v>72454.438309215533</v>
       </c>
       <c r="L62">
         <f t="shared" si="10"/>
-        <v>0.91150424744421243</v>
+        <v>0.55000000000000016</v>
       </c>
       <c r="O62" s="67"/>
       <c r="P62" s="68"/>
@@ -17998,15 +18059,15 @@
       </c>
       <c r="J63">
         <f t="shared" si="8"/>
-        <v>0.55200000000000005</v>
+        <v>0.44</v>
       </c>
       <c r="K63">
         <f t="shared" si="9"/>
-        <v>43094.320523221839</v>
+        <v>70844.339680121862</v>
       </c>
       <c r="L63">
         <f t="shared" si="10"/>
-        <v>0.92060461191144938</v>
+        <v>0.56000000000000016</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -18047,15 +18108,15 @@
       </c>
       <c r="J64">
         <f t="shared" si="8"/>
-        <v>0.54400000000000004</v>
+        <v>0.43</v>
       </c>
       <c r="K64">
         <f t="shared" si="9"/>
-        <v>42469.76515332007</v>
+        <v>69234.241051028177</v>
       </c>
       <c r="L64">
         <f t="shared" si="10"/>
-        <v>0.92921440127155985</v>
+        <v>0.57000000000000006</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -18096,15 +18157,15 @@
       </c>
       <c r="J65">
         <f t="shared" si="8"/>
-        <v>0.53600000000000003</v>
+        <v>0.42</v>
       </c>
       <c r="K65">
         <f t="shared" si="9"/>
-        <v>41845.209783418308</v>
+        <v>67624.142421934506</v>
       </c>
       <c r="L65">
         <f t="shared" si="10"/>
-        <v>0.93731164947497114</v>
+        <v>0.58000000000000007</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -18145,15 +18206,15 @@
       </c>
       <c r="J66">
         <f t="shared" si="8"/>
-        <v>0.52800000000000002</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="K66">
         <f t="shared" si="9"/>
-        <v>41220.654413516539</v>
+        <v>66014.043792840821</v>
       </c>
       <c r="L66">
         <f t="shared" si="10"/>
-        <v>0.94487305919637898</v>
+        <v>0.59000000000000008</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -18194,15 +18255,15 @@
       </c>
       <c r="J67">
         <f t="shared" si="8"/>
-        <v>0.52</v>
+        <v>0.4</v>
       </c>
       <c r="K67">
         <f t="shared" si="9"/>
-        <v>40596.099043614769</v>
+        <v>64403.94516374715</v>
       </c>
       <c r="L67">
         <f t="shared" si="10"/>
-        <v>0.9518738994289212</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -18243,15 +18304,15 @@
       </c>
       <c r="J68">
         <f t="shared" si="8"/>
-        <v>0.51200000000000001</v>
+        <v>0.39</v>
       </c>
       <c r="K68">
         <f t="shared" si="9"/>
-        <v>39971.543673713008</v>
+        <v>62793.846534653465</v>
       </c>
       <c r="L68">
         <f t="shared" si="10"/>
-        <v>0.95828789347780752</v>
+        <v>0.6100000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -18292,15 +18353,15 @@
       </c>
       <c r="J69">
         <f t="shared" si="8"/>
-        <v>0.504</v>
+        <v>0.38</v>
       </c>
       <c r="K69">
         <f t="shared" si="9"/>
-        <v>39346.988303811238</v>
+        <v>61183.747905559787</v>
       </c>
       <c r="L69">
         <f t="shared" si="10"/>
-        <v>0.96408709628667322</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -18341,15 +18402,15 @@
       </c>
       <c r="J70">
         <f t="shared" si="8"/>
-        <v>0.496</v>
+        <v>0.37</v>
       </c>
       <c r="K70">
         <f t="shared" si="9"/>
-        <v>38722.432933909477</v>
+        <v>59573.649276466109</v>
       </c>
       <c r="L70">
         <f t="shared" si="10"/>
-        <v>0.96924175989229144</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -18390,15 +18451,15 @@
       </c>
       <c r="J71">
         <f t="shared" si="8"/>
-        <v>0.48799999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="K71">
         <f t="shared" si="9"/>
-        <v>38097.877564007707</v>
+        <v>57963.550647372431</v>
       </c>
       <c r="L71">
         <f t="shared" si="10"/>
-        <v>0.9737201856453227</v>
+        <v>0.64000000000000012</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -18439,15 +18500,15 @@
       </c>
       <c r="J72">
         <f t="shared" ref="J72:J107" si="21">(100-A72) * 0.01 * (1 - $B$4) + $B$4</f>
-        <v>0.48000000000000004</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="K72">
         <f t="shared" ref="K72:K107" si="22">J72 * $F$2 * $K$4</f>
-        <v>37473.322194105946</v>
+        <v>56353.45201827876</v>
       </c>
       <c r="L72">
         <f t="shared" ref="L72:L107" si="23">IFERROR(H72/K72,1)</f>
-        <v>0.97748856165313691</v>
+        <v>0.64999999999999991</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -18488,15 +18549,15 @@
       </c>
       <c r="J73">
         <f t="shared" si="21"/>
-        <v>0.47200000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="K73">
         <f t="shared" si="22"/>
-        <v>36848.766824204176</v>
+        <v>54743.353389185075</v>
       </c>
       <c r="L73">
         <f t="shared" si="23"/>
-        <v>0.98051078369140132</v>
+        <v>0.65999999999999992</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -18537,15 +18598,15 @@
       </c>
       <c r="J74">
         <f t="shared" si="21"/>
-        <v>0.46400000000000002</v>
+        <v>0.33</v>
       </c>
       <c r="K74">
         <f t="shared" si="22"/>
-        <v>36224.211454302414</v>
+        <v>53133.254760091397</v>
       </c>
       <c r="L74">
         <f t="shared" si="23"/>
-        <v>0.9827482575892772</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -18586,15 +18647,15 @@
       </c>
       <c r="J75">
         <f t="shared" si="21"/>
-        <v>0.45600000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="K75">
         <f t="shared" si="22"/>
-        <v>35599.656084400653</v>
+        <v>51523.156130997719</v>
       </c>
       <c r="L75">
         <f t="shared" si="23"/>
-        <v>0.98415968081305982</v>
+        <v>0.67999999999999994</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -18635,15 +18696,15 @@
       </c>
       <c r="J76">
         <f t="shared" si="21"/>
-        <v>0.44800000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="K76">
         <f t="shared" si="22"/>
-        <v>34975.100714498883</v>
+        <v>49913.057501904033</v>
       </c>
       <c r="L76">
         <f t="shared" si="23"/>
-        <v>0.98470080064806564</v>
+        <v>0.69000000000000006</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -18684,15 +18745,15 @@
       </c>
       <c r="J77">
         <f t="shared" si="21"/>
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
       <c r="K77">
         <f t="shared" si="22"/>
-        <v>34350.545344597114</v>
+        <v>48302.958872810355</v>
       </c>
       <c r="L77">
         <f t="shared" si="23"/>
-        <v>0.98432414600036189</v>
+        <v>0.70000000000000029</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -18733,15 +18794,15 @@
       </c>
       <c r="J78">
         <f t="shared" si="21"/>
-        <v>0.432</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K78">
         <f t="shared" si="22"/>
-        <v>33725.989974695352</v>
+        <v>46692.860243716677</v>
       </c>
       <c r="L78">
         <f t="shared" si="23"/>
-        <v>0.9829787293986858</v>
+        <v>0.7100000000000003</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -18782,15 +18843,15 @@
       </c>
       <c r="J79">
         <f t="shared" si="21"/>
-        <v>0.42400000000000004</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K79">
         <f t="shared" si="22"/>
-        <v>33101.434604793591</v>
+        <v>45082.761614623007</v>
       </c>
       <c r="L79">
         <f t="shared" si="23"/>
-        <v>0.98060971526073737</v>
+        <v>0.71999999999999986</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -18831,15 +18892,15 @@
       </c>
       <c r="J80">
         <f t="shared" si="21"/>
-        <v>0.41600000000000004</v>
+        <v>0.27</v>
       </c>
       <c r="K80">
         <f t="shared" si="22"/>
-        <v>32476.879234891821</v>
+        <v>43472.662985529329</v>
       </c>
       <c r="L80">
         <f t="shared" si="23"/>
-        <v>0.97715804988250177</v>
+        <v>0.72999999999999987</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -18880,15 +18941,15 @@
       </c>
       <c r="J81">
         <f t="shared" si="21"/>
-        <v>0.40800000000000003</v>
+        <v>0.26</v>
       </c>
       <c r="K81">
         <f t="shared" si="22"/>
-        <v>31852.323864990056</v>
+        <v>41862.564356435643</v>
       </c>
       <c r="L81">
         <f t="shared" si="23"/>
-        <v>0.97256004789690242</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -18929,15 +18990,15 @@
       </c>
       <c r="J82">
         <f t="shared" si="21"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="K82">
         <f t="shared" si="22"/>
-        <v>31227.76849508829</v>
+        <v>40252.465727341965</v>
       </c>
       <c r="L82">
         <f t="shared" si="23"/>
-        <v>0.96674692910749793</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -18978,15 +19039,15 @@
       </c>
       <c r="J83">
         <f t="shared" si="21"/>
-        <v>0.39200000000000002</v>
+        <v>0.24</v>
       </c>
       <c r="K83">
         <f t="shared" si="22"/>
-        <v>30603.213125186521</v>
+        <v>38642.367098248287</v>
       </c>
       <c r="L83">
         <f t="shared" si="23"/>
-        <v>0.95964429860793277</v>
+        <v>0.76000000000000012</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -19027,15 +19088,15 @@
       </c>
       <c r="J84">
         <f t="shared" si="21"/>
-        <v>0.38400000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="K84">
         <f t="shared" si="22"/>
-        <v>29978.657755284756</v>
+        <v>37032.268469154609</v>
       </c>
       <c r="L84">
         <f t="shared" si="23"/>
-        <v>0.95117156191632157</v>
+        <v>0.76999999999999991</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -19076,15 +19137,15 @@
       </c>
       <c r="J85">
         <f t="shared" si="21"/>
-        <v>0.376</v>
+        <v>0.22</v>
       </c>
       <c r="K85">
         <f t="shared" si="22"/>
-        <v>29354.102385382987</v>
+        <v>35422.169840060931</v>
       </c>
       <c r="L85">
         <f t="shared" si="23"/>
-        <v>0.94124126544593856</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -19125,15 +19186,15 @@
       </c>
       <c r="J86">
         <f t="shared" si="21"/>
-        <v>0.36799999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="K86">
         <f t="shared" si="22"/>
-        <v>28729.547015481221</v>
+        <v>33812.071210967253</v>
       </c>
       <c r="L86">
         <f t="shared" si="23"/>
-        <v>0.92975835095034176</v>
+        <v>0.79000000000000015</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -19174,15 +19235,15 @@
       </c>
       <c r="J87">
         <f t="shared" si="21"/>
-        <v>0.36000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="K87">
         <f t="shared" si="22"/>
-        <v>28104.991645579463</v>
+        <v>32201.972581873575</v>
       </c>
       <c r="L87">
         <f t="shared" si="23"/>
-        <v>0.91661931056118318</v>
+        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -19223,15 +19284,15 @@
       </c>
       <c r="J88">
         <f t="shared" si="21"/>
-        <v>0.35200000000000004</v>
+        <v>0.19</v>
       </c>
       <c r="K88">
         <f t="shared" si="22"/>
-        <v>27480.436275677694</v>
+        <v>30591.873952779893</v>
       </c>
       <c r="L88">
         <f t="shared" si="23"/>
-        <v>0.90171122660390257</v>
+        <v>0.80999999999999994</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -19272,15 +19333,15 @@
       </c>
       <c r="J89">
         <f t="shared" si="21"/>
-        <v>0.34399999999999997</v>
+        <v>0.18</v>
       </c>
       <c r="K89">
         <f t="shared" si="22"/>
-        <v>26855.880905775924</v>
+        <v>28981.775323686215</v>
       </c>
       <c r="L89">
         <f t="shared" si="23"/>
-        <v>0.88491067743421226</v>
+        <v>0.82000000000000006</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -19321,15 +19382,15 @@
       </c>
       <c r="J90">
         <f t="shared" si="21"/>
-        <v>0.33600000000000002</v>
+        <v>0.17</v>
       </c>
       <c r="K90">
         <f t="shared" si="22"/>
-        <v>26231.325535874163</v>
+        <v>27371.676694592537</v>
       </c>
       <c r="L90">
         <f t="shared" si="23"/>
-        <v>0.86608248696551104</v>
+        <v>0.83000000000000018</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -19370,15 +19431,15 @@
       </c>
       <c r="J91">
         <f t="shared" si="21"/>
-        <v>0.32800000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="K91">
         <f t="shared" si="22"/>
-        <v>25606.770165972397</v>
+        <v>25761.578065498859</v>
       </c>
       <c r="L91">
         <f t="shared" si="23"/>
-        <v>0.84507829120031042</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -19419,15 +19480,15 @@
       </c>
       <c r="J92">
         <f t="shared" si="21"/>
-        <v>0.32</v>
+        <v>0.15</v>
       </c>
       <c r="K92">
         <f t="shared" si="22"/>
-        <v>24982.214796070632</v>
+        <v>24151.479436405178</v>
       </c>
       <c r="L92">
         <f t="shared" si="23"/>
-        <v>0.82173488974137321</v>
+        <v>0.85000000000000009</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -19468,15 +19529,15 @@
       </c>
       <c r="J93">
         <f t="shared" si="21"/>
-        <v>0.31200000000000006</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K93">
         <f t="shared" si="22"/>
-        <v>24357.659426168866</v>
+        <v>22541.380807311503</v>
       </c>
       <c r="L93">
         <f t="shared" si="23"/>
-        <v>0.79587234368918136</v>
+        <v>0.8600000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -19517,15 +19578,15 @@
       </c>
       <c r="J94">
         <f t="shared" si="21"/>
-        <v>0.30400000000000005</v>
+        <v>0.13</v>
       </c>
       <c r="K94">
         <f t="shared" si="22"/>
-        <v>23733.104056267101</v>
+        <v>20931.282178217822</v>
       </c>
       <c r="L94">
         <f t="shared" si="23"/>
-        <v>0.7672917732074247</v>
+        <v>0.87000000000000011</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -19566,15 +19627,15 @@
       </c>
       <c r="J95">
         <f t="shared" si="21"/>
-        <v>0.29600000000000004</v>
+        <v>0.12</v>
       </c>
       <c r="K95">
         <f t="shared" si="22"/>
-        <v>23108.548686365335</v>
+        <v>19321.183549124144</v>
       </c>
       <c r="L95">
         <f t="shared" si="23"/>
-        <v>0.73577279793694983</v>
+        <v>0.88000000000000012</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -19615,15 +19676,15 @@
       </c>
       <c r="J96">
         <f t="shared" si="21"/>
-        <v>0.28800000000000003</v>
+        <v>0.11</v>
       </c>
       <c r="K96">
         <f t="shared" si="22"/>
-        <v>22483.993316463569</v>
+        <v>17711.084920030466</v>
       </c>
       <c r="L96">
         <f t="shared" si="23"/>
-        <v>0.70107055081202985</v>
+        <v>0.8899999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -19664,15 +19725,15 @@
       </c>
       <c r="J97">
         <f t="shared" si="21"/>
-        <v>0.28000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="K97">
         <f t="shared" si="22"/>
-        <v>21859.437946561804</v>
+        <v>16100.986290936788</v>
       </c>
       <c r="L97">
         <f t="shared" si="23"/>
-        <v>0.66291217995942708</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -19713,15 +19774,15 @@
       </c>
       <c r="J98">
         <f t="shared" si="21"/>
-        <v>0.27200000000000002</v>
+        <v>0.09</v>
       </c>
       <c r="K98">
         <f t="shared" si="22"/>
-        <v>21234.882576660035</v>
+        <v>14490.887661843108</v>
       </c>
       <c r="L98">
         <f t="shared" si="23"/>
-        <v>0.62099273328552229</v>
+        <v>0.91000000000000014</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -19762,15 +19823,15 @@
       </c>
       <c r="J99">
         <f t="shared" si="21"/>
-        <v>0.26400000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="K99">
         <f t="shared" si="22"/>
-        <v>20610.327206758269</v>
+        <v>12880.78903274943</v>
       </c>
       <c r="L99">
         <f t="shared" si="23"/>
-        <v>0.57497029480656048</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -19811,15 +19872,15 @@
       </c>
       <c r="J100">
         <f t="shared" si="21"/>
-        <v>0.25600000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K100">
         <f t="shared" si="22"/>
-        <v>19985.771836856504</v>
+        <v>11270.690403655752</v>
       </c>
       <c r="L100">
         <f t="shared" si="23"/>
-        <v>0.52446020904081769</v>
+        <v>0.92999999999999994</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -19860,15 +19921,15 @@
       </c>
       <c r="J101">
         <f t="shared" si="21"/>
-        <v>0.248</v>
+        <v>0.06</v>
       </c>
       <c r="K101">
         <f t="shared" si="22"/>
-        <v>19361.216466954738</v>
+        <v>9660.5917745620718</v>
       </c>
       <c r="L101">
         <f t="shared" si="23"/>
-        <v>0.46902818754118625</v>
+        <v>0.94000000000000028</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -19909,15 +19970,15 @@
       </c>
       <c r="J102">
         <f t="shared" si="21"/>
-        <v>0.24000000000000002</v>
+        <v>0.05</v>
       </c>
       <c r="K102">
         <f t="shared" si="22"/>
-        <v>18736.661097052973</v>
+        <v>8050.4931454683938</v>
       </c>
       <c r="L102">
         <f t="shared" si="23"/>
-        <v>0.408182036734277</v>
+        <v>0.95000000000000018</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -19958,15 +20019,15 @@
       </c>
       <c r="J103">
         <f t="shared" si="21"/>
-        <v>0.23200000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="K103">
         <f t="shared" si="22"/>
-        <v>18112.105727151207</v>
+        <v>6440.3945163747148</v>
       </c>
       <c r="L103">
         <f t="shared" si="23"/>
-        <v>0.34136167427795788</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -20007,15 +20068,15 @@
       </c>
       <c r="J104">
         <f t="shared" si="21"/>
-        <v>0.224</v>
+        <v>0.03</v>
       </c>
       <c r="K104">
         <f t="shared" si="22"/>
-        <v>17487.550357249442</v>
+        <v>4830.2958872810359</v>
       </c>
       <c r="L104">
         <f t="shared" si="23"/>
-        <v>0.26792700606693509</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
@@ -20056,15 +20117,15 @@
       </c>
       <c r="J105">
         <f t="shared" si="21"/>
-        <v>0.21600000000000003</v>
+        <v>0.02</v>
       </c>
       <c r="K105">
         <f t="shared" si="22"/>
-        <v>16862.994987347676</v>
+        <v>3220.1972581873574</v>
       </c>
       <c r="L105">
         <f t="shared" si="23"/>
-        <v>0.18714310923957489</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -20105,15 +20166,15 @@
       </c>
       <c r="J106">
         <f t="shared" si="21"/>
-        <v>0.20800000000000002</v>
+        <v>0.01</v>
       </c>
       <c r="K106">
         <f t="shared" si="22"/>
-        <v>16238.439617445911</v>
+        <v>1610.0986290936787</v>
       </c>
       <c r="L106">
         <f t="shared" si="23"/>
-        <v>9.816199587860748E-2</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -20154,15 +20215,15 @@
       </c>
       <c r="J107">
         <f t="shared" si="21"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="K107">
         <f t="shared" si="22"/>
-        <v>15613.884247544145</v>
+        <v>0</v>
       </c>
       <c r="L107">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -20176,11 +20237,11 @@
       </c>
       <c r="K108">
         <f>LARGE(K7:K107,1)</f>
-        <v>78069.421237720715</v>
+        <v>161009.86290936786</v>
       </c>
       <c r="L108">
         <f>LARGE(L7:L107,1)</f>
-        <v>0.98470080064806564</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -20191,10 +20252,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H41"/>
+  <dimension ref="A3:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20204,7 +20265,12 @@
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -20217,8 +20283,18 @@
       <c r="G4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>100</v>
+      </c>
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <f>T4*0.01*4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="58">
         <v>0</v>
       </c>
@@ -20243,8 +20319,18 @@
       <c r="H5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>95</v>
+      </c>
+      <c r="U5">
+        <v>3.8</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V14" si="0">T5*0.01*4</f>
+        <v>3.8000000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1E-3</v>
       </c>
@@ -20252,7 +20338,7 @@
         <v>3.7585000000000002</v>
       </c>
       <c r="C6" s="70">
-        <f t="shared" ref="C6:C16" si="0">B6-B7</f>
+        <f t="shared" ref="C6:C16" si="1">B6-B7</f>
         <v>1.0870000000000002</v>
       </c>
       <c r="E6">
@@ -20262,11 +20348,21 @@
         <v>3.7585000000000002</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G16" si="1">F6-F7</f>
+        <f t="shared" ref="G6:G16" si="2">F6-F7</f>
         <v>1.0870000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>90</v>
+      </c>
+      <c r="U6">
+        <v>3.6</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.05</v>
       </c>
@@ -20274,7 +20370,7 @@
         <v>2.6715</v>
       </c>
       <c r="C7" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.36249999999999982</v>
       </c>
       <c r="E7">
@@ -20284,11 +20380,21 @@
         <v>2.6715</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.36249999999999982</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>85</v>
+      </c>
+      <c r="U7">
+        <v>3.4</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.1</v>
       </c>
@@ -20296,7 +20402,7 @@
         <v>2.3090000000000002</v>
       </c>
       <c r="C8" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23060000000000036</v>
       </c>
       <c r="E8">
@@ -20306,11 +20412,21 @@
         <v>2.3090000000000002</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23060000000000036</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>80</v>
+      </c>
+      <c r="U8">
+        <v>3.2</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.15</v>
       </c>
@@ -20318,7 +20434,7 @@
         <v>2.0783999999999998</v>
       </c>
       <c r="C9" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16859999999999986</v>
       </c>
       <c r="E9">
@@ -20328,11 +20444,21 @@
         <v>2.0783999999999998</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16859999999999986</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>75</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.2</v>
       </c>
@@ -20340,7 +20466,7 @@
         <v>1.9097999999999999</v>
       </c>
       <c r="C10" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13219999999999987</v>
       </c>
       <c r="E10">
@@ -20350,11 +20476,21 @@
         <v>1.9097999999999999</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.13219999999999987</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>70</v>
+      </c>
+      <c r="U10">
+        <v>2.8</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.25</v>
       </c>
@@ -20362,7 +20498,7 @@
         <v>1.7776000000000001</v>
       </c>
       <c r="C11" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10790000000000011</v>
       </c>
       <c r="E11">
@@ -20372,11 +20508,21 @@
         <v>1.7776000000000001</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.10790000000000011</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>65</v>
+      </c>
+      <c r="U11">
+        <v>2.6</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.3</v>
       </c>
@@ -20384,7 +20530,7 @@
         <v>1.6697</v>
       </c>
       <c r="C12" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.0700000000000003E-2</v>
       </c>
       <c r="E12">
@@ -20394,11 +20540,21 @@
         <v>1.6697</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.0700000000000003E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>60</v>
+      </c>
+      <c r="U12">
+        <v>2.4</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.35</v>
       </c>
@@ -20406,7 +20562,7 @@
         <v>1.579</v>
       </c>
       <c r="C13" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8000000000000069E-2</v>
       </c>
       <c r="E13">
@@ -20416,11 +20572,21 @@
         <v>1.579</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.8000000000000069E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>55</v>
+      </c>
+      <c r="U13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.4</v>
       </c>
@@ -20428,7 +20594,7 @@
         <v>1.5009999999999999</v>
       </c>
       <c r="C14" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8199999999999816E-2</v>
       </c>
       <c r="E14">
@@ -20438,11 +20604,21 @@
         <v>1.5009999999999999</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.8199999999999816E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>50</v>
+      </c>
+      <c r="U14">
+        <v>2</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.45</v>
       </c>
@@ -20450,7 +20626,7 @@
         <v>1.4328000000000001</v>
       </c>
       <c r="C15" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.030000000000002E-2</v>
       </c>
       <c r="E15">
@@ -20460,11 +20636,11 @@
         <v>1.4328000000000001</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.030000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.5</v>
       </c>
@@ -20472,7 +20648,7 @@
         <v>1.3725000000000001</v>
       </c>
       <c r="C16" s="70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3725000000000001</v>
       </c>
       <c r="E16">
@@ -20482,11 +20658,19 @@
         <v>1.3725000000000001</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3725000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -20500,7 +20684,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -20514,15 +20698,12 @@
         <v>1E-3</v>
       </c>
       <c r="F21" s="59">
-        <v>3.7585000000000002</v>
+        <f>$B$21*E21^2 + $B$22*E21 + $B$23</f>
+        <v>2.8773417457071169</v>
       </c>
       <c r="G21" s="59"/>
-      <c r="H21" t="str">
-        <f>"{"&amp;E21&amp;","&amp;F21&amp;"}"</f>
-        <v>{0.001,3.7585}</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -20536,15 +20717,12 @@
         <v>0.05</v>
       </c>
       <c r="F22" s="59">
-        <v>2.6715</v>
+        <f t="shared" ref="F22:F31" si="3">$B$21*E22^2 + $B$22*E22 + $B$23</f>
+        <v>2.6028418720925002</v>
       </c>
       <c r="G22" s="59"/>
-      <c r="H22" t="str">
-        <f t="shared" ref="H22:H31" si="2">"{"&amp;E22&amp;","&amp;F22&amp;"}"</f>
-        <v>{0.05,2.6715}</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -20558,15 +20736,12 @@
         <v>0.1</v>
       </c>
       <c r="F23" s="59">
-        <v>2.3090000000000002</v>
+        <f t="shared" si="3"/>
+        <v>2.3520847537699998</v>
       </c>
       <c r="G23" s="59"/>
-      <c r="H23" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.1,2.309}</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>2.0783999999999998</v>
       </c>
@@ -20574,17 +20749,14 @@
         <v>0.15</v>
       </c>
       <c r="F24" s="59">
-        <v>2.0783999999999998</v>
+        <f t="shared" si="3"/>
+        <v>2.1309688410324998</v>
       </c>
       <c r="G24" s="59"/>
-      <c r="H24" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.15,2.0784}</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25">
         <v>1.9097999999999999</v>
@@ -20593,15 +20765,12 @@
         <v>0.2</v>
       </c>
       <c r="F25" s="59">
-        <v>1.9097999999999999</v>
+        <f t="shared" si="3"/>
+        <v>1.93949413388</v>
       </c>
       <c r="G25" s="59"/>
-      <c r="H25" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.2,1.9098}</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -20615,15 +20784,12 @@
         <v>0.25</v>
       </c>
       <c r="F26" s="59">
-        <v>1.7776000000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.7776606323124999</v>
       </c>
       <c r="G26" s="59"/>
-      <c r="H26" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.25,1.7776}</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -20637,15 +20803,12 @@
         <v>0.3</v>
       </c>
       <c r="F27" s="59">
-        <v>1.6697</v>
+        <f t="shared" si="3"/>
+        <v>1.64546833633</v>
       </c>
       <c r="G27" s="59"/>
-      <c r="H27" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.3,1.6697}</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>95</v>
       </c>
@@ -20659,15 +20822,12 @@
         <v>0.35</v>
       </c>
       <c r="F28" s="59">
-        <v>1.579</v>
+        <f t="shared" si="3"/>
+        <v>1.5429172459325</v>
       </c>
       <c r="G28" s="59"/>
-      <c r="H28" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.35,1.579}</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>1.5009999999999999</v>
       </c>
@@ -20675,15 +20835,12 @@
         <v>0.4</v>
       </c>
       <c r="F29" s="59">
-        <v>1.5009999999999999</v>
+        <f t="shared" si="3"/>
+        <v>1.4700073611200002</v>
       </c>
       <c r="G29" s="59"/>
-      <c r="H29" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.4,1.501}</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>1.4328000000000001</v>
       </c>
@@ -20691,15 +20848,12 @@
         <v>0.45</v>
       </c>
       <c r="F30" s="59">
-        <v>1.4328000000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.4267386818925001</v>
       </c>
       <c r="G30" s="59"/>
-      <c r="H30" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.45,1.4328}</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>1.3725000000000001</v>
       </c>
@@ -20707,88 +20861,48 @@
         <v>0.5</v>
       </c>
       <c r="F31" s="59">
-        <v>1.3725000000000001</v>
+        <f t="shared" si="3"/>
+        <v>1.4131112082499999</v>
       </c>
       <c r="G31" s="59"/>
-      <c r="H31" t="str">
-        <f t="shared" si="2"/>
-        <v>{0.5,1.3725}</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <v>0.55000000000000004</v>
-      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32" s="71"/>
       <c r="G32" s="72"/>
-      <c r="H32" t="str">
-        <f>H21&amp;","&amp;H22&amp;","&amp;H23&amp;","&amp;H24&amp;","&amp;H25&amp;","&amp;H26&amp;","&amp;H27&amp;","&amp;H28&amp;","&amp;H29&amp;","&amp;H30&amp;","&amp;H31</f>
-        <v>{0.001,3.7585},{0.05,2.6715},{0.1,2.309},{0.15,2.0784},{0.2,1.9098},{0.25,1.7776},{0.3,1.6697},{0.35,1.579},{0.4,1.501},{0.45,1.4328},{0.5,1.3725}</v>
-      </c>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <v>0.6</v>
-      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" s="71"/>
       <c r="G33" s="72"/>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34">
-        <v>0.65</v>
-      </c>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" s="71"/>
       <c r="G34" s="72"/>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E35">
-        <v>0.7</v>
-      </c>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" s="71"/>
       <c r="G35" s="72"/>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E36">
-        <v>0.75</v>
-      </c>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" s="71"/>
       <c r="G36" s="72"/>
-      <c r="H36" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E37">
-        <v>0.8</v>
-      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" s="71"/>
       <c r="G37" s="72"/>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E38">
-        <v>0.85</v>
-      </c>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" s="71"/>
       <c r="G38" s="72"/>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E39">
-        <v>0.9</v>
-      </c>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" s="71"/>
       <c r="G39" s="72"/>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E40">
-        <v>0.95</v>
-      </c>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" s="71"/>
       <c r="G40" s="72"/>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E41">
-        <v>1</v>
-      </c>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" s="71"/>
       <c r="G41" s="72"/>
     </row>

</xml_diff>